<commit_message>
add multiparameter poisson-exp and exp-exp
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\Code\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C76A87-9F81-4C69-94C6-24FFDE6A2085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877C7FCE-DE08-43D1-BCD4-3EA1981FAEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
   <si>
     <t>Exponential-Exponential</t>
   </si>
@@ -169,13 +169,25 @@
   </si>
   <si>
     <t>Lambda</t>
+  </si>
+  <si>
+    <t>poisExpX</t>
+  </si>
+  <si>
+    <t>Poisson-Exponential-X</t>
+  </si>
+  <si>
+    <t>expExpX</t>
+  </si>
+  <si>
+    <t>Exponential-Exponential-X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,13 +195,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -201,13 +225,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -520,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,14 +559,15 @@
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -556,34 +584,34 @@
         <v>27</v>
       </c>
       <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>35</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>39</v>
-      </c>
-      <c r="N1" t="s">
-        <v>41</v>
       </c>
       <c r="O1" t="s">
         <v>40</v>
@@ -596,58 +624,58 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="str">
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="str">
         <f>B2&amp;"Slider"</f>
         <v>bernSlider</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="str">
-        <f>IF(F2=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+      <c r="I2" t="str">
+        <f>IF(E2=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
         <v>c()</v>
       </c>
-      <c r="H2" t="str">
+      <c r="J2" t="str">
         <f>B2&amp;"PlotDistr"</f>
         <v>bernPlotDistr</v>
       </c>
-      <c r="I2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" t="str">
+      <c r="K2" t="str">
         <f>B2&amp;"Draws"</f>
         <v>bernDraws</v>
       </c>
-      <c r="K2" t="str">
+      <c r="L2" t="str">
         <f>B2&amp;"Latex"</f>
         <v>bernLatex</v>
       </c>
-      <c r="L2" t="str">
+      <c r="M2" t="str">
         <f>$B2&amp;"ChartDomain"</f>
         <v>bernChartDomain</v>
       </c>
-      <c r="M2" t="str">
+      <c r="N2" t="str">
         <f>$B2&amp;"LikelihoodFun"</f>
         <v>bernLikelihoodFun</v>
       </c>
-      <c r="N2" t="s">
-        <v>43</v>
-      </c>
       <c r="O2" t="str">
-        <f>IF(F2=1,"",", margNum")</f>
+        <f>IF(E2=1,"",", margNum")</f>
         <v/>
       </c>
       <c r="P2" t="str">
-        <f>"function(a, margNum){MLEPlotter(a, "&amp;L2&amp;", "&amp;M2&amp;" ,"""&amp;N2&amp;""""&amp;O2&amp;")}"</f>
+        <f>"function(a, margNum){MLEPlotter(a, "&amp;M2&amp;", "&amp;N2&amp;" ,"""&amp;F2&amp;""""&amp;O2&amp;")}"</f>
         <v>function(a, margNum){MLEPlotter(a, bernChartDomain, bernLikelihoodFun ,"Pi")}</v>
       </c>
     </row>
@@ -656,599 +684,719 @@
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E12" si="0">B3&amp;"Slider"</f>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H13" si="0">B3&amp;"Slider"</f>
         <v>bernLogitSlider</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="str">
-        <f t="shared" ref="G3:G12" si="1">IF(F3=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+      <c r="I3" t="str">
+        <f>IF(E3=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
         <v>c()</v>
       </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H12" si="2">B3&amp;"PlotDistr"</f>
+      <c r="J3" t="str">
+        <f>B3&amp;"PlotDistr"</f>
         <v>bernLogitPlotDistr</v>
       </c>
-      <c r="I3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" t="str">
-        <f t="shared" ref="J3:J12" si="3">B3&amp;"Draws"</f>
+      <c r="K3" t="str">
+        <f>B3&amp;"Draws"</f>
         <v>bernLogitDraws</v>
       </c>
-      <c r="K3" t="str">
-        <f t="shared" ref="K3:K12" si="4">B3&amp;"Latex"</f>
+      <c r="L3" t="str">
+        <f>B3&amp;"Latex"</f>
         <v>bernLogitLatex</v>
       </c>
-      <c r="L3" t="str">
-        <f t="shared" ref="L3:L12" si="5">$B3&amp;"ChartDomain"</f>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M14" si="1">$B3&amp;"ChartDomain"</f>
         <v>bernLogitChartDomain</v>
       </c>
-      <c r="M3" t="str">
-        <f t="shared" ref="M3:M12" si="6">$B3&amp;"LikelihoodFun"</f>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N14" si="2">$B3&amp;"LikelihoodFun"</f>
         <v>bernLogitLikelihoodFun</v>
       </c>
-      <c r="N3" t="s">
-        <v>42</v>
-      </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O12" si="7">IF(F3=1,"",", margNum")</f>
+        <f>IF(E3=1,"",", margNum")</f>
         <v/>
       </c>
       <c r="P3" t="str">
-        <f t="shared" ref="P3:P12" si="8">"function(a, margNum){MLEPlotter(a, "&amp;L3&amp;", "&amp;M3&amp;" ,"""&amp;N3&amp;""""&amp;O3&amp;")}"</f>
+        <f>"function(a, margNum){MLEPlotter(a, "&amp;M3&amp;", "&amp;N3&amp;" ,"""&amp;F3&amp;""""&amp;O3&amp;")}"</f>
         <v>function(a, margNum){MLEPlotter(a, bernLogitChartDomain, bernLogitLikelihoodFun ,"Beta")}</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A12" si="9">A3+1</f>
+        <f t="shared" ref="A4:A14" si="3">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="str">
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="str">
         <f t="shared" si="0"/>
         <v>bernLogitXSlider</v>
       </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4" t="str">
+      <c r="I4" t="str">
+        <f>IF(E4=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+        <v>c("Beta0", "Beta1", "Beta2")</v>
+      </c>
+      <c r="J4" t="str">
+        <f>B4&amp;"PlotDistr"</f>
+        <v>bernLogitXPlotDistr</v>
+      </c>
+      <c r="K4" t="str">
+        <f>B4&amp;"Draws"</f>
+        <v>bernLogitXDraws</v>
+      </c>
+      <c r="L4" t="str">
+        <f>B4&amp;"Latex"</f>
+        <v>bernLogitXLatex</v>
+      </c>
+      <c r="M4" t="str">
         <f t="shared" si="1"/>
-        <v>c("Beta0", "Beta1", "Beta2")</v>
-      </c>
-      <c r="H4" t="str">
+        <v>bernLogitXChartDomain</v>
+      </c>
+      <c r="N4" t="str">
         <f t="shared" si="2"/>
-        <v>bernLogitXPlotDistr</v>
-      </c>
-      <c r="I4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" t="str">
-        <f t="shared" si="3"/>
-        <v>bernLogitXDraws</v>
-      </c>
-      <c r="K4" t="str">
-        <f t="shared" si="4"/>
-        <v>bernLogitXLatex</v>
-      </c>
-      <c r="L4" t="str">
-        <f t="shared" si="5"/>
-        <v>bernLogitXChartDomain</v>
-      </c>
-      <c r="M4" t="str">
-        <f t="shared" si="6"/>
         <v>bernLogitXLikelihoodFun</v>
       </c>
-      <c r="N4" t="s">
-        <v>42</v>
-      </c>
       <c r="O4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E4=1,"",", margNum")</f>
         <v>, margNum</v>
       </c>
       <c r="P4" t="str">
-        <f t="shared" si="8"/>
+        <f>"function(a, margNum){MLEPlotter(a, "&amp;M4&amp;", "&amp;N4&amp;" ,"""&amp;F4&amp;""""&amp;O4&amp;")}"</f>
         <v>function(a, margNum){MLEPlotter(a, bernLogitXChartDomain, bernLogitXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="str">
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="str">
         <f t="shared" si="0"/>
         <v>styNormSlider</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="str">
+      <c r="I5" t="str">
+        <f>IF(E5=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+        <v>c()</v>
+      </c>
+      <c r="J5" t="str">
+        <f>B5&amp;"PlotDistr"</f>
+        <v>styNormPlotDistr</v>
+      </c>
+      <c r="K5" t="str">
+        <f>B5&amp;"Draws"</f>
+        <v>styNormDraws</v>
+      </c>
+      <c r="L5" t="str">
+        <f>B5&amp;"Latex"</f>
+        <v>styNormLatex</v>
+      </c>
+      <c r="M5" t="str">
         <f t="shared" si="1"/>
-        <v>c()</v>
-      </c>
-      <c r="H5" t="str">
+        <v>styNormChartDomain</v>
+      </c>
+      <c r="N5" t="str">
         <f t="shared" si="2"/>
-        <v>styNormPlotDistr</v>
-      </c>
-      <c r="I5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" t="str">
-        <f t="shared" si="3"/>
-        <v>styNormDraws</v>
-      </c>
-      <c r="K5" t="str">
-        <f t="shared" si="4"/>
-        <v>styNormLatex</v>
-      </c>
-      <c r="L5" t="str">
-        <f t="shared" si="5"/>
-        <v>styNormChartDomain</v>
-      </c>
-      <c r="M5" t="str">
-        <f t="shared" si="6"/>
         <v>styNormLikelihoodFun</v>
       </c>
-      <c r="N5" t="s">
-        <v>42</v>
-      </c>
       <c r="O5" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E5=1,"",", margNum")</f>
         <v/>
       </c>
       <c r="P5" t="str">
-        <f t="shared" si="8"/>
+        <f>"function(a, margNum){MLEPlotter(a, "&amp;M5&amp;", "&amp;N5&amp;" ,"""&amp;F5&amp;""""&amp;O5&amp;")}"</f>
         <v>function(a, margNum){MLEPlotter(a, styNormChartDomain, styNormLikelihoodFun ,"Beta")}</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="str">
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="str">
         <f t="shared" si="0"/>
         <v>multiNormSlider</v>
       </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6" t="str">
+      <c r="I6" t="str">
+        <f>IF(E6=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+        <v>c("Beta0", "Beta1", "Beta2")</v>
+      </c>
+      <c r="J6" t="str">
+        <f>B6&amp;"PlotDistr"</f>
+        <v>multiNormPlotDistr</v>
+      </c>
+      <c r="K6" t="str">
+        <f>B6&amp;"Draws"</f>
+        <v>multiNormDraws</v>
+      </c>
+      <c r="L6" t="str">
+        <f>B6&amp;"Latex"</f>
+        <v>multiNormLatex</v>
+      </c>
+      <c r="M6" t="str">
         <f t="shared" si="1"/>
-        <v>c("Beta0", "Beta1", "Beta2")</v>
-      </c>
-      <c r="H6" t="str">
+        <v>multiNormChartDomain</v>
+      </c>
+      <c r="N6" t="str">
         <f t="shared" si="2"/>
-        <v>multiNormPlotDistr</v>
-      </c>
-      <c r="I6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" t="str">
-        <f t="shared" si="3"/>
-        <v>multiNormDraws</v>
-      </c>
-      <c r="K6" t="str">
-        <f t="shared" si="4"/>
-        <v>multiNormLatex</v>
-      </c>
-      <c r="L6" t="str">
-        <f t="shared" si="5"/>
-        <v>multiNormChartDomain</v>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" si="6"/>
         <v>multiNormLikelihoodFun</v>
       </c>
-      <c r="N6" t="s">
-        <v>42</v>
-      </c>
       <c r="O6" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E6=1,"",", margNum")</f>
         <v>, margNum</v>
       </c>
       <c r="P6" t="str">
-        <f t="shared" si="8"/>
+        <f>"function(a, margNum){MLEPlotter(a, "&amp;M6&amp;", "&amp;N6&amp;" ,"""&amp;F6&amp;""""&amp;O6&amp;")}"</f>
         <v>function(a, margNum){MLEPlotter(a, multiNormChartDomain, multiNormLikelihoodFun ,"Beta", margNum)}</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E7" t="str">
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" t="str">
         <f t="shared" si="0"/>
         <v>logNormSlider</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="str">
+      <c r="I7" t="str">
+        <f>IF(E7=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+        <v>c()</v>
+      </c>
+      <c r="J7" t="str">
+        <f>B7&amp;"PlotDistr"</f>
+        <v>logNormPlotDistr</v>
+      </c>
+      <c r="K7" t="str">
+        <f>B7&amp;"Draws"</f>
+        <v>logNormDraws</v>
+      </c>
+      <c r="L7" t="str">
+        <f>B7&amp;"Latex"</f>
+        <v>logNormLatex</v>
+      </c>
+      <c r="M7" t="str">
         <f t="shared" si="1"/>
-        <v>c()</v>
-      </c>
-      <c r="H7" t="str">
+        <v>logNormChartDomain</v>
+      </c>
+      <c r="N7" t="str">
         <f t="shared" si="2"/>
-        <v>logNormPlotDistr</v>
-      </c>
-      <c r="I7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" si="3"/>
-        <v>logNormDraws</v>
-      </c>
-      <c r="K7" t="str">
-        <f t="shared" si="4"/>
-        <v>logNormLatex</v>
-      </c>
-      <c r="L7" t="str">
-        <f t="shared" si="5"/>
-        <v>logNormChartDomain</v>
-      </c>
-      <c r="M7" t="str">
-        <f t="shared" si="6"/>
         <v>logNormLikelihoodFun</v>
       </c>
-      <c r="N7" t="s">
-        <v>42</v>
-      </c>
       <c r="O7" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E7=1,"",", margNum")</f>
         <v/>
       </c>
       <c r="P7" t="str">
-        <f t="shared" si="8"/>
+        <f>"function(a, margNum){MLEPlotter(a, "&amp;M7&amp;", "&amp;N7&amp;" ,"""&amp;F7&amp;""""&amp;O7&amp;")}"</f>
         <v>function(a, margNum){MLEPlotter(a, logNormChartDomain, logNormLikelihoodFun ,"Beta")}</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="str">
+      <c r="E8" s="1">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="str">
         <f t="shared" si="0"/>
         <v>logNormXSlider</v>
       </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8" t="str">
+      <c r="I8" t="str">
+        <f>IF(E8=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+        <v>c("Beta0", "Beta1", "Beta2")</v>
+      </c>
+      <c r="J8" t="str">
+        <f>B8&amp;"PlotDistr"</f>
+        <v>logNormXPlotDistr</v>
+      </c>
+      <c r="K8" t="str">
+        <f>B8&amp;"Draws"</f>
+        <v>logNormXDraws</v>
+      </c>
+      <c r="L8" t="str">
+        <f>B8&amp;"Latex"</f>
+        <v>logNormXLatex</v>
+      </c>
+      <c r="M8" t="str">
         <f t="shared" si="1"/>
-        <v>c("Beta0", "Beta1", "Beta2")</v>
-      </c>
-      <c r="H8" t="str">
+        <v>logNormXChartDomain</v>
+      </c>
+      <c r="N8" t="str">
         <f t="shared" si="2"/>
-        <v>logNormXPlotDistr</v>
-      </c>
-      <c r="I8" t="s">
-        <v>37</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" si="3"/>
-        <v>logNormXDraws</v>
-      </c>
-      <c r="K8" t="str">
-        <f t="shared" si="4"/>
-        <v>logNormXLatex</v>
-      </c>
-      <c r="L8" t="str">
-        <f t="shared" si="5"/>
-        <v>logNormXChartDomain</v>
-      </c>
-      <c r="M8" t="str">
-        <f t="shared" si="6"/>
         <v>logNormXLikelihoodFun</v>
       </c>
-      <c r="N8" t="s">
-        <v>42</v>
-      </c>
       <c r="O8" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E8=1,"",", margNum")</f>
         <v>, margNum</v>
       </c>
       <c r="P8" t="str">
-        <f t="shared" si="8"/>
+        <f>"function(a, margNum){MLEPlotter(a, "&amp;M8&amp;", "&amp;N8&amp;" ,"""&amp;F8&amp;""""&amp;O8&amp;")}"</f>
         <v>function(a, margNum){MLEPlotter(a, logNormXChartDomain, logNormXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="str">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" t="str">
         <f t="shared" si="0"/>
         <v>poisSlider</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="str">
+      <c r="I9" t="str">
+        <f>IF(E9=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+        <v>c()</v>
+      </c>
+      <c r="J9" t="str">
+        <f>B9&amp;"PlotDistr"</f>
+        <v>poisPlotDistr</v>
+      </c>
+      <c r="K9" t="str">
+        <f>B9&amp;"Draws"</f>
+        <v>poisDraws</v>
+      </c>
+      <c r="L9" t="str">
+        <f>B9&amp;"Latex"</f>
+        <v>poisLatex</v>
+      </c>
+      <c r="M9" t="str">
         <f t="shared" si="1"/>
-        <v>c()</v>
-      </c>
-      <c r="H9" t="str">
+        <v>poisChartDomain</v>
+      </c>
+      <c r="N9" t="str">
         <f t="shared" si="2"/>
-        <v>poisPlotDistr</v>
-      </c>
-      <c r="I9" t="s">
-        <v>36</v>
-      </c>
-      <c r="J9" t="str">
-        <f t="shared" si="3"/>
-        <v>poisDraws</v>
-      </c>
-      <c r="K9" t="str">
-        <f t="shared" si="4"/>
-        <v>poisLatex</v>
-      </c>
-      <c r="L9" t="str">
-        <f t="shared" si="5"/>
-        <v>poisChartDomain</v>
-      </c>
-      <c r="M9" t="str">
-        <f t="shared" si="6"/>
         <v>poisLikelihoodFun</v>
       </c>
-      <c r="N9" t="s">
-        <v>44</v>
-      </c>
       <c r="O9" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E9=1,"",", margNum")</f>
         <v/>
       </c>
       <c r="P9" t="str">
-        <f t="shared" si="8"/>
+        <f>"function(a, margNum){MLEPlotter(a, "&amp;M9&amp;", "&amp;N9&amp;" ,"""&amp;F9&amp;""""&amp;O9&amp;")}"</f>
         <v>function(a, margNum){MLEPlotter(a, poisChartDomain, poisLikelihoodFun ,"Lambda")}</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E10" t="str">
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" t="str">
         <f t="shared" si="0"/>
         <v>poisExpSlider</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="str">
+      <c r="I10" t="str">
+        <f>IF(E10=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+        <v>c()</v>
+      </c>
+      <c r="J10" t="str">
+        <f>B10&amp;"PlotDistr"</f>
+        <v>poisExpPlotDistr</v>
+      </c>
+      <c r="K10" t="str">
+        <f>B10&amp;"Draws"</f>
+        <v>poisExpDraws</v>
+      </c>
+      <c r="L10" t="str">
+        <f>B10&amp;"Latex"</f>
+        <v>poisExpLatex</v>
+      </c>
+      <c r="M10" t="str">
         <f t="shared" si="1"/>
-        <v>c()</v>
-      </c>
-      <c r="H10" t="str">
+        <v>poisExpChartDomain</v>
+      </c>
+      <c r="N10" t="str">
         <f t="shared" si="2"/>
-        <v>poisExpPlotDistr</v>
-      </c>
-      <c r="I10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" t="str">
-        <f t="shared" si="3"/>
-        <v>poisExpDraws</v>
-      </c>
-      <c r="K10" t="str">
-        <f t="shared" si="4"/>
-        <v>poisExpLatex</v>
-      </c>
-      <c r="L10" t="str">
-        <f t="shared" si="5"/>
-        <v>poisExpChartDomain</v>
-      </c>
-      <c r="M10" t="str">
-        <f t="shared" si="6"/>
         <v>poisExpLikelihoodFun</v>
       </c>
-      <c r="N10" t="s">
-        <v>42</v>
-      </c>
       <c r="O10" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(E10=1,"",", margNum")</f>
         <v/>
       </c>
       <c r="P10" t="str">
-        <f t="shared" si="8"/>
+        <f>"function(a, margNum){MLEPlotter(a, "&amp;M10&amp;", "&amp;N10&amp;" ,"""&amp;F10&amp;""""&amp;O10&amp;")}"</f>
         <v>function(a, margNum){MLEPlotter(a, poisExpChartDomain, poisExpLikelihoodFun ,"Beta")}</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v>expSlider</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" t="str">
+      <c r="B11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" ref="H11" si="4">B11&amp;"Slider"</f>
+        <v>poisExpXSlider</v>
+      </c>
+      <c r="I11" t="str">
+        <f>IF(E11=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+        <v>c("Beta0", "Beta1", "Beta2")</v>
+      </c>
+      <c r="J11" t="str">
+        <f>B11&amp;"PlotDistr"</f>
+        <v>poisExpXPlotDistr</v>
+      </c>
+      <c r="K11" t="str">
+        <f>B11&amp;"Draws"</f>
+        <v>poisExpXDraws</v>
+      </c>
+      <c r="L11" t="str">
+        <f>B11&amp;"Latex"</f>
+        <v>poisExpXLatex</v>
+      </c>
+      <c r="M11" t="str">
         <f t="shared" si="1"/>
-        <v>c()</v>
-      </c>
-      <c r="H11" t="str">
+        <v>poisExpXChartDomain</v>
+      </c>
+      <c r="N11" t="str">
         <f t="shared" si="2"/>
-        <v>expPlotDistr</v>
-      </c>
-      <c r="I11" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" t="str">
-        <f t="shared" si="3"/>
-        <v>expDraws</v>
-      </c>
-      <c r="K11" t="str">
-        <f t="shared" si="4"/>
-        <v>expLatex</v>
-      </c>
-      <c r="L11" t="str">
-        <f t="shared" si="5"/>
-        <v>expChartDomain</v>
-      </c>
-      <c r="M11" t="str">
-        <f t="shared" si="6"/>
-        <v>expLikelihoodFun</v>
-      </c>
-      <c r="N11" t="s">
-        <v>44</v>
+        <v>poisExpXLikelihoodFun</v>
       </c>
       <c r="O11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <f>IF(E11=1,"",", margNum")</f>
+        <v>, margNum</v>
       </c>
       <c r="P11" t="str">
-        <f t="shared" si="8"/>
-        <v>function(a, margNum){MLEPlotter(a, expChartDomain, expLikelihoodFun ,"Lambda")}</v>
+        <f>"function(a, margNum){MLEPlotter(a, "&amp;M11&amp;", "&amp;N11&amp;" ,"""&amp;F11&amp;""""&amp;O11&amp;")}"</f>
+        <v>function(a, margNum){MLEPlotter(a, poisExpXChartDomain, poisExpXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>expSlider</v>
+      </c>
+      <c r="I12" t="str">
+        <f>IF(E12=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+        <v>c()</v>
+      </c>
+      <c r="J12" t="str">
+        <f>B12&amp;"PlotDistr"</f>
+        <v>expPlotDistr</v>
+      </c>
+      <c r="K12" t="str">
+        <f>B12&amp;"Draws"</f>
+        <v>expDraws</v>
+      </c>
+      <c r="L12" t="str">
+        <f>B12&amp;"Latex"</f>
+        <v>expLatex</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="1"/>
+        <v>expChartDomain</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="2"/>
+        <v>expLikelihoodFun</v>
+      </c>
+      <c r="O12" t="str">
+        <f>IF(E12=1,"",", margNum")</f>
+        <v/>
+      </c>
+      <c r="P12" t="str">
+        <f>"function(a, margNum){MLEPlotter(a, "&amp;M12&amp;", "&amp;N12&amp;" ,"""&amp;F12&amp;""""&amp;O12&amp;")}"</f>
+        <v>function(a, margNum){MLEPlotter(a, expChartDomain, expLikelihoodFun ,"Lambda")}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E12" t="str">
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" t="str">
         <f t="shared" si="0"/>
         <v>expExpSlider</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="str">
+      <c r="I13" t="str">
+        <f>IF(E13=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+        <v>c()</v>
+      </c>
+      <c r="J13" t="str">
+        <f>B13&amp;"PlotDistr"</f>
+        <v>expExpPlotDistr</v>
+      </c>
+      <c r="K13" t="str">
+        <f>B13&amp;"Draws"</f>
+        <v>expExpDraws</v>
+      </c>
+      <c r="L13" t="str">
+        <f>B13&amp;"Latex"</f>
+        <v>expExpLatex</v>
+      </c>
+      <c r="M13" t="str">
         <f t="shared" si="1"/>
-        <v>c()</v>
-      </c>
-      <c r="H12" t="str">
+        <v>expExpChartDomain</v>
+      </c>
+      <c r="N13" t="str">
         <f t="shared" si="2"/>
-        <v>expExpPlotDistr</v>
-      </c>
-      <c r="I12" t="s">
+        <v>expExpLikelihoodFun</v>
+      </c>
+      <c r="O13" t="str">
+        <f>IF(E13=1,"",", margNum")</f>
+        <v/>
+      </c>
+      <c r="P13" t="str">
+        <f>"function(a, margNum){MLEPlotter(a, "&amp;M13&amp;", "&amp;N13&amp;" ,"""&amp;F13&amp;""""&amp;O13&amp;")}"</f>
+        <v>function(a, margNum){MLEPlotter(a, expExpChartDomain, expExpLikelihoodFun ,"Beta")}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J12" t="str">
-        <f t="shared" si="3"/>
-        <v>expExpDraws</v>
-      </c>
-      <c r="K12" t="str">
-        <f t="shared" si="4"/>
-        <v>expExpLatex</v>
-      </c>
-      <c r="L12" t="str">
-        <f t="shared" si="5"/>
-        <v>expExpChartDomain</v>
-      </c>
-      <c r="M12" t="str">
-        <f t="shared" si="6"/>
-        <v>expExpLikelihoodFun</v>
-      </c>
-      <c r="N12" t="s">
-        <v>42</v>
-      </c>
-      <c r="O12" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="P12" t="str">
-        <f t="shared" si="8"/>
-        <v>function(a, margNum){MLEPlotter(a, expExpChartDomain, expExpLikelihoodFun ,"Beta")}</v>
+      <c r="H14" t="str">
+        <f t="shared" ref="H14" si="5">B14&amp;"Slider"</f>
+        <v>expExpXSlider</v>
+      </c>
+      <c r="I14" t="str">
+        <f>IF(E14=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+        <v>c("Beta0", "Beta1", "Beta2")</v>
+      </c>
+      <c r="J14" t="str">
+        <f>B14&amp;"PlotDistr"</f>
+        <v>expExpXPlotDistr</v>
+      </c>
+      <c r="K14" t="str">
+        <f>B14&amp;"Draws"</f>
+        <v>expExpXDraws</v>
+      </c>
+      <c r="L14" t="str">
+        <f>B14&amp;"Latex"</f>
+        <v>expExpXLatex</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="1"/>
+        <v>expExpXChartDomain</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="2"/>
+        <v>expExpXLikelihoodFun</v>
+      </c>
+      <c r="O14" t="str">
+        <f>IF(E14=1,"",", margNum")</f>
+        <v>, margNum</v>
+      </c>
+      <c r="P14" t="str">
+        <f>"function(a, margNum){MLEPlotter(a, "&amp;M14&amp;", "&amp;N14&amp;" ,"""&amp;F14&amp;""""&amp;O14&amp;")}"</f>
+        <v>function(a, margNum){MLEPlotter(a, expExpXChartDomain, expExpXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sim setup. Bug fixes
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\Code\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877C7FCE-DE08-43D1-BCD4-3EA1981FAEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3000D9-AA28-4034-A0CF-D60FDCD636A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,19 +647,19 @@
         <v>bernSlider</v>
       </c>
       <c r="I2" t="str">
-        <f>IF(E2=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+        <f t="shared" ref="I2:I14" si="0">IF(E2=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
         <v>c()</v>
       </c>
       <c r="J2" t="str">
-        <f>B2&amp;"PlotDistr"</f>
+        <f t="shared" ref="J2:J14" si="1">B2&amp;"PlotDistr"</f>
         <v>bernPlotDistr</v>
       </c>
       <c r="K2" t="str">
-        <f>B2&amp;"Draws"</f>
+        <f t="shared" ref="K2:K14" si="2">B2&amp;"Draws"</f>
         <v>bernDraws</v>
       </c>
       <c r="L2" t="str">
-        <f>B2&amp;"Latex"</f>
+        <f t="shared" ref="L2:L14" si="3">B2&amp;"Latex"</f>
         <v>bernLatex</v>
       </c>
       <c r="M2" t="str">
@@ -671,11 +671,11 @@
         <v>bernLikelihoodFun</v>
       </c>
       <c r="O2" t="str">
-        <f>IF(E2=1,"",", margNum")</f>
+        <f t="shared" ref="O2:O14" si="4">IF(E2=1,"",", margNum")</f>
         <v/>
       </c>
       <c r="P2" t="str">
-        <f>"function(a, margNum){MLEPlotter(a, "&amp;M2&amp;", "&amp;N2&amp;" ,"""&amp;F2&amp;""""&amp;O2&amp;")}"</f>
+        <f t="shared" ref="P2:P14" si="5">"function(a, margNum){MLEPlotter(a, "&amp;M2&amp;", "&amp;N2&amp;" ,"""&amp;F2&amp;""""&amp;O2&amp;")}"</f>
         <v>function(a, margNum){MLEPlotter(a, bernChartDomain, bernLikelihoodFun ,"Pi")}</v>
       </c>
     </row>
@@ -703,45 +703,45 @@
         <v>36</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H13" si="0">B3&amp;"Slider"</f>
+        <f t="shared" ref="H3:H13" si="6">B3&amp;"Slider"</f>
         <v>bernLogitSlider</v>
       </c>
       <c r="I3" t="str">
-        <f>IF(E3=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+        <f t="shared" si="0"/>
         <v>c()</v>
       </c>
       <c r="J3" t="str">
-        <f>B3&amp;"PlotDistr"</f>
+        <f t="shared" si="1"/>
         <v>bernLogitPlotDistr</v>
       </c>
       <c r="K3" t="str">
-        <f>B3&amp;"Draws"</f>
+        <f t="shared" si="2"/>
         <v>bernLogitDraws</v>
       </c>
       <c r="L3" t="str">
-        <f>B3&amp;"Latex"</f>
+        <f t="shared" si="3"/>
         <v>bernLogitLatex</v>
       </c>
       <c r="M3" t="str">
-        <f t="shared" ref="M3:M14" si="1">$B3&amp;"ChartDomain"</f>
+        <f t="shared" ref="M3:M14" si="7">$B3&amp;"ChartDomain"</f>
         <v>bernLogitChartDomain</v>
       </c>
       <c r="N3" t="str">
-        <f t="shared" ref="N3:N14" si="2">$B3&amp;"LikelihoodFun"</f>
+        <f t="shared" ref="N3:N14" si="8">$B3&amp;"LikelihoodFun"</f>
         <v>bernLogitLikelihoodFun</v>
       </c>
       <c r="O3" t="str">
-        <f>IF(E3=1,"",", margNum")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="P3" t="str">
-        <f>"function(a, margNum){MLEPlotter(a, "&amp;M3&amp;", "&amp;N3&amp;" ,"""&amp;F3&amp;""""&amp;O3&amp;")}"</f>
+        <f t="shared" si="5"/>
         <v>function(a, margNum){MLEPlotter(a, bernLogitChartDomain, bernLogitLikelihoodFun ,"Beta")}</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A14" si="3">A3+1</f>
+        <f t="shared" ref="A4:A14" si="9">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -763,45 +763,45 @@
         <v>36</v>
       </c>
       <c r="H4" t="str">
+        <f t="shared" si="6"/>
+        <v>bernLogitXSlider</v>
+      </c>
+      <c r="I4" t="str">
         <f t="shared" si="0"/>
-        <v>bernLogitXSlider</v>
-      </c>
-      <c r="I4" t="str">
-        <f>IF(E4=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="J4" t="str">
-        <f>B4&amp;"PlotDistr"</f>
+        <f t="shared" si="1"/>
         <v>bernLogitXPlotDistr</v>
       </c>
       <c r="K4" t="str">
-        <f>B4&amp;"Draws"</f>
+        <f t="shared" si="2"/>
         <v>bernLogitXDraws</v>
       </c>
       <c r="L4" t="str">
-        <f>B4&amp;"Latex"</f>
+        <f t="shared" si="3"/>
         <v>bernLogitXLatex</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>bernLogitXChartDomain</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>bernLogitXLikelihoodFun</v>
       </c>
       <c r="O4" t="str">
-        <f>IF(E4=1,"",", margNum")</f>
+        <f t="shared" si="4"/>
         <v>, margNum</v>
       </c>
       <c r="P4" t="str">
-        <f>"function(a, margNum){MLEPlotter(a, "&amp;M4&amp;", "&amp;N4&amp;" ,"""&amp;F4&amp;""""&amp;O4&amp;")}"</f>
+        <f t="shared" si="5"/>
         <v>function(a, margNum){MLEPlotter(a, bernLogitXChartDomain, bernLogitXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -823,45 +823,45 @@
         <v>37</v>
       </c>
       <c r="H5" t="str">
+        <f t="shared" si="6"/>
+        <v>styNormSlider</v>
+      </c>
+      <c r="I5" t="str">
         <f t="shared" si="0"/>
-        <v>styNormSlider</v>
-      </c>
-      <c r="I5" t="str">
-        <f>IF(E5=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
         <v>c()</v>
       </c>
       <c r="J5" t="str">
-        <f>B5&amp;"PlotDistr"</f>
+        <f t="shared" si="1"/>
         <v>styNormPlotDistr</v>
       </c>
       <c r="K5" t="str">
-        <f>B5&amp;"Draws"</f>
+        <f t="shared" si="2"/>
         <v>styNormDraws</v>
       </c>
       <c r="L5" t="str">
-        <f>B5&amp;"Latex"</f>
+        <f t="shared" si="3"/>
         <v>styNormLatex</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>styNormChartDomain</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>styNormLikelihoodFun</v>
       </c>
       <c r="O5" t="str">
-        <f>IF(E5=1,"",", margNum")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="P5" t="str">
-        <f>"function(a, margNum){MLEPlotter(a, "&amp;M5&amp;", "&amp;N5&amp;" ,"""&amp;F5&amp;""""&amp;O5&amp;")}"</f>
+        <f t="shared" si="5"/>
         <v>function(a, margNum){MLEPlotter(a, styNormChartDomain, styNormLikelihoodFun ,"Beta")}</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -883,45 +883,45 @@
         <v>37</v>
       </c>
       <c r="H6" t="str">
+        <f t="shared" si="6"/>
+        <v>multiNormSlider</v>
+      </c>
+      <c r="I6" t="str">
         <f t="shared" si="0"/>
-        <v>multiNormSlider</v>
-      </c>
-      <c r="I6" t="str">
-        <f>IF(E6=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="J6" t="str">
-        <f>B6&amp;"PlotDistr"</f>
+        <f t="shared" si="1"/>
         <v>multiNormPlotDistr</v>
       </c>
       <c r="K6" t="str">
-        <f>B6&amp;"Draws"</f>
+        <f t="shared" si="2"/>
         <v>multiNormDraws</v>
       </c>
       <c r="L6" t="str">
-        <f>B6&amp;"Latex"</f>
+        <f t="shared" si="3"/>
         <v>multiNormLatex</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>multiNormChartDomain</v>
       </c>
       <c r="N6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>multiNormLikelihoodFun</v>
       </c>
       <c r="O6" t="str">
-        <f>IF(E6=1,"",", margNum")</f>
+        <f t="shared" si="4"/>
         <v>, margNum</v>
       </c>
       <c r="P6" t="str">
-        <f>"function(a, margNum){MLEPlotter(a, "&amp;M6&amp;", "&amp;N6&amp;" ,"""&amp;F6&amp;""""&amp;O6&amp;")}"</f>
+        <f t="shared" si="5"/>
         <v>function(a, margNum){MLEPlotter(a, multiNormChartDomain, multiNormLikelihoodFun ,"Beta", margNum)}</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -943,45 +943,45 @@
         <v>37</v>
       </c>
       <c r="H7" t="str">
+        <f t="shared" si="6"/>
+        <v>logNormSlider</v>
+      </c>
+      <c r="I7" t="str">
         <f t="shared" si="0"/>
-        <v>logNormSlider</v>
-      </c>
-      <c r="I7" t="str">
-        <f>IF(E7=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
         <v>c()</v>
       </c>
       <c r="J7" t="str">
-        <f>B7&amp;"PlotDistr"</f>
+        <f t="shared" si="1"/>
         <v>logNormPlotDistr</v>
       </c>
       <c r="K7" t="str">
-        <f>B7&amp;"Draws"</f>
+        <f t="shared" si="2"/>
         <v>logNormDraws</v>
       </c>
       <c r="L7" t="str">
-        <f>B7&amp;"Latex"</f>
+        <f t="shared" si="3"/>
         <v>logNormLatex</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>logNormChartDomain</v>
       </c>
       <c r="N7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>logNormLikelihoodFun</v>
       </c>
       <c r="O7" t="str">
-        <f>IF(E7=1,"",", margNum")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="P7" t="str">
-        <f>"function(a, margNum){MLEPlotter(a, "&amp;M7&amp;", "&amp;N7&amp;" ,"""&amp;F7&amp;""""&amp;O7&amp;")}"</f>
+        <f t="shared" si="5"/>
         <v>function(a, margNum){MLEPlotter(a, logNormChartDomain, logNormLikelihoodFun ,"Beta")}</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1003,45 +1003,45 @@
         <v>37</v>
       </c>
       <c r="H8" t="str">
+        <f t="shared" si="6"/>
+        <v>logNormXSlider</v>
+      </c>
+      <c r="I8" t="str">
         <f t="shared" si="0"/>
-        <v>logNormXSlider</v>
-      </c>
-      <c r="I8" t="str">
-        <f>IF(E8=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="J8" t="str">
-        <f>B8&amp;"PlotDistr"</f>
+        <f t="shared" si="1"/>
         <v>logNormXPlotDistr</v>
       </c>
       <c r="K8" t="str">
-        <f>B8&amp;"Draws"</f>
+        <f t="shared" si="2"/>
         <v>logNormXDraws</v>
       </c>
       <c r="L8" t="str">
-        <f>B8&amp;"Latex"</f>
+        <f t="shared" si="3"/>
         <v>logNormXLatex</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>logNormXChartDomain</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>logNormXLikelihoodFun</v>
       </c>
       <c r="O8" t="str">
-        <f>IF(E8=1,"",", margNum")</f>
+        <f t="shared" si="4"/>
         <v>, margNum</v>
       </c>
       <c r="P8" t="str">
-        <f>"function(a, margNum){MLEPlotter(a, "&amp;M8&amp;", "&amp;N8&amp;" ,"""&amp;F8&amp;""""&amp;O8&amp;")}"</f>
+        <f t="shared" si="5"/>
         <v>function(a, margNum){MLEPlotter(a, logNormXChartDomain, logNormXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1063,45 +1063,45 @@
         <v>36</v>
       </c>
       <c r="H9" t="str">
+        <f t="shared" si="6"/>
+        <v>poisSlider</v>
+      </c>
+      <c r="I9" t="str">
         <f t="shared" si="0"/>
-        <v>poisSlider</v>
-      </c>
-      <c r="I9" t="str">
-        <f>IF(E9=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
         <v>c()</v>
       </c>
       <c r="J9" t="str">
-        <f>B9&amp;"PlotDistr"</f>
+        <f t="shared" si="1"/>
         <v>poisPlotDistr</v>
       </c>
       <c r="K9" t="str">
-        <f>B9&amp;"Draws"</f>
+        <f t="shared" si="2"/>
         <v>poisDraws</v>
       </c>
       <c r="L9" t="str">
-        <f>B9&amp;"Latex"</f>
+        <f t="shared" si="3"/>
         <v>poisLatex</v>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>poisChartDomain</v>
       </c>
       <c r="N9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>poisLikelihoodFun</v>
       </c>
       <c r="O9" t="str">
-        <f>IF(E9=1,"",", margNum")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="P9" t="str">
-        <f>"function(a, margNum){MLEPlotter(a, "&amp;M9&amp;", "&amp;N9&amp;" ,"""&amp;F9&amp;""""&amp;O9&amp;")}"</f>
+        <f t="shared" si="5"/>
         <v>function(a, margNum){MLEPlotter(a, poisChartDomain, poisLikelihoodFun ,"Lambda")}</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1123,45 +1123,45 @@
         <v>36</v>
       </c>
       <c r="H10" t="str">
+        <f t="shared" si="6"/>
+        <v>poisExpSlider</v>
+      </c>
+      <c r="I10" t="str">
         <f t="shared" si="0"/>
-        <v>poisExpSlider</v>
-      </c>
-      <c r="I10" t="str">
-        <f>IF(E10=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
         <v>c()</v>
       </c>
       <c r="J10" t="str">
-        <f>B10&amp;"PlotDistr"</f>
+        <f t="shared" si="1"/>
         <v>poisExpPlotDistr</v>
       </c>
       <c r="K10" t="str">
-        <f>B10&amp;"Draws"</f>
+        <f t="shared" si="2"/>
         <v>poisExpDraws</v>
       </c>
       <c r="L10" t="str">
-        <f>B10&amp;"Latex"</f>
+        <f t="shared" si="3"/>
         <v>poisExpLatex</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>poisExpChartDomain</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>poisExpLikelihoodFun</v>
       </c>
       <c r="O10" t="str">
-        <f>IF(E10=1,"",", margNum")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="P10" t="str">
-        <f>"function(a, margNum){MLEPlotter(a, "&amp;M10&amp;", "&amp;N10&amp;" ,"""&amp;F10&amp;""""&amp;O10&amp;")}"</f>
+        <f t="shared" si="5"/>
         <v>function(a, margNum){MLEPlotter(a, poisExpChartDomain, poisExpLikelihoodFun ,"Beta")}</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1183,45 +1183,45 @@
         <v>36</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" ref="H11" si="4">B11&amp;"Slider"</f>
+        <f t="shared" ref="H11" si="10">B11&amp;"Slider"</f>
         <v>poisExpXSlider</v>
       </c>
       <c r="I11" t="str">
-        <f>IF(E11=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+        <f t="shared" si="0"/>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="J11" t="str">
-        <f>B11&amp;"PlotDistr"</f>
+        <f t="shared" si="1"/>
         <v>poisExpXPlotDistr</v>
       </c>
       <c r="K11" t="str">
-        <f>B11&amp;"Draws"</f>
+        <f t="shared" si="2"/>
         <v>poisExpXDraws</v>
       </c>
       <c r="L11" t="str">
-        <f>B11&amp;"Latex"</f>
+        <f t="shared" si="3"/>
         <v>poisExpXLatex</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>poisExpXChartDomain</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>poisExpXLikelihoodFun</v>
       </c>
       <c r="O11" t="str">
-        <f>IF(E11=1,"",", margNum")</f>
+        <f t="shared" si="4"/>
         <v>, margNum</v>
       </c>
       <c r="P11" t="str">
-        <f>"function(a, margNum){MLEPlotter(a, "&amp;M11&amp;", "&amp;N11&amp;" ,"""&amp;F11&amp;""""&amp;O11&amp;")}"</f>
+        <f t="shared" si="5"/>
         <v>function(a, margNum){MLEPlotter(a, poisExpXChartDomain, poisExpXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1243,45 +1243,45 @@
         <v>37</v>
       </c>
       <c r="H12" t="str">
+        <f t="shared" si="6"/>
+        <v>expSlider</v>
+      </c>
+      <c r="I12" t="str">
         <f t="shared" si="0"/>
-        <v>expSlider</v>
-      </c>
-      <c r="I12" t="str">
-        <f>IF(E12=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
         <v>c()</v>
       </c>
       <c r="J12" t="str">
-        <f>B12&amp;"PlotDistr"</f>
+        <f t="shared" si="1"/>
         <v>expPlotDistr</v>
       </c>
       <c r="K12" t="str">
-        <f>B12&amp;"Draws"</f>
+        <f t="shared" si="2"/>
         <v>expDraws</v>
       </c>
       <c r="L12" t="str">
-        <f>B12&amp;"Latex"</f>
+        <f t="shared" si="3"/>
         <v>expLatex</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>expChartDomain</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>expLikelihoodFun</v>
       </c>
       <c r="O12" t="str">
-        <f>IF(E12=1,"",", margNum")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="P12" t="str">
-        <f>"function(a, margNum){MLEPlotter(a, "&amp;M12&amp;", "&amp;N12&amp;" ,"""&amp;F12&amp;""""&amp;O12&amp;")}"</f>
+        <f t="shared" si="5"/>
         <v>function(a, margNum){MLEPlotter(a, expChartDomain, expLikelihoodFun ,"Lambda")}</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1303,45 +1303,45 @@
         <v>37</v>
       </c>
       <c r="H13" t="str">
+        <f t="shared" si="6"/>
+        <v>expExpSlider</v>
+      </c>
+      <c r="I13" t="str">
         <f t="shared" si="0"/>
-        <v>expExpSlider</v>
-      </c>
-      <c r="I13" t="str">
-        <f>IF(E13=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
         <v>c()</v>
       </c>
       <c r="J13" t="str">
-        <f>B13&amp;"PlotDistr"</f>
+        <f t="shared" si="1"/>
         <v>expExpPlotDistr</v>
       </c>
       <c r="K13" t="str">
-        <f>B13&amp;"Draws"</f>
+        <f t="shared" si="2"/>
         <v>expExpDraws</v>
       </c>
       <c r="L13" t="str">
-        <f>B13&amp;"Latex"</f>
+        <f t="shared" si="3"/>
         <v>expExpLatex</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>expExpChartDomain</v>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>expExpLikelihoodFun</v>
       </c>
       <c r="O13" t="str">
-        <f>IF(E13=1,"",", margNum")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="P13" t="str">
-        <f>"function(a, margNum){MLEPlotter(a, "&amp;M13&amp;", "&amp;N13&amp;" ,"""&amp;F13&amp;""""&amp;O13&amp;")}"</f>
+        <f t="shared" si="5"/>
         <v>function(a, margNum){MLEPlotter(a, expExpChartDomain, expExpLikelihoodFun ,"Beta")}</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1363,39 +1363,39 @@
         <v>37</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" ref="H14" si="5">B14&amp;"Slider"</f>
+        <f t="shared" ref="H14" si="11">B14&amp;"Slider"</f>
         <v>expExpXSlider</v>
       </c>
       <c r="I14" t="str">
-        <f>IF(E14=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+        <f t="shared" si="0"/>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="J14" t="str">
-        <f>B14&amp;"PlotDistr"</f>
+        <f t="shared" si="1"/>
         <v>expExpXPlotDistr</v>
       </c>
       <c r="K14" t="str">
-        <f>B14&amp;"Draws"</f>
+        <f t="shared" si="2"/>
         <v>expExpXDraws</v>
       </c>
       <c r="L14" t="str">
-        <f>B14&amp;"Latex"</f>
+        <f t="shared" si="3"/>
         <v>expExpXLatex</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>expExpXChartDomain</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>expExpXLikelihoodFun</v>
       </c>
       <c r="O14" t="str">
-        <f>IF(E14=1,"",", margNum")</f>
+        <f t="shared" si="4"/>
         <v>, margNum</v>
       </c>
       <c r="P14" t="str">
-        <f>"function(a, margNum){MLEPlotter(a, "&amp;M14&amp;", "&amp;N14&amp;" ,"""&amp;F14&amp;""""&amp;O14&amp;")}"</f>
+        <f t="shared" si="5"/>
         <v>function(a, margNum){MLEPlotter(a, expExpXChartDomain, expExpXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
     </row>

</xml_diff>

<commit_message>
code cleanup and refactor to extricate transformed params
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\Code\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574C691A-4460-4863-A5C5-D0B74BD4CA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BB9F21-AAC0-4313-BDD8-F5DAEECE664A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
   <si>
     <t>Bernoulli-Pi</t>
   </si>
@@ -93,9 +93,6 @@
     <t>styNorm</t>
   </si>
   <si>
-    <t>multiNorm</t>
-  </si>
-  <si>
     <t>logNorm</t>
   </si>
   <si>
@@ -181,6 +178,12 @@
   </si>
   <si>
     <t>Poisson-Exp-X</t>
+  </si>
+  <si>
+    <t>transformFun</t>
+  </si>
+  <si>
+    <t>styNormX</t>
   </si>
 </sst>
 </file>
@@ -547,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,13 +567,14 @@
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="26" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -578,49 +582,52 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
       </c>
       <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P1" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -637,10 +644,10 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H2" t="str">
         <f>B2&amp;"Slider"</f>
@@ -651,35 +658,39 @@
         <v>c()</v>
       </c>
       <c r="J2" t="str">
-        <f t="shared" ref="J2:J14" si="1">B2&amp;"PlotDistr"</f>
+        <f>$B2&amp;"ParamTransform"</f>
+        <v>bernParamTransform</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="J2:K14" si="1">B2&amp;"PlotDistr"</f>
         <v>bernPlotDistr</v>
       </c>
-      <c r="K2" t="str">
-        <f t="shared" ref="K2:K14" si="2">B2&amp;"Draws"</f>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L14" si="2">B2&amp;"Draws"</f>
         <v>bernDraws</v>
       </c>
-      <c r="L2" t="str">
-        <f t="shared" ref="L2:L14" si="3">B2&amp;"Latex"</f>
+      <c r="M2" t="str">
+        <f t="shared" ref="M2:M14" si="3">B2&amp;"Latex"</f>
         <v>bernLatex</v>
       </c>
-      <c r="M2" t="str">
+      <c r="N2" t="str">
         <f>$B2&amp;"ChartDomain"</f>
         <v>bernChartDomain</v>
       </c>
-      <c r="N2" t="str">
+      <c r="O2" t="str">
         <f>$B2&amp;"LikelihoodFun"</f>
         <v>bernLikelihoodFun</v>
       </c>
-      <c r="O2" t="str">
-        <f t="shared" ref="O2:O14" si="4">IF(E2=1,"",", margNum")</f>
+      <c r="P2" t="str">
+        <f t="shared" ref="P2:P14" si="4">IF(E2=1,"",", margNum")</f>
         <v/>
       </c>
-      <c r="P2" t="str">
-        <f>"function(a, margNum){MLEstimator(a, "&amp;M2&amp;", "&amp;N2&amp;" ,"""&amp;F2&amp;""""&amp;O2&amp;")}"</f>
+      <c r="Q2" t="str">
+        <f>"function(a, margNum){MLEstimator(a, "&amp;N2&amp;", "&amp;O2&amp;" ,"""&amp;F2&amp;""""&amp;P2&amp;")}"</f>
         <v>function(a, margNum){MLEstimator(a, bernChartDomain, bernLikelihoodFun ,"Pi")}</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -697,10 +708,10 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H13" si="5">B3&amp;"Slider"</f>
@@ -711,37 +722,41 @@
         <v>c()</v>
       </c>
       <c r="J3" t="str">
+        <f t="shared" ref="J3:J14" si="6">$B3&amp;"ParamTransform"</f>
+        <v>bernLogitParamTransform</v>
+      </c>
+      <c r="K3" t="str">
         <f t="shared" si="1"/>
         <v>bernLogitPlotDistr</v>
       </c>
-      <c r="K3" t="str">
+      <c r="L3" t="str">
         <f t="shared" si="2"/>
         <v>bernLogitDraws</v>
       </c>
-      <c r="L3" t="str">
+      <c r="M3" t="str">
         <f t="shared" si="3"/>
         <v>bernLogitLatex</v>
       </c>
-      <c r="M3" t="str">
-        <f t="shared" ref="M3:M14" si="6">$B3&amp;"ChartDomain"</f>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N14" si="7">$B3&amp;"ChartDomain"</f>
         <v>bernLogitChartDomain</v>
       </c>
-      <c r="N3" t="str">
-        <f t="shared" ref="N3:N14" si="7">$B3&amp;"LikelihoodFun"</f>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O14" si="8">$B3&amp;"LikelihoodFun"</f>
         <v>bernLogitLikelihoodFun</v>
       </c>
-      <c r="O3" t="str">
+      <c r="P3" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="P3" t="str">
-        <f t="shared" ref="P3:P14" si="8">"function(a, margNum){MLEstimator(a, "&amp;M3&amp;", "&amp;N3&amp;" ,"""&amp;F3&amp;""""&amp;O3&amp;")}"</f>
+      <c r="Q3" t="str">
+        <f t="shared" ref="Q3:Q14" si="9">"function(a, margNum){MLEstimator(a, "&amp;N3&amp;", "&amp;O3&amp;" ,"""&amp;F3&amp;""""&amp;P3&amp;")}"</f>
         <v>function(a, margNum){MLEstimator(a, bernLogitChartDomain, bernLogitLikelihoodFun ,"Beta")}</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A14" si="9">A3+1</f>
+        <f t="shared" ref="A4:A14" si="10">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -757,10 +772,10 @@
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="5"/>
@@ -771,37 +786,41 @@
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="J4" t="str">
+        <f t="shared" si="6"/>
+        <v>bernLogitXParamTransform</v>
+      </c>
+      <c r="K4" t="str">
         <f t="shared" si="1"/>
         <v>bernLogitXPlotDistr</v>
       </c>
-      <c r="K4" t="str">
+      <c r="L4" t="str">
         <f t="shared" si="2"/>
         <v>bernLogitXDraws</v>
       </c>
-      <c r="L4" t="str">
+      <c r="M4" t="str">
         <f t="shared" si="3"/>
         <v>bernLogitXLatex</v>
       </c>
-      <c r="M4" t="str">
-        <f t="shared" si="6"/>
-        <v>bernLogitXChartDomain</v>
-      </c>
       <c r="N4" t="str">
         <f t="shared" si="7"/>
+        <v>bernLogitXChartDomain</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="8"/>
         <v>bernLogitXLikelihoodFun</v>
       </c>
-      <c r="O4" t="str">
+      <c r="P4" t="str">
         <f t="shared" si="4"/>
         <v>, margNum</v>
       </c>
-      <c r="P4" t="str">
-        <f t="shared" si="8"/>
+      <c r="Q4" t="str">
+        <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, bernLogitXChartDomain, bernLogitXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -817,10 +836,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="5"/>
@@ -831,41 +850,45 @@
         <v>c()</v>
       </c>
       <c r="J5" t="str">
+        <f t="shared" si="6"/>
+        <v>styNormParamTransform</v>
+      </c>
+      <c r="K5" t="str">
         <f t="shared" si="1"/>
         <v>styNormPlotDistr</v>
       </c>
-      <c r="K5" t="str">
+      <c r="L5" t="str">
         <f t="shared" si="2"/>
         <v>styNormDraws</v>
       </c>
-      <c r="L5" t="str">
+      <c r="M5" t="str">
         <f t="shared" si="3"/>
         <v>styNormLatex</v>
       </c>
-      <c r="M5" t="str">
-        <f t="shared" si="6"/>
-        <v>styNormChartDomain</v>
-      </c>
       <c r="N5" t="str">
         <f t="shared" si="7"/>
+        <v>styNormChartDomain</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="8"/>
         <v>styNormLikelihoodFun</v>
       </c>
-      <c r="O5" t="str">
+      <c r="P5" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="P5" t="str">
-        <f t="shared" si="8"/>
+      <c r="Q5" t="str">
+        <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, styNormChartDomain, styNormLikelihoodFun ,"Beta")}</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -877,55 +900,59 @@
         <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="5"/>
-        <v>multiNormSlider</v>
+        <v>styNormXSlider</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="J6" t="str">
+        <f t="shared" si="6"/>
+        <v>styNormXParamTransform</v>
+      </c>
+      <c r="K6" t="str">
         <f t="shared" si="1"/>
-        <v>multiNormPlotDistr</v>
-      </c>
-      <c r="K6" t="str">
+        <v>styNormXPlotDistr</v>
+      </c>
+      <c r="L6" t="str">
         <f t="shared" si="2"/>
-        <v>multiNormDraws</v>
-      </c>
-      <c r="L6" t="str">
+        <v>styNormXDraws</v>
+      </c>
+      <c r="M6" t="str">
         <f t="shared" si="3"/>
-        <v>multiNormLatex</v>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" si="6"/>
-        <v>multiNormChartDomain</v>
+        <v>styNormXLatex</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="7"/>
-        <v>multiNormLikelihoodFun</v>
+        <v>styNormXChartDomain</v>
       </c>
       <c r="O6" t="str">
+        <f t="shared" si="8"/>
+        <v>styNormXLikelihoodFun</v>
+      </c>
+      <c r="P6" t="str">
         <f t="shared" si="4"/>
         <v>, margNum</v>
       </c>
-      <c r="P6" t="str">
-        <f t="shared" si="8"/>
-        <v>function(a, margNum){MLEstimator(a, multiNormChartDomain, multiNormLikelihoodFun ,"Beta", margNum)}</v>
+      <c r="Q6" t="str">
+        <f t="shared" si="9"/>
+        <v>function(a, margNum){MLEstimator(a, styNormXChartDomain, styNormXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -937,10 +964,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="5"/>
@@ -951,41 +978,45 @@
         <v>c()</v>
       </c>
       <c r="J7" t="str">
+        <f t="shared" si="6"/>
+        <v>logNormParamTransform</v>
+      </c>
+      <c r="K7" t="str">
         <f t="shared" si="1"/>
         <v>logNormPlotDistr</v>
       </c>
-      <c r="K7" t="str">
+      <c r="L7" t="str">
         <f t="shared" si="2"/>
         <v>logNormDraws</v>
       </c>
-      <c r="L7" t="str">
+      <c r="M7" t="str">
         <f t="shared" si="3"/>
         <v>logNormLatex</v>
       </c>
-      <c r="M7" t="str">
-        <f t="shared" si="6"/>
-        <v>logNormChartDomain</v>
-      </c>
       <c r="N7" t="str">
         <f t="shared" si="7"/>
+        <v>logNormChartDomain</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="8"/>
         <v>logNormLikelihoodFun</v>
       </c>
-      <c r="O7" t="str">
+      <c r="P7" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="P7" t="str">
-        <f t="shared" si="8"/>
+      <c r="Q7" t="str">
+        <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, logNormChartDomain, logNormLikelihoodFun ,"Beta")}</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
@@ -997,10 +1028,10 @@
         <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="5"/>
@@ -1011,37 +1042,41 @@
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="J8" t="str">
+        <f t="shared" si="6"/>
+        <v>logNormXParamTransform</v>
+      </c>
+      <c r="K8" t="str">
         <f t="shared" si="1"/>
         <v>logNormXPlotDistr</v>
       </c>
-      <c r="K8" t="str">
+      <c r="L8" t="str">
         <f t="shared" si="2"/>
         <v>logNormXDraws</v>
       </c>
-      <c r="L8" t="str">
+      <c r="M8" t="str">
         <f t="shared" si="3"/>
         <v>logNormXLatex</v>
       </c>
-      <c r="M8" t="str">
-        <f t="shared" si="6"/>
-        <v>logNormXChartDomain</v>
-      </c>
       <c r="N8" t="str">
         <f t="shared" si="7"/>
+        <v>logNormXChartDomain</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="8"/>
         <v>logNormXLikelihoodFun</v>
       </c>
-      <c r="O8" t="str">
+      <c r="P8" t="str">
         <f t="shared" si="4"/>
         <v>, margNum</v>
       </c>
-      <c r="P8" t="str">
-        <f t="shared" si="8"/>
+      <c r="Q8" t="str">
+        <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, logNormXChartDomain, logNormXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1057,10 +1092,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="5"/>
@@ -1071,44 +1106,48 @@
         <v>c()</v>
       </c>
       <c r="J9" t="str">
+        <f t="shared" si="6"/>
+        <v>poisParamTransform</v>
+      </c>
+      <c r="K9" t="str">
         <f t="shared" si="1"/>
         <v>poisPlotDistr</v>
       </c>
-      <c r="K9" t="str">
+      <c r="L9" t="str">
         <f t="shared" si="2"/>
         <v>poisDraws</v>
       </c>
-      <c r="L9" t="str">
+      <c r="M9" t="str">
         <f t="shared" si="3"/>
         <v>poisLatex</v>
       </c>
-      <c r="M9" t="str">
-        <f t="shared" si="6"/>
-        <v>poisChartDomain</v>
-      </c>
       <c r="N9" t="str">
         <f t="shared" si="7"/>
+        <v>poisChartDomain</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="8"/>
         <v>poisLikelihoodFun</v>
       </c>
-      <c r="O9" t="str">
+      <c r="P9" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="P9" t="str">
-        <f t="shared" si="8"/>
+      <c r="Q9" t="str">
+        <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, poisChartDomain, poisLikelihoodFun ,"Lambda")}</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
@@ -1117,10 +1156,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="5"/>
@@ -1131,44 +1170,48 @@
         <v>c()</v>
       </c>
       <c r="J10" t="str">
+        <f t="shared" si="6"/>
+        <v>poisExpParamTransform</v>
+      </c>
+      <c r="K10" t="str">
         <f t="shared" si="1"/>
         <v>poisExpPlotDistr</v>
       </c>
-      <c r="K10" t="str">
+      <c r="L10" t="str">
         <f t="shared" si="2"/>
         <v>poisExpDraws</v>
       </c>
-      <c r="L10" t="str">
+      <c r="M10" t="str">
         <f t="shared" si="3"/>
         <v>poisExpLatex</v>
       </c>
-      <c r="M10" t="str">
-        <f t="shared" si="6"/>
-        <v>poisExpChartDomain</v>
-      </c>
       <c r="N10" t="str">
         <f t="shared" si="7"/>
+        <v>poisExpChartDomain</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="8"/>
         <v>poisExpLikelihoodFun</v>
       </c>
-      <c r="O10" t="str">
+      <c r="P10" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="P10" t="str">
-        <f t="shared" si="8"/>
+      <c r="Q10" t="str">
+        <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, poisExpChartDomain, poisExpLikelihoodFun ,"Beta")}</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>7</v>
@@ -1177,13 +1220,13 @@
         <v>3</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" ref="H11" si="10">B11&amp;"Slider"</f>
+        <f t="shared" ref="H11" si="11">B11&amp;"Slider"</f>
         <v>poisExpXSlider</v>
       </c>
       <c r="I11" t="str">
@@ -1191,41 +1234,45 @@
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="J11" t="str">
+        <f t="shared" si="6"/>
+        <v>poisExpXParamTransform</v>
+      </c>
+      <c r="K11" t="str">
         <f t="shared" si="1"/>
         <v>poisExpXPlotDistr</v>
       </c>
-      <c r="K11" t="str">
+      <c r="L11" t="str">
         <f t="shared" si="2"/>
         <v>poisExpXDraws</v>
       </c>
-      <c r="L11" t="str">
+      <c r="M11" t="str">
         <f t="shared" si="3"/>
         <v>poisExpXLatex</v>
       </c>
-      <c r="M11" t="str">
-        <f t="shared" si="6"/>
-        <v>poisExpXChartDomain</v>
-      </c>
       <c r="N11" t="str">
         <f t="shared" si="7"/>
+        <v>poisExpXChartDomain</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="8"/>
         <v>poisExpXLikelihoodFun</v>
       </c>
-      <c r="O11" t="str">
+      <c r="P11" t="str">
         <f t="shared" si="4"/>
         <v>, margNum</v>
       </c>
-      <c r="P11" t="str">
-        <f t="shared" si="8"/>
+      <c r="Q11" t="str">
+        <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, poisExpXChartDomain, poisExpXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>8</v>
@@ -1237,10 +1284,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="5"/>
@@ -1251,44 +1298,48 @@
         <v>c()</v>
       </c>
       <c r="J12" t="str">
+        <f t="shared" si="6"/>
+        <v>expParamTransform</v>
+      </c>
+      <c r="K12" t="str">
         <f t="shared" si="1"/>
         <v>expPlotDistr</v>
       </c>
-      <c r="K12" t="str">
+      <c r="L12" t="str">
         <f t="shared" si="2"/>
         <v>expDraws</v>
       </c>
-      <c r="L12" t="str">
+      <c r="M12" t="str">
         <f t="shared" si="3"/>
         <v>expLatex</v>
       </c>
-      <c r="M12" t="str">
-        <f t="shared" si="6"/>
-        <v>expChartDomain</v>
-      </c>
       <c r="N12" t="str">
         <f t="shared" si="7"/>
+        <v>expChartDomain</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="8"/>
         <v>expLikelihoodFun</v>
       </c>
-      <c r="O12" t="str">
+      <c r="P12" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="P12" t="str">
-        <f t="shared" si="8"/>
+      <c r="Q12" t="str">
+        <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, expChartDomain, expLikelihoodFun ,"Lambda")}</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
@@ -1297,10 +1348,10 @@
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="5"/>
@@ -1311,44 +1362,48 @@
         <v>c()</v>
       </c>
       <c r="J13" t="str">
+        <f t="shared" si="6"/>
+        <v>expExpParamTransform</v>
+      </c>
+      <c r="K13" t="str">
         <f t="shared" si="1"/>
         <v>expExpPlotDistr</v>
       </c>
-      <c r="K13" t="str">
+      <c r="L13" t="str">
         <f t="shared" si="2"/>
         <v>expExpDraws</v>
       </c>
-      <c r="L13" t="str">
+      <c r="M13" t="str">
         <f t="shared" si="3"/>
         <v>expExpLatex</v>
       </c>
-      <c r="M13" t="str">
-        <f t="shared" si="6"/>
-        <v>expExpChartDomain</v>
-      </c>
       <c r="N13" t="str">
         <f t="shared" si="7"/>
+        <v>expExpChartDomain</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="8"/>
         <v>expExpLikelihoodFun</v>
       </c>
-      <c r="O13" t="str">
+      <c r="P13" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="P13" t="str">
-        <f t="shared" si="8"/>
+      <c r="Q13" t="str">
+        <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, expExpChartDomain, expExpLikelihoodFun ,"Beta")}</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
@@ -1357,13 +1412,13 @@
         <v>3</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" ref="H14" si="11">B14&amp;"Slider"</f>
+        <f t="shared" ref="H14" si="12">B14&amp;"Slider"</f>
         <v>expExpXSlider</v>
       </c>
       <c r="I14" t="str">
@@ -1371,31 +1426,35 @@
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="J14" t="str">
+        <f t="shared" si="6"/>
+        <v>expExpXParamTransform</v>
+      </c>
+      <c r="K14" t="str">
         <f t="shared" si="1"/>
         <v>expExpXPlotDistr</v>
       </c>
-      <c r="K14" t="str">
+      <c r="L14" t="str">
         <f t="shared" si="2"/>
         <v>expExpXDraws</v>
       </c>
-      <c r="L14" t="str">
+      <c r="M14" t="str">
         <f t="shared" si="3"/>
         <v>expExpXLatex</v>
       </c>
-      <c r="M14" t="str">
-        <f t="shared" si="6"/>
-        <v>expExpXChartDomain</v>
-      </c>
       <c r="N14" t="str">
         <f t="shared" si="7"/>
+        <v>expExpXChartDomain</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="8"/>
         <v>expExpXLikelihoodFun</v>
       </c>
-      <c r="O14" t="str">
+      <c r="P14" t="str">
         <f t="shared" si="4"/>
         <v>, margNum</v>
       </c>
-      <c r="P14" t="str">
-        <f t="shared" si="8"/>
+      <c r="Q14" t="str">
+        <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, expExpXChartDomain, expExpXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor, adding expected values
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\Code\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BB9F21-AAC0-4313-BDD8-F5DAEECE664A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D2F8CC-DB2B-4959-B486-8C8EE0BDDF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -180,10 +180,10 @@
     <t>Poisson-Exp-X</t>
   </si>
   <si>
-    <t>transformFun</t>
-  </si>
-  <si>
     <t>styNormX</t>
+  </si>
+  <si>
+    <t>transformFunList</t>
   </si>
 </sst>
 </file>
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +603,7 @@
         <v>27</v>
       </c>
       <c r="J1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K1" t="s">
         <v>28</v>
@@ -662,7 +662,7 @@
         <v>bernParamTransform</v>
       </c>
       <c r="K2" t="str">
-        <f t="shared" ref="J2:K14" si="1">B2&amp;"PlotDistr"</f>
+        <f t="shared" ref="K2:K14" si="1">B2&amp;"PlotDistr"</f>
         <v>bernPlotDistr</v>
       </c>
       <c r="L2" t="str">
@@ -888,7 +888,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
better labeling of charts, bugfix
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\Code\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D2F8CC-DB2B-4959-B486-8C8EE0BDDF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767A6655-30C2-404A-AB87-9CC9738E76AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
   <si>
     <t>Bernoulli-Pi</t>
   </si>
@@ -184,6 +184,18 @@
   </si>
   <si>
     <t>transformFunList</t>
+  </si>
+  <si>
+    <t>simXAxis_Mu</t>
+  </si>
+  <si>
+    <t>$\\tilde{\\mu}$</t>
+  </si>
+  <si>
+    <t>$\\tilde{\\lambda}$</t>
+  </si>
+  <si>
+    <t>$\\tilde{\\pi} = \\tilde{Pr}(Y=1)$</t>
   </si>
 </sst>
 </file>
@@ -232,9 +244,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -550,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +587,7 @@
     <col min="14" max="16" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -626,8 +639,11 @@
       <c r="Q1" t="s">
         <v>29</v>
       </c>
+      <c r="R1" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -689,8 +705,11 @@
         <f>"function(a, margNum){MLEstimator(a, "&amp;N2&amp;", "&amp;O2&amp;" ,"""&amp;F2&amp;""""&amp;P2&amp;")}"</f>
         <v>function(a, margNum){MLEstimator(a, bernChartDomain, bernLikelihoodFun ,"Pi")}</v>
       </c>
+      <c r="R2" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -753,8 +772,11 @@
         <f t="shared" ref="Q3:Q14" si="9">"function(a, margNum){MLEstimator(a, "&amp;N3&amp;", "&amp;O3&amp;" ,"""&amp;F3&amp;""""&amp;P3&amp;")}"</f>
         <v>function(a, margNum){MLEstimator(a, bernLogitChartDomain, bernLogitLikelihoodFun ,"Beta")}</v>
       </c>
+      <c r="R3" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A14" si="10">A3+1</f>
         <v>3</v>
@@ -817,8 +839,11 @@
         <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, bernLogitXChartDomain, bernLogitXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
+      <c r="R4" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="10"/>
         <v>4</v>
@@ -881,8 +906,12 @@
         <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, styNormChartDomain, styNormLikelihoodFun ,"Beta")}</v>
       </c>
+      <c r="R5" t="s">
+        <v>51</v>
+      </c>
+      <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="10"/>
         <v>5</v>
@@ -945,8 +974,12 @@
         <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, styNormXChartDomain, styNormXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
+      <c r="R6" t="s">
+        <v>51</v>
+      </c>
+      <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="10"/>
         <v>6</v>
@@ -1009,8 +1042,12 @@
         <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, logNormChartDomain, logNormLikelihoodFun ,"Beta")}</v>
       </c>
+      <c r="R7" t="s">
+        <v>51</v>
+      </c>
+      <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="10"/>
         <v>7</v>
@@ -1073,8 +1110,12 @@
         <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, logNormXChartDomain, logNormXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
+      <c r="R8" t="s">
+        <v>51</v>
+      </c>
+      <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="10"/>
         <v>8</v>
@@ -1137,8 +1178,12 @@
         <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, poisChartDomain, poisLikelihoodFun ,"Lambda")}</v>
       </c>
+      <c r="R9" t="s">
+        <v>52</v>
+      </c>
+      <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="10"/>
         <v>9</v>
@@ -1201,8 +1246,12 @@
         <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, poisExpChartDomain, poisExpLikelihoodFun ,"Beta")}</v>
       </c>
+      <c r="R10" t="s">
+        <v>52</v>
+      </c>
+      <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="10"/>
         <v>10</v>
@@ -1265,8 +1314,12 @@
         <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, poisExpXChartDomain, poisExpXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
+      <c r="R11" t="s">
+        <v>52</v>
+      </c>
+      <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="10"/>
         <v>11</v>
@@ -1329,8 +1382,12 @@
         <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, expChartDomain, expLikelihoodFun ,"Lambda")}</v>
       </c>
+      <c r="R12" t="s">
+        <v>52</v>
+      </c>
+      <c r="T12" s="2"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="10"/>
         <v>12</v>
@@ -1393,8 +1450,12 @@
         <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, expExpChartDomain, expExpLikelihoodFun ,"Beta")}</v>
       </c>
+      <c r="R13" t="s">
+        <v>52</v>
+      </c>
+      <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="10"/>
         <v>13</v>
@@ -1457,8 +1518,13 @@
         <f t="shared" si="9"/>
         <v>function(a, margNum){MLEstimator(a, expExpXChartDomain, expExpXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
+      <c r="R14" t="s">
+        <v>52</v>
+      </c>
+      <c r="T14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Indentation changes, file renames, other vis changes
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\Code\probSimulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zagre\Documents\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767A6655-30C2-404A-AB87-9CC9738E76AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0244E0-5F70-4782-A057-C9B34CD55B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
   <si>
     <t>Bernoulli-Pi</t>
   </si>
@@ -196,6 +196,18 @@
   </si>
   <si>
     <t>$\\tilde{\\pi} = \\tilde{Pr}(Y=1)$</t>
+  </si>
+  <si>
+    <t>paramTex</t>
+  </si>
+  <si>
+    <t>\\pi</t>
+  </si>
+  <si>
+    <t>\\lambda</t>
+  </si>
+  <si>
+    <t>\\beta</t>
   </si>
 </sst>
 </file>
@@ -565,29 +577,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="15.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -642,8 +654,11 @@
       <c r="R1" t="s">
         <v>50</v>
       </c>
+      <c r="S1" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -708,8 +723,11 @@
       <c r="R2" t="s">
         <v>53</v>
       </c>
+      <c r="S2" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -775,8 +793,11 @@
       <c r="R3" t="s">
         <v>53</v>
       </c>
+      <c r="S3" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A14" si="10">A3+1</f>
         <v>3</v>
@@ -842,8 +863,11 @@
       <c r="R4" t="s">
         <v>53</v>
       </c>
+      <c r="S4" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="10"/>
         <v>4</v>
@@ -909,9 +933,12 @@
       <c r="R5" t="s">
         <v>51</v>
       </c>
+      <c r="S5" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="10"/>
         <v>5</v>
@@ -977,9 +1004,12 @@
       <c r="R6" t="s">
         <v>51</v>
       </c>
+      <c r="S6" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="10"/>
         <v>6</v>
@@ -1045,9 +1075,12 @@
       <c r="R7" t="s">
         <v>51</v>
       </c>
+      <c r="S7" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="10"/>
         <v>7</v>
@@ -1113,9 +1146,12 @@
       <c r="R8" t="s">
         <v>51</v>
       </c>
+      <c r="S8" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="10"/>
         <v>8</v>
@@ -1181,9 +1217,12 @@
       <c r="R9" t="s">
         <v>52</v>
       </c>
+      <c r="S9" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="10"/>
         <v>9</v>
@@ -1249,9 +1288,12 @@
       <c r="R10" t="s">
         <v>52</v>
       </c>
+      <c r="S10" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="10"/>
         <v>10</v>
@@ -1317,9 +1359,12 @@
       <c r="R11" t="s">
         <v>52</v>
       </c>
+      <c r="S11" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="10"/>
         <v>11</v>
@@ -1385,9 +1430,12 @@
       <c r="R12" t="s">
         <v>52</v>
       </c>
+      <c r="S12" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="T12" s="2"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="10"/>
         <v>12</v>
@@ -1453,9 +1501,12 @@
       <c r="R13" t="s">
         <v>52</v>
       </c>
+      <c r="S13" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="10"/>
         <v>13</v>
@@ -1520,6 +1571,9 @@
       </c>
       <c r="R14" t="s">
         <v>52</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="T14" s="2"/>
     </row>

</xml_diff>

<commit_message>
huge reorganization of most LaTeX generation. Better formatted front page.
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\Code\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DCB9B2-32CA-455F-9051-1AE1785AD0E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AA3425-F306-4C1A-988F-E99821DC9F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="59">
   <si>
     <t>Bernoulli-Pi</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>\lambda</t>
+  </si>
+  <si>
+    <t>metaParamTex</t>
   </si>
 </sst>
 </file>
@@ -578,7 +581,7 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S14"/>
+      <selection activeCell="T14" sqref="T9:T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,6 +660,9 @@
       <c r="S1" t="s">
         <v>54</v>
       </c>
+      <c r="T1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -724,6 +730,9 @@
         <v>53</v>
       </c>
       <c r="S2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>55</v>
       </c>
     </row>
@@ -796,6 +805,9 @@
       <c r="S3" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="T3" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -866,6 +878,9 @@
       <c r="S4" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="T4" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -936,7 +951,9 @@
       <c r="S5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="T5" s="2"/>
+      <c r="T5" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1007,7 +1024,9 @@
       <c r="S6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="T6" s="2"/>
+      <c r="T6" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1078,7 +1097,9 @@
       <c r="S7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="T7" s="2"/>
+      <c r="T7" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1149,7 +1170,9 @@
       <c r="S8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="T8" s="2"/>
+      <c r="T8" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1220,7 +1243,9 @@
       <c r="S9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="T9" s="2"/>
+      <c r="T9" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1291,7 +1316,9 @@
       <c r="S10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="T10" s="2"/>
+      <c r="T10" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1362,7 +1389,9 @@
       <c r="S11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="T11" s="2"/>
+      <c r="T11" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1433,7 +1462,9 @@
       <c r="S12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="T12" s="2"/>
+      <c r="T12" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1504,7 +1535,9 @@
       <c r="S13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="T13" s="2"/>
+      <c r="T13" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1575,7 +1608,9 @@
       <c r="S14" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="T14" s="2"/>
+      <c r="T14" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
many medium changes to visualization. Fix breaks-related bugs. refactor sliders.
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\Code\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AA3425-F306-4C1A-988F-E99821DC9F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC02A751-7FC3-4ACC-BBD5-B41DF1557AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="60">
   <si>
     <t>Bernoulli-Pi</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>metaParamTex</t>
+  </si>
+  <si>
+    <t>\mu</t>
   </si>
 </sst>
 </file>
@@ -580,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T14" sqref="T9:T14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5:T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,7 +955,7 @@
         <v>56</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -1025,7 +1028,7 @@
         <v>56</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1098,7 +1101,7 @@
         <v>56</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -1171,7 +1174,7 @@
         <v>56</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
first round of changes
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\Code\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC02A751-7FC3-4ACC-BBD5-B41DF1557AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EA7AE6-4876-4E06-9FE9-6E5C5E0051C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -584,7 +584,7 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5:T8"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
more features for probability tab. fixes on sim tab.
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\Code\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EA7AE6-4876-4E06-9FE9-6E5C5E0051C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72307D4-844F-4320-A223-B9433A6D24FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="63">
   <si>
     <t>Bernoulli-Pi</t>
   </si>
@@ -214,6 +214,15 @@
   </si>
   <si>
     <t>\mu</t>
+  </si>
+  <si>
+    <t>QOIList</t>
+  </si>
+  <si>
+    <t>list("Predicted Values", "Expected Values")</t>
+  </si>
+  <si>
+    <t>list("Predicted Values", "Expected Values", "Probability Y &gt; 1")</t>
   </si>
 </sst>
 </file>
@@ -581,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +614,7 @@
     <col min="14" max="16" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -666,8 +675,11 @@
       <c r="T1" t="s">
         <v>58</v>
       </c>
+      <c r="U1" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -738,8 +750,11 @@
       <c r="T2" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="U2" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -811,8 +826,11 @@
       <c r="T3" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="U3" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A14" si="10">A3+1</f>
         <v>3</v>
@@ -884,8 +902,11 @@
       <c r="T4" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="U4" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="10"/>
         <v>4</v>
@@ -957,8 +978,11 @@
       <c r="T5" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="U5" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="10"/>
         <v>5</v>
@@ -1030,8 +1054,11 @@
       <c r="T6" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="U6" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="10"/>
         <v>6</v>
@@ -1103,8 +1130,11 @@
       <c r="T7" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="U7" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="10"/>
         <v>7</v>
@@ -1176,8 +1206,11 @@
       <c r="T8" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="U8" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="10"/>
         <v>8</v>
@@ -1249,8 +1282,11 @@
       <c r="T9" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="U9" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="10"/>
         <v>9</v>
@@ -1322,8 +1358,11 @@
       <c r="T10" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="U10" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="10"/>
         <v>10</v>
@@ -1395,8 +1434,11 @@
       <c r="T11" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="U11" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="10"/>
         <v>11</v>
@@ -1468,8 +1510,11 @@
       <c r="T12" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="U12" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="10"/>
         <v>12</v>
@@ -1541,8 +1586,11 @@
       <c r="T13" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="U13" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="10"/>
         <v>13</v>
@@ -1613,6 +1661,9 @@
       </c>
       <c r="T14" s="2" t="s">
         <v>57</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix damn sim bug
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\Code\probSimulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zagre\Documents\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779649F1-1326-46CF-B6B5-FB57845573F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D15DC2-BA44-4F5A-9236-7CA5D38BE34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -210,12 +210,6 @@
     <t>list("Predicted Values", "Expected Values", "Probability Y &gt; 1")</t>
   </si>
   <si>
-    <t>list("Predicted Values", "Expected Values", "Sim.  Parameter")</t>
-  </si>
-  <si>
-    <t>list("Predicted Values", "Expected Values", "Probability Y &gt; 1", "Sim.  Parameter")</t>
-  </si>
-  <si>
     <t>simXAxis_param</t>
   </si>
   <si>
@@ -235,6 +229,12 @@
   </si>
   <si>
     <t>Expected Values of Y</t>
+  </si>
+  <si>
+    <t>list("Predicted Values", "Expected Values", "Sim. Parameter")</t>
+  </si>
+  <si>
+    <t>list("Predicted Values", "Expected Values", "Probability Y &gt; 1", "Sim. Parameter")</t>
   </si>
 </sst>
 </file>
@@ -604,29 +604,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="15.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -679,7 +679,7 @@
         <v>29</v>
       </c>
       <c r="R1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="S1" t="s">
         <v>50</v>
@@ -691,7 +691,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -754,7 +754,7 @@
         <v>function(a, margNum){MLEstimator(a, bernChartDomain, bernLikelihoodFun ,"Pi")}</v>
       </c>
       <c r="R2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>51</v>
@@ -763,10 +763,10 @@
         <v>51</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -830,7 +830,7 @@
         <v>function(a, margNum){MLEstimator(a, bernLogitChartDomain, bernLogitLikelihoodFun ,"Beta")}</v>
       </c>
       <c r="R3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>52</v>
@@ -839,10 +839,10 @@
         <v>51</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A14" si="10">A3+1</f>
         <v>3</v>
@@ -906,7 +906,7 @@
         <v>function(a, margNum){MLEstimator(a, bernLogitXChartDomain, bernLogitXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
       <c r="R4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>52</v>
@@ -915,10 +915,10 @@
         <v>51</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="10"/>
         <v>4</v>
@@ -982,7 +982,7 @@
         <v>function(a, margNum){MLEstimator(a, styNormChartDomain, styNormLikelihoodFun ,"Beta")}</v>
       </c>
       <c r="R5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>52</v>
@@ -991,10 +991,10 @@
         <v>55</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="10"/>
         <v>5</v>
@@ -1058,7 +1058,7 @@
         <v>function(a, margNum){MLEstimator(a, styNormXChartDomain, styNormXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
       <c r="R6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>52</v>
@@ -1067,10 +1067,10 @@
         <v>55</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="10"/>
         <v>6</v>
@@ -1134,7 +1134,7 @@
         <v>function(a, margNum){MLEstimator(a, logNormChartDomain, logNormLikelihoodFun ,"Beta")}</v>
       </c>
       <c r="R7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="S7" s="2" t="s">
         <v>52</v>
@@ -1146,7 +1146,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="10"/>
         <v>7</v>
@@ -1210,7 +1210,7 @@
         <v>function(a, margNum){MLEstimator(a, logNormXChartDomain, logNormXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
       <c r="R8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="S8" s="2" t="s">
         <v>52</v>
@@ -1222,7 +1222,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="10"/>
         <v>8</v>
@@ -1286,7 +1286,7 @@
         <v>function(a, margNum){MLEstimator(a, poisChartDomain, poisLikelihoodFun ,"Lambda")}</v>
       </c>
       <c r="R9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="S9" s="2" t="s">
         <v>53</v>
@@ -1295,10 +1295,10 @@
         <v>53</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="10"/>
         <v>9</v>
@@ -1362,7 +1362,7 @@
         <v>function(a, margNum){MLEstimator(a, poisExpChartDomain, poisExpLikelihoodFun ,"Beta")}</v>
       </c>
       <c r="R10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="S10" s="2" t="s">
         <v>52</v>
@@ -1371,10 +1371,10 @@
         <v>53</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="10"/>
         <v>10</v>
@@ -1438,7 +1438,7 @@
         <v>function(a, margNum){MLEstimator(a, poisExpXChartDomain, poisExpXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
       <c r="R11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="S11" s="2" t="s">
         <v>52</v>
@@ -1447,10 +1447,10 @@
         <v>53</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="10"/>
         <v>11</v>
@@ -1514,7 +1514,7 @@
         <v>function(a, margNum){MLEstimator(a, expChartDomain, expLikelihoodFun ,"Lambda")}</v>
       </c>
       <c r="R12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="S12" s="2" t="s">
         <v>53</v>
@@ -1523,10 +1523,10 @@
         <v>53</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="10"/>
         <v>12</v>
@@ -1590,7 +1590,7 @@
         <v>function(a, margNum){MLEstimator(a, expExpChartDomain, expExpLikelihoodFun ,"Beta")}</v>
       </c>
       <c r="R13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="S13" s="2" t="s">
         <v>52</v>
@@ -1599,10 +1599,10 @@
         <v>53</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="10"/>
         <v>13</v>
@@ -1666,7 +1666,7 @@
         <v>function(a, margNum){MLEstimator(a, expExpXChartDomain, expExpXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
       <c r="R14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="S14" s="2" t="s">
         <v>52</v>
@@ -1675,7 +1675,7 @@
         <v>53</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wide-ranging changes, mostly to UI. Reducing indentation.
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zagre\Documents\probSimulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\Code\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D15DC2-BA44-4F5A-9236-7CA5D38BE34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B88CA3-D66B-4CF9-8DFF-9E411D651536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="68">
   <si>
     <t>Bernoulli-Pi</t>
   </si>
@@ -213,28 +213,31 @@
     <t>simXAxis_param</t>
   </si>
   <si>
-    <t>Expected Values of Y $ = \\tilde{\\pi} = \\tilde{Pr}(Y=1)$</t>
-  </si>
-  <si>
-    <t>Expected Values of Y $ =\\tilde{\\pi} = \\tilde{Pr}(Y=1)$</t>
-  </si>
-  <si>
-    <t>Expected Values of Y $ =\\tilde{\\mu} = \\text{mean of } Y$</t>
-  </si>
-  <si>
-    <t>Expected Values of Y $ =\\tilde{\\lambda} = \\text{mean of } Y$</t>
-  </si>
-  <si>
-    <t>Expected Values of Y $ =\\tilde{\\lambda}$</t>
-  </si>
-  <si>
-    <t>Expected Values of Y</t>
-  </si>
-  <si>
     <t>list("Predicted Values", "Expected Values", "Sim. Parameter")</t>
   </si>
   <si>
     <t>list("Predicted Values", "Expected Values", "Probability Y &gt; 1", "Sim. Parameter")</t>
+  </si>
+  <si>
+    <t>$ \\tilde{E}(y) = \\tilde{\\pi} = \\tilde{Pr}(Y=1)$</t>
+  </si>
+  <si>
+    <t>$ \\tilde{E}(y) =\\tilde{\\pi} = \\tilde{Pr}(Y=1)$</t>
+  </si>
+  <si>
+    <t>$ \\tilde{E}(y) =\\tilde{\\mu} = \\text{mean of } Y$</t>
+  </si>
+  <si>
+    <t>$ \\tilde{E}(y)$</t>
+  </si>
+  <si>
+    <t>$ \\tilde{E}(y) =\\tilde{\\lambda} = \\text{mean of } Y$</t>
+  </si>
+  <si>
+    <t>$ \\tilde{E}(y) =\\tilde{\\lambda}$</t>
+  </si>
+  <si>
+    <t>list("Predicted Values", "Expected Values")</t>
   </si>
 </sst>
 </file>
@@ -604,29 +607,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26" customWidth="1"/>
-    <col min="11" max="11" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="15.54296875" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -691,7 +694,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -754,7 +757,7 @@
         <v>function(a, margNum){MLEstimator(a, bernChartDomain, bernLikelihoodFun ,"Pi")}</v>
       </c>
       <c r="R2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>51</v>
@@ -763,10 +766,10 @@
         <v>51</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -830,7 +833,7 @@
         <v>function(a, margNum){MLEstimator(a, bernLogitChartDomain, bernLogitLikelihoodFun ,"Beta")}</v>
       </c>
       <c r="R3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>52</v>
@@ -839,10 +842,10 @@
         <v>51</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A14" si="10">A3+1</f>
         <v>3</v>
@@ -906,7 +909,7 @@
         <v>function(a, margNum){MLEstimator(a, bernLogitXChartDomain, bernLogitXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
       <c r="R4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>52</v>
@@ -915,10 +918,10 @@
         <v>51</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="10"/>
         <v>4</v>
@@ -982,7 +985,7 @@
         <v>function(a, margNum){MLEstimator(a, styNormChartDomain, styNormLikelihoodFun ,"Beta")}</v>
       </c>
       <c r="R5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>52</v>
@@ -991,10 +994,10 @@
         <v>55</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="10"/>
         <v>5</v>
@@ -1058,7 +1061,7 @@
         <v>function(a, margNum){MLEstimator(a, styNormXChartDomain, styNormXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
       <c r="R6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>52</v>
@@ -1067,10 +1070,10 @@
         <v>55</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="10"/>
         <v>6</v>
@@ -1146,7 +1149,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="10"/>
         <v>7</v>
@@ -1219,10 +1222,10 @@
         <v>55</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="10"/>
         <v>8</v>
@@ -1286,7 +1289,7 @@
         <v>function(a, margNum){MLEstimator(a, poisChartDomain, poisLikelihoodFun ,"Lambda")}</v>
       </c>
       <c r="R9" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="S9" s="2" t="s">
         <v>53</v>
@@ -1295,10 +1298,10 @@
         <v>53</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="10"/>
         <v>9</v>
@@ -1362,7 +1365,7 @@
         <v>function(a, margNum){MLEstimator(a, poisExpChartDomain, poisExpLikelihoodFun ,"Beta")}</v>
       </c>
       <c r="R10" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="S10" s="2" t="s">
         <v>52</v>
@@ -1371,10 +1374,10 @@
         <v>53</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="10"/>
         <v>10</v>
@@ -1438,7 +1441,7 @@
         <v>function(a, margNum){MLEstimator(a, poisExpXChartDomain, poisExpXLikelihoodFun ,"Beta", margNum)}</v>
       </c>
       <c r="R11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="S11" s="2" t="s">
         <v>52</v>
@@ -1447,10 +1450,10 @@
         <v>53</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="10"/>
         <v>11</v>
@@ -1514,7 +1517,7 @@
         <v>function(a, margNum){MLEstimator(a, expChartDomain, expLikelihoodFun ,"Lambda")}</v>
       </c>
       <c r="R12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="S12" s="2" t="s">
         <v>53</v>
@@ -1523,10 +1526,10 @@
         <v>53</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="10"/>
         <v>12</v>
@@ -1599,10 +1602,10 @@
         <v>53</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="10"/>
         <v>13</v>
@@ -1675,7 +1678,7 @@
         <v>53</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enormous change to get assumed distr working properly
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\Code\probSimulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B88CA3-D66B-4CF9-8DFF-9E411D651536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BEF219-3E38-4D97-9911-16F455634B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="72">
   <si>
     <t>Bernoulli-Pi</t>
   </si>
@@ -147,9 +147,6 @@
     <t>likelihoodFun</t>
   </si>
   <si>
-    <t>addon</t>
-  </si>
-  <si>
     <t>paramName</t>
   </si>
   <si>
@@ -238,6 +235,21 @@
   </si>
   <si>
     <t>list("Predicted Values", "Expected Values")</t>
+  </si>
+  <si>
+    <t>list("Bernoulli-Pi","Bernoulli-Logit", "Bernoulli-Logit-X")</t>
+  </si>
+  <si>
+    <t>list("Poisson", "Poisson-Exp", "Poisson-Exp-X")</t>
+  </si>
+  <si>
+    <t>assumedDistrChoices</t>
+  </si>
+  <si>
+    <t>list("Stylized-Normal","Stylized-Normal-X","Log-Normal", "Log-Normal-X","Exponential", "Exponential-Exp", "Exponential-Exp-X")</t>
+  </si>
+  <si>
+    <t>list("Stylized-Normal","Stylized-Normal-X")</t>
   </si>
 </sst>
 </file>
@@ -286,10 +298,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -607,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,13 +631,14 @@
     <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -646,52 +658,52 @@
         <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
         <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="J1" t="s">
         <v>49</v>
       </c>
       <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>31</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>32</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>35</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>29</v>
-      </c>
-      <c r="R1" t="s">
-        <v>58</v>
-      </c>
-      <c r="S1" t="s">
-        <v>50</v>
-      </c>
-      <c r="T1" t="s">
-        <v>54</v>
-      </c>
-      <c r="U1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -711,62 +723,61 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H2" t="str">
+      <c r="H2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="1" t="str">
         <f>B2&amp;"Slider"</f>
         <v>bernSlider</v>
       </c>
-      <c r="I2" t="str">
-        <f t="shared" ref="I2:I14" si="0">IF(E2=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+      <c r="N2" t="str">
+        <f t="shared" ref="N2:N14" si="0">IF(E2=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
         <v>c()</v>
       </c>
-      <c r="J2" t="str">
+      <c r="O2" t="str">
         <f>$B2&amp;"ParamTransform"</f>
         <v>bernParamTransform</v>
       </c>
-      <c r="K2" t="str">
-        <f t="shared" ref="K2:K14" si="1">B2&amp;"PlotDistr"</f>
+      <c r="P2" t="str">
+        <f t="shared" ref="P2:P14" si="1">B2&amp;"PlotDistr"</f>
         <v>bernPlotDistr</v>
       </c>
-      <c r="L2" t="str">
-        <f t="shared" ref="L2:L14" si="2">B2&amp;"Draws"</f>
+      <c r="Q2" t="str">
+        <f t="shared" ref="Q2:Q14" si="2">B2&amp;"Draws"</f>
         <v>bernDraws</v>
       </c>
-      <c r="M2" t="str">
-        <f t="shared" ref="M2:M14" si="3">B2&amp;"Latex"</f>
+      <c r="R2" t="str">
+        <f t="shared" ref="R2:R14" si="3">B2&amp;"Latex"</f>
         <v>bernLatex</v>
       </c>
-      <c r="N2" t="str">
+      <c r="S2" t="str">
         <f>$B2&amp;"ChartDomain"</f>
         <v>bernChartDomain</v>
       </c>
-      <c r="O2" t="str">
+      <c r="T2" t="str">
         <f>$B2&amp;"LikelihoodFun"</f>
         <v>bernLikelihoodFun</v>
       </c>
-      <c r="P2" t="str">
-        <f t="shared" ref="P2:P14" si="4">IF(E2=1,"",", margNum")</f>
-        <v/>
-      </c>
-      <c r="Q2" t="str">
-        <f>"function(a, margNum){MLEstimator(a, "&amp;N2&amp;", "&amp;O2&amp;" ,"""&amp;F2&amp;""""&amp;P2&amp;")}"</f>
-        <v>function(a, margNum){MLEstimator(a, bernChartDomain, bernLikelihoodFun ,"Pi")}</v>
-      </c>
-      <c r="R2" t="s">
-        <v>61</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>59</v>
+      <c r="U2" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;S2&amp;", likelihoodFun = "&amp;T2&amp;" , paramName = """&amp;F2&amp;""",  xVals = xVals, margNum = margNum)}"</f>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernChartDomain, likelihoodFun = bernLikelihoodFun , paramName = "Pi",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -787,67 +798,66 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H13" si="5">B3&amp;"Slider"</f>
+      <c r="H3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="1" t="str">
+        <f t="shared" ref="M3:M13" si="4">B3&amp;"Slider"</f>
         <v>bernLogitSlider</v>
       </c>
-      <c r="I3" t="str">
+      <c r="N3" t="str">
         <f t="shared" si="0"/>
         <v>c()</v>
       </c>
-      <c r="J3" t="str">
-        <f t="shared" ref="J3:J14" si="6">$B3&amp;"ParamTransform"</f>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O14" si="5">$B3&amp;"ParamTransform"</f>
         <v>bernLogitParamTransform</v>
       </c>
-      <c r="K3" t="str">
+      <c r="P3" t="str">
         <f t="shared" si="1"/>
         <v>bernLogitPlotDistr</v>
       </c>
-      <c r="L3" t="str">
+      <c r="Q3" t="str">
         <f t="shared" si="2"/>
         <v>bernLogitDraws</v>
       </c>
-      <c r="M3" t="str">
+      <c r="R3" t="str">
         <f t="shared" si="3"/>
         <v>bernLogitLatex</v>
       </c>
-      <c r="N3" t="str">
-        <f t="shared" ref="N3:N14" si="7">$B3&amp;"ChartDomain"</f>
+      <c r="S3" t="str">
+        <f t="shared" ref="S3:S14" si="6">$B3&amp;"ChartDomain"</f>
         <v>bernLogitChartDomain</v>
       </c>
-      <c r="O3" t="str">
-        <f t="shared" ref="O3:O14" si="8">$B3&amp;"LikelihoodFun"</f>
+      <c r="T3" t="str">
+        <f t="shared" ref="T3:T14" si="7">$B3&amp;"LikelihoodFun"</f>
         <v>bernLogitLikelihoodFun</v>
       </c>
-      <c r="P3" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q14" si="9">"function(a, margNum){MLEstimator(a, "&amp;N3&amp;", "&amp;O3&amp;" ,"""&amp;F3&amp;""""&amp;P3&amp;")}"</f>
-        <v>function(a, margNum){MLEstimator(a, bernLogitChartDomain, bernLogitLikelihoodFun ,"Beta")}</v>
-      </c>
-      <c r="R3" t="s">
-        <v>62</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>59</v>
+      <c r="U3" t="str">
+        <f t="shared" ref="U3:U14" si="8">"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;S3&amp;", likelihoodFun = "&amp;T3&amp;" , paramName = """&amp;F3&amp;""",  xVals = xVals, margNum = margNum)}"</f>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernLogitChartDomain, likelihoodFun = bernLogitLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A14" si="10">A3+1</f>
+        <f t="shared" ref="A4:A14" si="9">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -863,67 +873,66 @@
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H4" t="str">
-        <f t="shared" si="5"/>
+      <c r="H4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>bernLogitXSlider</v>
       </c>
-      <c r="I4" t="str">
+      <c r="N4" t="str">
         <f t="shared" si="0"/>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
-      <c r="J4" t="str">
-        <f t="shared" si="6"/>
+      <c r="O4" t="str">
+        <f t="shared" si="5"/>
         <v>bernLogitXParamTransform</v>
       </c>
-      <c r="K4" t="str">
+      <c r="P4" t="str">
         <f t="shared" si="1"/>
         <v>bernLogitXPlotDistr</v>
       </c>
-      <c r="L4" t="str">
+      <c r="Q4" t="str">
         <f t="shared" si="2"/>
         <v>bernLogitXDraws</v>
       </c>
-      <c r="M4" t="str">
+      <c r="R4" t="str">
         <f t="shared" si="3"/>
         <v>bernLogitXLatex</v>
       </c>
-      <c r="N4" t="str">
+      <c r="S4" t="str">
+        <f t="shared" si="6"/>
+        <v>bernLogitXChartDomain</v>
+      </c>
+      <c r="T4" t="str">
         <f t="shared" si="7"/>
-        <v>bernLogitXChartDomain</v>
-      </c>
-      <c r="O4" t="str">
+        <v>bernLogitXLikelihoodFun</v>
+      </c>
+      <c r="U4" t="str">
         <f t="shared" si="8"/>
-        <v>bernLogitXLikelihoodFun</v>
-      </c>
-      <c r="P4" t="str">
-        <f t="shared" si="4"/>
-        <v>, margNum</v>
-      </c>
-      <c r="Q4" t="str">
-        <f t="shared" si="9"/>
-        <v>function(a, margNum){MLEstimator(a, bernLogitXChartDomain, bernLogitXLikelihoodFun ,"Beta", margNum)}</v>
-      </c>
-      <c r="R4" t="s">
-        <v>62</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>59</v>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernLogitXChartDomain, likelihoodFun = bernLogitXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -939,71 +948,70 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H5" t="str">
-        <f t="shared" si="5"/>
+      <c r="H5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M5" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>styNormSlider</v>
       </c>
-      <c r="I5" t="str">
+      <c r="N5" t="str">
         <f t="shared" si="0"/>
         <v>c()</v>
       </c>
-      <c r="J5" t="str">
-        <f t="shared" si="6"/>
+      <c r="O5" t="str">
+        <f t="shared" si="5"/>
         <v>styNormParamTransform</v>
       </c>
-      <c r="K5" t="str">
+      <c r="P5" t="str">
         <f t="shared" si="1"/>
         <v>styNormPlotDistr</v>
       </c>
-      <c r="L5" t="str">
+      <c r="Q5" t="str">
         <f t="shared" si="2"/>
         <v>styNormDraws</v>
       </c>
-      <c r="M5" t="str">
+      <c r="R5" t="str">
         <f t="shared" si="3"/>
         <v>styNormLatex</v>
       </c>
-      <c r="N5" t="str">
+      <c r="S5" t="str">
+        <f t="shared" si="6"/>
+        <v>styNormChartDomain</v>
+      </c>
+      <c r="T5" t="str">
         <f t="shared" si="7"/>
-        <v>styNormChartDomain</v>
-      </c>
-      <c r="O5" t="str">
+        <v>styNormLikelihoodFun</v>
+      </c>
+      <c r="U5" t="str">
         <f t="shared" si="8"/>
-        <v>styNormLikelihoodFun</v>
-      </c>
-      <c r="P5" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="Q5" t="str">
-        <f t="shared" si="9"/>
-        <v>function(a, margNum){MLEstimator(a, styNormChartDomain, styNormLikelihoodFun ,"Beta")}</v>
-      </c>
-      <c r="R5" t="s">
-        <v>63</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>60</v>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = styNormChartDomain, likelihoodFun = styNormLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -1015,67 +1023,66 @@
         <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H6" t="str">
-        <f t="shared" si="5"/>
+      <c r="H6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M6" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>styNormXSlider</v>
       </c>
-      <c r="I6" t="str">
+      <c r="N6" t="str">
         <f t="shared" si="0"/>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
-      <c r="J6" t="str">
-        <f t="shared" si="6"/>
+      <c r="O6" t="str">
+        <f t="shared" si="5"/>
         <v>styNormXParamTransform</v>
       </c>
-      <c r="K6" t="str">
+      <c r="P6" t="str">
         <f t="shared" si="1"/>
         <v>styNormXPlotDistr</v>
       </c>
-      <c r="L6" t="str">
+      <c r="Q6" t="str">
         <f t="shared" si="2"/>
         <v>styNormXDraws</v>
       </c>
-      <c r="M6" t="str">
+      <c r="R6" t="str">
         <f t="shared" si="3"/>
         <v>styNormXLatex</v>
       </c>
-      <c r="N6" t="str">
+      <c r="S6" t="str">
+        <f t="shared" si="6"/>
+        <v>styNormXChartDomain</v>
+      </c>
+      <c r="T6" t="str">
         <f t="shared" si="7"/>
-        <v>styNormXChartDomain</v>
-      </c>
-      <c r="O6" t="str">
+        <v>styNormXLikelihoodFun</v>
+      </c>
+      <c r="U6" t="str">
         <f t="shared" si="8"/>
-        <v>styNormXLikelihoodFun</v>
-      </c>
-      <c r="P6" t="str">
-        <f t="shared" si="4"/>
-        <v>, margNum</v>
-      </c>
-      <c r="Q6" t="str">
-        <f t="shared" si="9"/>
-        <v>function(a, margNum){MLEstimator(a, styNormXChartDomain, styNormXLikelihoodFun ,"Beta", margNum)}</v>
-      </c>
-      <c r="R6" t="s">
-        <v>63</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>60</v>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = styNormXChartDomain, likelihoodFun = styNormXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1091,67 +1098,66 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H7" t="str">
-        <f t="shared" si="5"/>
+      <c r="H7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M7" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>logNormSlider</v>
       </c>
-      <c r="I7" t="str">
+      <c r="N7" t="str">
         <f t="shared" si="0"/>
         <v>c()</v>
       </c>
-      <c r="J7" t="str">
-        <f t="shared" si="6"/>
+      <c r="O7" t="str">
+        <f t="shared" si="5"/>
         <v>logNormParamTransform</v>
       </c>
-      <c r="K7" t="str">
+      <c r="P7" t="str">
         <f t="shared" si="1"/>
         <v>logNormPlotDistr</v>
       </c>
-      <c r="L7" t="str">
+      <c r="Q7" t="str">
         <f t="shared" si="2"/>
         <v>logNormDraws</v>
       </c>
-      <c r="M7" t="str">
+      <c r="R7" t="str">
         <f t="shared" si="3"/>
         <v>logNormLatex</v>
       </c>
-      <c r="N7" t="str">
+      <c r="S7" t="str">
+        <f t="shared" si="6"/>
+        <v>logNormChartDomain</v>
+      </c>
+      <c r="T7" t="str">
         <f t="shared" si="7"/>
-        <v>logNormChartDomain</v>
-      </c>
-      <c r="O7" t="str">
+        <v>logNormLikelihoodFun</v>
+      </c>
+      <c r="U7" t="str">
         <f t="shared" si="8"/>
-        <v>logNormLikelihoodFun</v>
-      </c>
-      <c r="P7" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="Q7" t="str">
-        <f t="shared" si="9"/>
-        <v>function(a, margNum){MLEstimator(a, logNormChartDomain, logNormLikelihoodFun ,"Beta")}</v>
-      </c>
-      <c r="R7" t="s">
-        <v>64</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>57</v>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = logNormChartDomain, likelihoodFun = logNormLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1167,67 +1173,66 @@
         <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H8" t="str">
-        <f t="shared" si="5"/>
+      <c r="H8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>logNormXSlider</v>
       </c>
-      <c r="I8" t="str">
+      <c r="N8" t="str">
         <f t="shared" si="0"/>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
-      <c r="J8" t="str">
-        <f t="shared" si="6"/>
+      <c r="O8" t="str">
+        <f t="shared" si="5"/>
         <v>logNormXParamTransform</v>
       </c>
-      <c r="K8" t="str">
+      <c r="P8" t="str">
         <f t="shared" si="1"/>
         <v>logNormXPlotDistr</v>
       </c>
-      <c r="L8" t="str">
+      <c r="Q8" t="str">
         <f t="shared" si="2"/>
         <v>logNormXDraws</v>
       </c>
-      <c r="M8" t="str">
+      <c r="R8" t="str">
         <f t="shared" si="3"/>
         <v>logNormXLatex</v>
       </c>
-      <c r="N8" t="str">
+      <c r="S8" t="str">
+        <f t="shared" si="6"/>
+        <v>logNormXChartDomain</v>
+      </c>
+      <c r="T8" t="str">
         <f t="shared" si="7"/>
-        <v>logNormXChartDomain</v>
-      </c>
-      <c r="O8" t="str">
+        <v>logNormXLikelihoodFun</v>
+      </c>
+      <c r="U8" t="str">
         <f t="shared" si="8"/>
-        <v>logNormXLikelihoodFun</v>
-      </c>
-      <c r="P8" t="str">
-        <f t="shared" si="4"/>
-        <v>, margNum</v>
-      </c>
-      <c r="Q8" t="str">
-        <f t="shared" si="9"/>
-        <v>function(a, margNum){MLEstimator(a, logNormXChartDomain, logNormXLikelihoodFun ,"Beta", margNum)}</v>
-      </c>
-      <c r="R8" t="s">
-        <v>64</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>67</v>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = logNormXChartDomain, likelihoodFun = logNormXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1243,74 +1248,73 @@
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H9" t="str">
-        <f t="shared" si="5"/>
+      <c r="H9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M9" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>poisSlider</v>
       </c>
-      <c r="I9" t="str">
+      <c r="N9" t="str">
         <f t="shared" si="0"/>
         <v>c()</v>
       </c>
-      <c r="J9" t="str">
-        <f t="shared" si="6"/>
+      <c r="O9" t="str">
+        <f t="shared" si="5"/>
         <v>poisParamTransform</v>
       </c>
-      <c r="K9" t="str">
+      <c r="P9" t="str">
         <f t="shared" si="1"/>
         <v>poisPlotDistr</v>
       </c>
-      <c r="L9" t="str">
+      <c r="Q9" t="str">
         <f t="shared" si="2"/>
         <v>poisDraws</v>
       </c>
-      <c r="M9" t="str">
+      <c r="R9" t="str">
         <f t="shared" si="3"/>
         <v>poisLatex</v>
       </c>
-      <c r="N9" t="str">
+      <c r="S9" t="str">
+        <f t="shared" si="6"/>
+        <v>poisChartDomain</v>
+      </c>
+      <c r="T9" t="str">
         <f t="shared" si="7"/>
-        <v>poisChartDomain</v>
-      </c>
-      <c r="O9" t="str">
+        <v>poisLikelihoodFun</v>
+      </c>
+      <c r="U9" t="str">
         <f t="shared" si="8"/>
-        <v>poisLikelihoodFun</v>
-      </c>
-      <c r="P9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="Q9" t="str">
-        <f t="shared" si="9"/>
-        <v>function(a, margNum){MLEstimator(a, poisChartDomain, poisLikelihoodFun ,"Lambda")}</v>
-      </c>
-      <c r="R9" t="s">
-        <v>65</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="T9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>59</v>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisChartDomain, likelihoodFun = poisLikelihoodFun , paramName = "Lambda",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
@@ -1319,74 +1323,73 @@
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H10" t="str">
-        <f t="shared" si="5"/>
+      <c r="H10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M10" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>poisExpSlider</v>
       </c>
-      <c r="I10" t="str">
+      <c r="N10" t="str">
         <f t="shared" si="0"/>
         <v>c()</v>
       </c>
-      <c r="J10" t="str">
-        <f t="shared" si="6"/>
+      <c r="O10" t="str">
+        <f t="shared" si="5"/>
         <v>poisExpParamTransform</v>
       </c>
-      <c r="K10" t="str">
+      <c r="P10" t="str">
         <f t="shared" si="1"/>
         <v>poisExpPlotDistr</v>
       </c>
-      <c r="L10" t="str">
+      <c r="Q10" t="str">
         <f t="shared" si="2"/>
         <v>poisExpDraws</v>
       </c>
-      <c r="M10" t="str">
+      <c r="R10" t="str">
         <f t="shared" si="3"/>
         <v>poisExpLatex</v>
       </c>
-      <c r="N10" t="str">
+      <c r="S10" t="str">
+        <f t="shared" si="6"/>
+        <v>poisExpChartDomain</v>
+      </c>
+      <c r="T10" t="str">
         <f t="shared" si="7"/>
-        <v>poisExpChartDomain</v>
-      </c>
-      <c r="O10" t="str">
+        <v>poisExpLikelihoodFun</v>
+      </c>
+      <c r="U10" t="str">
         <f t="shared" si="8"/>
-        <v>poisExpLikelihoodFun</v>
-      </c>
-      <c r="P10" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="Q10" t="str">
-        <f t="shared" si="9"/>
-        <v>function(a, margNum){MLEstimator(a, poisExpChartDomain, poisExpLikelihoodFun ,"Beta")}</v>
-      </c>
-      <c r="R10" t="s">
-        <v>65</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>60</v>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisExpChartDomain, likelihoodFun = poisExpLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>7</v>
@@ -1395,67 +1398,66 @@
         <v>3</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H11" t="str">
-        <f t="shared" ref="H11" si="11">B11&amp;"Slider"</f>
+      <c r="H11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M11" s="1" t="str">
+        <f t="shared" ref="M11" si="10">B11&amp;"Slider"</f>
         <v>poisExpXSlider</v>
       </c>
-      <c r="I11" t="str">
+      <c r="N11" t="str">
         <f t="shared" si="0"/>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
-      <c r="J11" t="str">
-        <f t="shared" si="6"/>
+      <c r="O11" t="str">
+        <f t="shared" si="5"/>
         <v>poisExpXParamTransform</v>
       </c>
-      <c r="K11" t="str">
+      <c r="P11" t="str">
         <f t="shared" si="1"/>
         <v>poisExpXPlotDistr</v>
       </c>
-      <c r="L11" t="str">
+      <c r="Q11" t="str">
         <f t="shared" si="2"/>
         <v>poisExpXDraws</v>
       </c>
-      <c r="M11" t="str">
+      <c r="R11" t="str">
         <f t="shared" si="3"/>
         <v>poisExpXLatex</v>
       </c>
-      <c r="N11" t="str">
+      <c r="S11" t="str">
+        <f t="shared" si="6"/>
+        <v>poisExpXChartDomain</v>
+      </c>
+      <c r="T11" t="str">
         <f t="shared" si="7"/>
-        <v>poisExpXChartDomain</v>
-      </c>
-      <c r="O11" t="str">
+        <v>poisExpXLikelihoodFun</v>
+      </c>
+      <c r="U11" t="str">
         <f t="shared" si="8"/>
-        <v>poisExpXLikelihoodFun</v>
-      </c>
-      <c r="P11" t="str">
-        <f t="shared" si="4"/>
-        <v>, margNum</v>
-      </c>
-      <c r="Q11" t="str">
-        <f t="shared" si="9"/>
-        <v>function(a, margNum){MLEstimator(a, poisExpXChartDomain, poisExpXLikelihoodFun ,"Beta", margNum)}</v>
-      </c>
-      <c r="R11" t="s">
-        <v>65</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>60</v>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisExpXChartDomain, likelihoodFun = poisExpXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1471,74 +1473,73 @@
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H12" t="str">
-        <f t="shared" si="5"/>
+      <c r="H12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M12" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>expSlider</v>
       </c>
-      <c r="I12" t="str">
+      <c r="N12" t="str">
         <f t="shared" si="0"/>
         <v>c()</v>
       </c>
-      <c r="J12" t="str">
-        <f t="shared" si="6"/>
+      <c r="O12" t="str">
+        <f t="shared" si="5"/>
         <v>expParamTransform</v>
       </c>
-      <c r="K12" t="str">
+      <c r="P12" t="str">
         <f t="shared" si="1"/>
         <v>expPlotDistr</v>
       </c>
-      <c r="L12" t="str">
+      <c r="Q12" t="str">
         <f t="shared" si="2"/>
         <v>expDraws</v>
       </c>
-      <c r="M12" t="str">
+      <c r="R12" t="str">
         <f t="shared" si="3"/>
         <v>expLatex</v>
       </c>
-      <c r="N12" t="str">
+      <c r="S12" t="str">
+        <f t="shared" si="6"/>
+        <v>expChartDomain</v>
+      </c>
+      <c r="T12" t="str">
         <f t="shared" si="7"/>
-        <v>expChartDomain</v>
-      </c>
-      <c r="O12" t="str">
+        <v>expLikelihoodFun</v>
+      </c>
+      <c r="U12" t="str">
         <f t="shared" si="8"/>
-        <v>expLikelihoodFun</v>
-      </c>
-      <c r="P12" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="Q12" t="str">
-        <f t="shared" si="9"/>
-        <v>function(a, margNum){MLEstimator(a, expChartDomain, expLikelihoodFun ,"Lambda")}</v>
-      </c>
-      <c r="R12" t="s">
-        <v>66</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="T12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>60</v>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expChartDomain, likelihoodFun = expLikelihoodFun , paramName = "Lambda",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
@@ -1547,74 +1548,73 @@
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H13" t="str">
-        <f t="shared" si="5"/>
+      <c r="H13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M13" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>expExpSlider</v>
       </c>
-      <c r="I13" t="str">
+      <c r="N13" t="str">
         <f t="shared" si="0"/>
         <v>c()</v>
       </c>
-      <c r="J13" t="str">
-        <f t="shared" si="6"/>
+      <c r="O13" t="str">
+        <f t="shared" si="5"/>
         <v>expExpParamTransform</v>
       </c>
-      <c r="K13" t="str">
+      <c r="P13" t="str">
         <f t="shared" si="1"/>
         <v>expExpPlotDistr</v>
       </c>
-      <c r="L13" t="str">
+      <c r="Q13" t="str">
         <f t="shared" si="2"/>
         <v>expExpDraws</v>
       </c>
-      <c r="M13" t="str">
+      <c r="R13" t="str">
         <f t="shared" si="3"/>
         <v>expExpLatex</v>
       </c>
-      <c r="N13" t="str">
+      <c r="S13" t="str">
+        <f t="shared" si="6"/>
+        <v>expExpChartDomain</v>
+      </c>
+      <c r="T13" t="str">
         <f t="shared" si="7"/>
-        <v>expExpChartDomain</v>
-      </c>
-      <c r="O13" t="str">
+        <v>expExpLikelihoodFun</v>
+      </c>
+      <c r="U13" t="str">
         <f t="shared" si="8"/>
-        <v>expExpLikelihoodFun</v>
-      </c>
-      <c r="P13" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="Q13" t="str">
-        <f t="shared" si="9"/>
-        <v>function(a, margNum){MLEstimator(a, expExpChartDomain, expExpLikelihoodFun ,"Beta")}</v>
-      </c>
-      <c r="R13" t="s">
-        <v>64</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>60</v>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expExpChartDomain, likelihoodFun = expExpLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
@@ -1623,62 +1623,61 @@
         <v>3</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H14" t="str">
-        <f t="shared" ref="H14" si="12">B14&amp;"Slider"</f>
+      <c r="H14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M14" s="1" t="str">
+        <f t="shared" ref="M14" si="11">B14&amp;"Slider"</f>
         <v>expExpXSlider</v>
       </c>
-      <c r="I14" t="str">
+      <c r="N14" t="str">
         <f t="shared" si="0"/>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
-      <c r="J14" t="str">
-        <f t="shared" si="6"/>
+      <c r="O14" t="str">
+        <f t="shared" si="5"/>
         <v>expExpXParamTransform</v>
       </c>
-      <c r="K14" t="str">
+      <c r="P14" t="str">
         <f t="shared" si="1"/>
         <v>expExpXPlotDistr</v>
       </c>
-      <c r="L14" t="str">
+      <c r="Q14" t="str">
         <f t="shared" si="2"/>
         <v>expExpXDraws</v>
       </c>
-      <c r="M14" t="str">
+      <c r="R14" t="str">
         <f t="shared" si="3"/>
         <v>expExpXLatex</v>
       </c>
-      <c r="N14" t="str">
+      <c r="S14" t="str">
+        <f t="shared" si="6"/>
+        <v>expExpXChartDomain</v>
+      </c>
+      <c r="T14" t="str">
         <f t="shared" si="7"/>
-        <v>expExpXChartDomain</v>
-      </c>
-      <c r="O14" t="str">
+        <v>expExpXLikelihoodFun</v>
+      </c>
+      <c r="U14" t="str">
         <f t="shared" si="8"/>
-        <v>expExpXLikelihoodFun</v>
-      </c>
-      <c r="P14" t="str">
-        <f t="shared" si="4"/>
-        <v>, margNum</v>
-      </c>
-      <c r="Q14" t="str">
-        <f t="shared" si="9"/>
-        <v>function(a, margNum){MLEstimator(a, expExpXChartDomain, expExpXLikelihoodFun ,"Beta", margNum)}</v>
-      </c>
-      <c r="R14" t="s">
-        <v>64</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>60</v>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expExpXChartDomain, likelihoodFun = expExpXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor. Addition of normal dist
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF0EBD6-BAC2-409E-B657-886078D27EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88ED5574-91F0-4D0B-89FA-4D3B8476EFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="75">
   <si>
     <t>Bernoulli-Pi</t>
   </si>
@@ -222,18 +222,9 @@
     <t>$ \\tilde{E}(y) =\\tilde{\\pi} = \\tilde{Pr}(Y=1)$</t>
   </si>
   <si>
-    <t>$ \\tilde{E}(y) =\\tilde{\\mu} = \\text{mean of } Y$</t>
-  </si>
-  <si>
     <t>$ \\tilde{E}(y)$</t>
   </si>
   <si>
-    <t>$ \\tilde{E}(y) =\\tilde{\\lambda} = \\text{mean of } Y$</t>
-  </si>
-  <si>
-    <t>$ \\tilde{E}(y) =\\tilde{\\lambda}$</t>
-  </si>
-  <si>
     <t>list("Predicted Values", "Expected Values")</t>
   </si>
   <si>
@@ -250,6 +241,24 @@
   </si>
   <si>
     <t>list("Stylized-Normal","Stylized-Normal-X")</t>
+  </si>
+  <si>
+    <t>Normal-X</t>
+  </si>
+  <si>
+    <t>fullNormX</t>
+  </si>
+  <si>
+    <t>list("Normal-X")</t>
+  </si>
+  <si>
+    <t>nCovarList</t>
+  </si>
+  <si>
+    <t>$ \\tilde{E}(y) =\\tilde{\\mu} = \\bar{Y}$</t>
+  </si>
+  <si>
+    <t>$ \\tilde{E}(y) =\\tilde{\\lambda} = \\bar{Y}$</t>
   </si>
 </sst>
 </file>
@@ -616,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,19 +638,20 @@
     <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -658,55 +668,58 @@
         <v>26</v>
       </c>
       <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
-        <v>69</v>
-      </c>
       <c r="I1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" t="s">
         <v>57</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>49</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>53</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>55</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>48</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>31</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>35</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>36</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -722,67 +735,69 @@
       <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="I2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>50</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M2" s="1" t="str">
+      <c r="N2" s="1" t="str">
         <f>B2&amp;"Slider"</f>
         <v>bernSlider</v>
       </c>
-      <c r="N2" t="str">
-        <f t="shared" ref="N2:N14" si="0">IF(E2=1,"c()", "c(""Beta0"", ""Beta1"", ""Beta2"")")</f>
+      <c r="O2" t="str">
+        <f>IF(E2=1,"c()", IF(E2=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
-      <c r="O2" t="str">
+      <c r="P2" t="str">
         <f>$B2&amp;"ParamTransform"</f>
         <v>bernParamTransform</v>
       </c>
-      <c r="P2" t="str">
-        <f t="shared" ref="P2:P14" si="1">B2&amp;"PlotDistr"</f>
+      <c r="Q2" t="str">
+        <f t="shared" ref="Q2:Q15" si="0">B2&amp;"PlotDistr"</f>
         <v>bernPlotDistr</v>
       </c>
-      <c r="Q2" t="str">
-        <f t="shared" ref="Q2:Q14" si="2">B2&amp;"Draws"</f>
+      <c r="R2" t="str">
+        <f t="shared" ref="R2:R15" si="1">B2&amp;"Draws"</f>
         <v>bernDraws</v>
       </c>
-      <c r="R2" t="str">
-        <f t="shared" ref="R2:R14" si="3">B2&amp;"Latex"</f>
+      <c r="S2" t="str">
+        <f t="shared" ref="S2:S15" si="2">B2&amp;"Latex"</f>
         <v>bernLatex</v>
       </c>
-      <c r="S2" t="str">
+      <c r="T2" t="str">
         <f>$B2&amp;"ChartDomain"</f>
         <v>bernChartDomain</v>
       </c>
-      <c r="T2" t="str">
+      <c r="U2" t="str">
         <f>$B2&amp;"LikelihoodFun"</f>
         <v>bernLikelihoodFun</v>
       </c>
-      <c r="U2" t="str">
-        <f t="shared" ref="U2:U14" si="4">"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;S2&amp;", likelihoodFun = "&amp;T2&amp;" , paramName = """&amp;F2&amp;""",  xVals = xVals, margNum = margNum)}"</f>
+      <c r="V2" t="str">
+        <f t="shared" ref="V2:V15" si="3">"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;T2&amp;", likelihoodFun = "&amp;U2&amp;" , paramName = """&amp;G2&amp;""",  xVals = xVals, margNum = margNum)}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernChartDomain, likelihoodFun = bernLikelihoodFun , paramName = "Pi",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -797,67 +812,69 @@
       <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="I3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M3" s="1" t="str">
-        <f t="shared" ref="M3:M13" si="5">B3&amp;"Slider"</f>
+      <c r="N3" s="1" t="str">
+        <f t="shared" ref="N3:N14" si="4">B3&amp;"Slider"</f>
         <v>bernLogitSlider</v>
       </c>
-      <c r="N3" t="str">
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O15" si="5">IF(E3=1,"c()", IF(E3=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+        <v>c()</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" ref="P3:P15" si="6">$B3&amp;"ParamTransform"</f>
+        <v>bernLogitParamTransform</v>
+      </c>
+      <c r="Q3" t="str">
         <f t="shared" si="0"/>
-        <v>c()</v>
-      </c>
-      <c r="O3" t="str">
-        <f t="shared" ref="O3:O14" si="6">$B3&amp;"ParamTransform"</f>
-        <v>bernLogitParamTransform</v>
-      </c>
-      <c r="P3" t="str">
+        <v>bernLogitPlotDistr</v>
+      </c>
+      <c r="R3" t="str">
         <f t="shared" si="1"/>
-        <v>bernLogitPlotDistr</v>
-      </c>
-      <c r="Q3" t="str">
+        <v>bernLogitDraws</v>
+      </c>
+      <c r="S3" t="str">
         <f t="shared" si="2"/>
-        <v>bernLogitDraws</v>
-      </c>
-      <c r="R3" t="str">
+        <v>bernLogitLatex</v>
+      </c>
+      <c r="T3" t="str">
+        <f t="shared" ref="T3:T15" si="7">$B3&amp;"ChartDomain"</f>
+        <v>bernLogitChartDomain</v>
+      </c>
+      <c r="U3" t="str">
+        <f t="shared" ref="U3:U15" si="8">$B3&amp;"LikelihoodFun"</f>
+        <v>bernLogitLikelihoodFun</v>
+      </c>
+      <c r="V3" t="str">
         <f t="shared" si="3"/>
-        <v>bernLogitLatex</v>
-      </c>
-      <c r="S3" t="str">
-        <f t="shared" ref="S3:S14" si="7">$B3&amp;"ChartDomain"</f>
-        <v>bernLogitChartDomain</v>
-      </c>
-      <c r="T3" t="str">
-        <f t="shared" ref="T3:T14" si="8">$B3&amp;"LikelihoodFun"</f>
-        <v>bernLogitLikelihoodFun</v>
-      </c>
-      <c r="U3" t="str">
-        <f t="shared" si="4"/>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernLogitChartDomain, likelihoodFun = bernLogitLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A14" si="9">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -872,67 +889,69 @@
       <c r="E4" s="1">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="I4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="1" t="str">
+      <c r="N4" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>bernLogitXSlider</v>
+      </c>
+      <c r="O4" t="str">
         <f t="shared" si="5"/>
-        <v>bernLogitXSlider</v>
-      </c>
-      <c r="N4" t="str">
-        <f t="shared" si="0"/>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
-      <c r="O4" t="str">
+      <c r="P4" t="str">
         <f t="shared" si="6"/>
         <v>bernLogitXParamTransform</v>
       </c>
-      <c r="P4" t="str">
+      <c r="Q4" t="str">
+        <f t="shared" si="0"/>
+        <v>bernLogitXPlotDistr</v>
+      </c>
+      <c r="R4" t="str">
         <f t="shared" si="1"/>
-        <v>bernLogitXPlotDistr</v>
-      </c>
-      <c r="Q4" t="str">
+        <v>bernLogitXDraws</v>
+      </c>
+      <c r="S4" t="str">
         <f t="shared" si="2"/>
-        <v>bernLogitXDraws</v>
-      </c>
-      <c r="R4" t="str">
-        <f t="shared" si="3"/>
         <v>bernLogitXLatex</v>
       </c>
-      <c r="S4" t="str">
+      <c r="T4" t="str">
         <f t="shared" si="7"/>
         <v>bernLogitXChartDomain</v>
       </c>
-      <c r="T4" t="str">
+      <c r="U4" t="str">
         <f t="shared" si="8"/>
         <v>bernLogitXLikelihoodFun</v>
       </c>
-      <c r="U4" t="str">
-        <f t="shared" si="4"/>
+      <c r="V4" t="str">
+        <f t="shared" si="3"/>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernLogitXChartDomain, likelihoodFun = bernLogitXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -947,67 +966,69 @@
       <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M5" s="1" t="str">
+      <c r="N5" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>styNormSlider</v>
+      </c>
+      <c r="O5" t="str">
         <f t="shared" si="5"/>
-        <v>styNormSlider</v>
-      </c>
-      <c r="N5" t="str">
-        <f t="shared" si="0"/>
         <v>c()</v>
       </c>
-      <c r="O5" t="str">
+      <c r="P5" t="str">
         <f t="shared" si="6"/>
         <v>styNormParamTransform</v>
       </c>
-      <c r="P5" t="str">
+      <c r="Q5" t="str">
+        <f t="shared" si="0"/>
+        <v>styNormPlotDistr</v>
+      </c>
+      <c r="R5" t="str">
         <f t="shared" si="1"/>
-        <v>styNormPlotDistr</v>
-      </c>
-      <c r="Q5" t="str">
+        <v>styNormDraws</v>
+      </c>
+      <c r="S5" t="str">
         <f t="shared" si="2"/>
-        <v>styNormDraws</v>
-      </c>
-      <c r="R5" t="str">
-        <f t="shared" si="3"/>
         <v>styNormLatex</v>
       </c>
-      <c r="S5" t="str">
+      <c r="T5" t="str">
         <f t="shared" si="7"/>
         <v>styNormChartDomain</v>
       </c>
-      <c r="T5" t="str">
+      <c r="U5" t="str">
         <f t="shared" si="8"/>
         <v>styNormLikelihoodFun</v>
       </c>
-      <c r="U5" t="str">
-        <f t="shared" si="4"/>
+      <c r="V5" t="str">
+        <f t="shared" si="3"/>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = styNormChartDomain, likelihoodFun = styNormLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1022,661 +1043,757 @@
       <c r="E6" s="1">
         <v>3</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M6" s="1" t="str">
+      <c r="N6" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>styNormXSlider</v>
+      </c>
+      <c r="O6" t="str">
         <f t="shared" si="5"/>
-        <v>styNormXSlider</v>
-      </c>
-      <c r="N6" t="str">
-        <f t="shared" si="0"/>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
-      <c r="O6" t="str">
+      <c r="P6" t="str">
         <f t="shared" si="6"/>
         <v>styNormXParamTransform</v>
       </c>
-      <c r="P6" t="str">
+      <c r="Q6" t="str">
+        <f t="shared" si="0"/>
+        <v>styNormXPlotDistr</v>
+      </c>
+      <c r="R6" t="str">
         <f t="shared" si="1"/>
-        <v>styNormXPlotDistr</v>
-      </c>
-      <c r="Q6" t="str">
+        <v>styNormXDraws</v>
+      </c>
+      <c r="S6" t="str">
         <f t="shared" si="2"/>
-        <v>styNormXDraws</v>
-      </c>
-      <c r="R6" t="str">
-        <f t="shared" si="3"/>
         <v>styNormXLatex</v>
       </c>
-      <c r="S6" t="str">
+      <c r="T6" t="str">
         <f t="shared" si="7"/>
         <v>styNormXChartDomain</v>
       </c>
-      <c r="T6" t="str">
+      <c r="U6" t="str">
         <f t="shared" si="8"/>
         <v>styNormXLikelihoodFun</v>
       </c>
-      <c r="U6" t="str">
+      <c r="V6" t="str">
+        <f t="shared" si="3"/>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = styNormXChartDomain, likelihoodFun = styNormXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = styNormXChartDomain, likelihoodFun = styNormXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
+        <v>fullNormXSlider</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="5"/>
+        <v>c("Beta0", "Beta1", "Beta2","Sigma")</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="6"/>
+        <v>fullNormXParamTransform</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="0"/>
+        <v>fullNormXPlotDistr</v>
+      </c>
+      <c r="R7" t="str">
+        <f t="shared" si="1"/>
+        <v>fullNormXDraws</v>
+      </c>
+      <c r="S7" t="str">
+        <f t="shared" si="2"/>
+        <v>fullNormXLatex</v>
+      </c>
+      <c r="T7" t="str">
+        <f t="shared" si="7"/>
+        <v>fullNormXChartDomain</v>
+      </c>
+      <c r="U7" t="str">
+        <f t="shared" si="8"/>
+        <v>fullNormXLikelihoodFun</v>
+      </c>
+      <c r="V7" t="str">
+        <f t="shared" si="3"/>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = fullNormXChartDomain, likelihoodFun = fullNormXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="9"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="I8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M7" s="1" t="str">
+      <c r="N8" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>logNormSlider</v>
+      </c>
+      <c r="O8" t="str">
         <f t="shared" si="5"/>
-        <v>logNormSlider</v>
-      </c>
-      <c r="N7" t="str">
-        <f t="shared" si="0"/>
         <v>c()</v>
       </c>
-      <c r="O7" t="str">
+      <c r="P8" t="str">
         <f t="shared" si="6"/>
         <v>logNormParamTransform</v>
       </c>
-      <c r="P7" t="str">
+      <c r="Q8" t="str">
+        <f t="shared" si="0"/>
+        <v>logNormPlotDistr</v>
+      </c>
+      <c r="R8" t="str">
         <f t="shared" si="1"/>
-        <v>logNormPlotDistr</v>
-      </c>
-      <c r="Q7" t="str">
+        <v>logNormDraws</v>
+      </c>
+      <c r="S8" t="str">
         <f t="shared" si="2"/>
-        <v>logNormDraws</v>
-      </c>
-      <c r="R7" t="str">
-        <f t="shared" si="3"/>
         <v>logNormLatex</v>
       </c>
-      <c r="S7" t="str">
+      <c r="T8" t="str">
         <f t="shared" si="7"/>
         <v>logNormChartDomain</v>
       </c>
-      <c r="T7" t="str">
+      <c r="U8" t="str">
         <f t="shared" si="8"/>
         <v>logNormLikelihoodFun</v>
       </c>
-      <c r="U7" t="str">
+      <c r="V8" t="str">
+        <f t="shared" si="3"/>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = logNormChartDomain, likelihoodFun = logNormLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N9" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = logNormChartDomain, likelihoodFun = logNormLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="9"/>
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1">
-        <v>3</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M8" s="1" t="str">
+        <v>logNormXSlider</v>
+      </c>
+      <c r="O9" t="str">
         <f t="shared" si="5"/>
-        <v>logNormXSlider</v>
-      </c>
-      <c r="N8" t="str">
-        <f t="shared" si="0"/>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
-      <c r="O8" t="str">
+      <c r="P9" t="str">
         <f t="shared" si="6"/>
         <v>logNormXParamTransform</v>
       </c>
-      <c r="P8" t="str">
+      <c r="Q9" t="str">
+        <f t="shared" si="0"/>
+        <v>logNormXPlotDistr</v>
+      </c>
+      <c r="R9" t="str">
         <f t="shared" si="1"/>
-        <v>logNormXPlotDistr</v>
-      </c>
-      <c r="Q8" t="str">
+        <v>logNormXDraws</v>
+      </c>
+      <c r="S9" t="str">
         <f t="shared" si="2"/>
-        <v>logNormXDraws</v>
-      </c>
-      <c r="R8" t="str">
-        <f t="shared" si="3"/>
         <v>logNormXLatex</v>
       </c>
-      <c r="S8" t="str">
+      <c r="T9" t="str">
         <f t="shared" si="7"/>
         <v>logNormXChartDomain</v>
       </c>
-      <c r="T8" t="str">
+      <c r="U9" t="str">
         <f t="shared" si="8"/>
         <v>logNormXLikelihoodFun</v>
       </c>
-      <c r="U8" t="str">
+      <c r="V9" t="str">
+        <f t="shared" si="3"/>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = logNormXChartDomain, likelihoodFun = logNormXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N10" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = logNormXChartDomain, likelihoodFun = logNormXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="9"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M9" s="1" t="str">
+        <v>poisSlider</v>
+      </c>
+      <c r="O10" t="str">
         <f t="shared" si="5"/>
-        <v>poisSlider</v>
-      </c>
-      <c r="N9" t="str">
-        <f t="shared" si="0"/>
         <v>c()</v>
       </c>
-      <c r="O9" t="str">
+      <c r="P10" t="str">
         <f t="shared" si="6"/>
         <v>poisParamTransform</v>
       </c>
-      <c r="P9" t="str">
+      <c r="Q10" t="str">
+        <f t="shared" si="0"/>
+        <v>poisPlotDistr</v>
+      </c>
+      <c r="R10" t="str">
         <f t="shared" si="1"/>
-        <v>poisPlotDistr</v>
-      </c>
-      <c r="Q9" t="str">
+        <v>poisDraws</v>
+      </c>
+      <c r="S10" t="str">
         <f t="shared" si="2"/>
-        <v>poisDraws</v>
-      </c>
-      <c r="R9" t="str">
-        <f t="shared" si="3"/>
         <v>poisLatex</v>
       </c>
-      <c r="S9" t="str">
+      <c r="T10" t="str">
         <f t="shared" si="7"/>
         <v>poisChartDomain</v>
       </c>
-      <c r="T9" t="str">
+      <c r="U10" t="str">
         <f t="shared" si="8"/>
         <v>poisLikelihoodFun</v>
       </c>
-      <c r="U9" t="str">
+      <c r="V10" t="str">
+        <f t="shared" si="3"/>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisChartDomain, likelihoodFun = poisLikelihoodFun , paramName = "Lambda",  xVals = xVals, margNum = margNum)}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N11" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisChartDomain, likelihoodFun = poisLikelihoodFun , paramName = "Lambda",  xVals = xVals, margNum = margNum)}</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="9"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M10" s="1" t="str">
+        <v>poisExpSlider</v>
+      </c>
+      <c r="O11" t="str">
         <f t="shared" si="5"/>
-        <v>poisExpSlider</v>
-      </c>
-      <c r="N10" t="str">
-        <f t="shared" si="0"/>
         <v>c()</v>
       </c>
-      <c r="O10" t="str">
+      <c r="P11" t="str">
         <f t="shared" si="6"/>
         <v>poisExpParamTransform</v>
       </c>
-      <c r="P10" t="str">
+      <c r="Q11" t="str">
+        <f t="shared" si="0"/>
+        <v>poisExpPlotDistr</v>
+      </c>
+      <c r="R11" t="str">
         <f t="shared" si="1"/>
-        <v>poisExpPlotDistr</v>
-      </c>
-      <c r="Q10" t="str">
+        <v>poisExpDraws</v>
+      </c>
+      <c r="S11" t="str">
         <f t="shared" si="2"/>
-        <v>poisExpDraws</v>
-      </c>
-      <c r="R10" t="str">
-        <f t="shared" si="3"/>
         <v>poisExpLatex</v>
       </c>
-      <c r="S10" t="str">
+      <c r="T11" t="str">
         <f t="shared" si="7"/>
         <v>poisExpChartDomain</v>
       </c>
-      <c r="T10" t="str">
+      <c r="U11" t="str">
         <f t="shared" si="8"/>
         <v>poisExpLikelihoodFun</v>
       </c>
-      <c r="U10" t="str">
-        <f t="shared" si="4"/>
+      <c r="V11" t="str">
+        <f t="shared" si="3"/>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisExpChartDomain, likelihoodFun = poisExpLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="9"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="1">
         <v>3</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="I12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="1" t="str">
-        <f t="shared" ref="M11" si="10">B11&amp;"Slider"</f>
+      <c r="N12" s="1" t="str">
+        <f t="shared" ref="N12" si="9">B12&amp;"Slider"</f>
         <v>poisExpXSlider</v>
       </c>
-      <c r="N11" t="str">
-        <f t="shared" si="0"/>
+      <c r="O12" t="str">
+        <f t="shared" si="5"/>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
-      <c r="O11" t="str">
+      <c r="P12" t="str">
         <f t="shared" si="6"/>
         <v>poisExpXParamTransform</v>
       </c>
-      <c r="P11" t="str">
+      <c r="Q12" t="str">
+        <f t="shared" si="0"/>
+        <v>poisExpXPlotDistr</v>
+      </c>
+      <c r="R12" t="str">
         <f t="shared" si="1"/>
-        <v>poisExpXPlotDistr</v>
-      </c>
-      <c r="Q11" t="str">
+        <v>poisExpXDraws</v>
+      </c>
+      <c r="S12" t="str">
         <f t="shared" si="2"/>
-        <v>poisExpXDraws</v>
-      </c>
-      <c r="R11" t="str">
-        <f t="shared" si="3"/>
         <v>poisExpXLatex</v>
       </c>
-      <c r="S11" t="str">
+      <c r="T12" t="str">
         <f t="shared" si="7"/>
         <v>poisExpXChartDomain</v>
       </c>
-      <c r="T11" t="str">
+      <c r="U12" t="str">
         <f t="shared" si="8"/>
         <v>poisExpXLikelihoodFun</v>
       </c>
-      <c r="U11" t="str">
+      <c r="V12" t="str">
+        <f t="shared" si="3"/>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisExpXChartDomain, likelihoodFun = poisExpXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N13" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisExpXChartDomain, likelihoodFun = poisExpXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="9"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M12" s="1" t="str">
+        <v>expSlider</v>
+      </c>
+      <c r="O13" t="str">
         <f t="shared" si="5"/>
-        <v>expSlider</v>
-      </c>
-      <c r="N12" t="str">
-        <f t="shared" si="0"/>
         <v>c()</v>
       </c>
-      <c r="O12" t="str">
+      <c r="P13" t="str">
         <f t="shared" si="6"/>
         <v>expParamTransform</v>
       </c>
-      <c r="P12" t="str">
+      <c r="Q13" t="str">
+        <f t="shared" si="0"/>
+        <v>expPlotDistr</v>
+      </c>
+      <c r="R13" t="str">
         <f t="shared" si="1"/>
-        <v>expPlotDistr</v>
-      </c>
-      <c r="Q12" t="str">
+        <v>expDraws</v>
+      </c>
+      <c r="S13" t="str">
         <f t="shared" si="2"/>
-        <v>expDraws</v>
-      </c>
-      <c r="R12" t="str">
-        <f t="shared" si="3"/>
         <v>expLatex</v>
       </c>
-      <c r="S12" t="str">
+      <c r="T13" t="str">
         <f t="shared" si="7"/>
         <v>expChartDomain</v>
       </c>
-      <c r="T12" t="str">
+      <c r="U13" t="str">
         <f t="shared" si="8"/>
         <v>expLikelihoodFun</v>
       </c>
-      <c r="U12" t="str">
+      <c r="V13" t="str">
+        <f t="shared" si="3"/>
+        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expChartDomain, likelihoodFun = expLikelihoodFun , paramName = "Lambda",  xVals = xVals, margNum = margNum)}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N14" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expChartDomain, likelihoodFun = expLikelihoodFun , paramName = "Lambda",  xVals = xVals, margNum = margNum)}</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="9"/>
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M13" s="1" t="str">
+        <v>expExpSlider</v>
+      </c>
+      <c r="O14" t="str">
         <f t="shared" si="5"/>
-        <v>expExpSlider</v>
-      </c>
-      <c r="N13" t="str">
-        <f t="shared" si="0"/>
         <v>c()</v>
       </c>
-      <c r="O13" t="str">
+      <c r="P14" t="str">
         <f t="shared" si="6"/>
         <v>expExpParamTransform</v>
       </c>
-      <c r="P13" t="str">
+      <c r="Q14" t="str">
+        <f t="shared" si="0"/>
+        <v>expExpPlotDistr</v>
+      </c>
+      <c r="R14" t="str">
         <f t="shared" si="1"/>
-        <v>expExpPlotDistr</v>
-      </c>
-      <c r="Q13" t="str">
+        <v>expExpDraws</v>
+      </c>
+      <c r="S14" t="str">
         <f t="shared" si="2"/>
-        <v>expExpDraws</v>
-      </c>
-      <c r="R13" t="str">
-        <f t="shared" si="3"/>
         <v>expExpLatex</v>
       </c>
-      <c r="S13" t="str">
+      <c r="T14" t="str">
         <f t="shared" si="7"/>
         <v>expExpChartDomain</v>
       </c>
-      <c r="T13" t="str">
+      <c r="U14" t="str">
         <f t="shared" si="8"/>
         <v>expExpLikelihoodFun</v>
       </c>
-      <c r="U13" t="str">
-        <f t="shared" si="4"/>
+      <c r="V14" t="str">
+        <f t="shared" si="3"/>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expExpChartDomain, likelihoodFun = expExpLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f t="shared" si="9"/>
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E15" s="1">
         <v>3</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F15" s="1">
+        <v>3</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J14" s="1" t="s">
+      <c r="I15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M14" s="1" t="str">
-        <f t="shared" ref="M14" si="11">B14&amp;"Slider"</f>
+      <c r="N15" s="1" t="str">
+        <f t="shared" ref="N15" si="10">B15&amp;"Slider"</f>
         <v>expExpXSlider</v>
       </c>
-      <c r="N14" t="str">
-        <f t="shared" si="0"/>
+      <c r="O15" t="str">
+        <f t="shared" si="5"/>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
-      <c r="O14" t="str">
+      <c r="P15" t="str">
         <f t="shared" si="6"/>
         <v>expExpXParamTransform</v>
       </c>
-      <c r="P14" t="str">
+      <c r="Q15" t="str">
+        <f t="shared" si="0"/>
+        <v>expExpXPlotDistr</v>
+      </c>
+      <c r="R15" t="str">
         <f t="shared" si="1"/>
-        <v>expExpXPlotDistr</v>
-      </c>
-      <c r="Q14" t="str">
+        <v>expExpXDraws</v>
+      </c>
+      <c r="S15" t="str">
         <f t="shared" si="2"/>
-        <v>expExpXDraws</v>
-      </c>
-      <c r="R14" t="str">
-        <f t="shared" si="3"/>
         <v>expExpXLatex</v>
       </c>
-      <c r="S14" t="str">
+      <c r="T15" t="str">
         <f t="shared" si="7"/>
         <v>expExpXChartDomain</v>
       </c>
-      <c r="T14" t="str">
+      <c r="U15" t="str">
         <f t="shared" si="8"/>
         <v>expExpXLikelihoodFun</v>
       </c>
-      <c r="U14" t="str">
-        <f t="shared" si="4"/>
+      <c r="V15" t="str">
+        <f t="shared" si="3"/>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expExpXChartDomain, likelihoodFun = expExpXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum)}</v>
       </c>
     </row>

</xml_diff>

<commit_message>
assorted bugfixes and tweaks
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F432AE25-4BC3-489C-B5DF-F9F95A107041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28F97C5-2433-44E1-86F7-D090AB6E9C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -663,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
   <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
refactor and simplification of slider creation
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19707163-8199-4948-AFFB-939E26B503FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB57B2A4-D612-48C0-A489-7468D490E158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="103">
   <si>
     <t>Bernoulli-Pi</t>
   </si>
@@ -292,6 +292,57 @@
   </si>
   <si>
     <t>list("Poisson", "Poisson-Exp", "Poisson-Exp-X", "Stylized-Normal", "Stylized-Normal-X", "Normal-X")</t>
+  </si>
+  <si>
+    <t>c(.3)</t>
+  </si>
+  <si>
+    <t>sliderMin</t>
+  </si>
+  <si>
+    <t>sliderMax</t>
+  </si>
+  <si>
+    <t>sliderStarts</t>
+  </si>
+  <si>
+    <t>sliderStep</t>
+  </si>
+  <si>
+    <t>paramHTML</t>
+  </si>
+  <si>
+    <t>multi slider?</t>
+  </si>
+  <si>
+    <t>sliderFun</t>
+  </si>
+  <si>
+    <t>c(1.3)</t>
+  </si>
+  <si>
+    <t>c(1,-1,.25)</t>
+  </si>
+  <si>
+    <t>c(.25)</t>
+  </si>
+  <si>
+    <t>c(.2, .1, -.2)</t>
+  </si>
+  <si>
+    <t>c(1)</t>
+  </si>
+  <si>
+    <t>c(1,-1,.5)</t>
+  </si>
+  <si>
+    <t>c(2)</t>
+  </si>
+  <si>
+    <t>c(-.3,1,.3)</t>
+  </si>
+  <si>
+    <t>c(1,-1,.25,1)</t>
   </si>
 </sst>
 </file>
@@ -658,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
-  <dimension ref="A1:W15"/>
+  <dimension ref="A1:AD15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,17 +726,23 @@
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" customWidth="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16" customWidth="1"/>
-    <col min="16" max="16" width="26" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26" customWidth="1"/>
-    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="16" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" customWidth="1"/>
+    <col min="16" max="16" width="4.28515625" customWidth="1"/>
+    <col min="17" max="17" width="5.5703125" customWidth="1"/>
+    <col min="18" max="18" width="6" customWidth="1"/>
+    <col min="19" max="20" width="4.28515625" customWidth="1"/>
+    <col min="21" max="21" width="16" customWidth="1"/>
+    <col min="22" max="22" width="16" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26" customWidth="1"/>
+    <col min="25" max="25" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -726,37 +783,58 @@
         <v>55</v>
       </c>
       <c r="N1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>89</v>
+      </c>
+      <c r="R1" t="s">
+        <v>90</v>
+      </c>
+      <c r="S1" t="s">
+        <v>91</v>
+      </c>
+      <c r="T1" t="s">
+        <v>92</v>
+      </c>
+      <c r="U1" t="s">
+        <v>93</v>
+      </c>
+      <c r="V1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
-        <v>72</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="W1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="X1" t="s">
         <v>48</v>
       </c>
-      <c r="R1" t="s">
+      <c r="Y1" t="s">
         <v>28</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Z1" t="s">
         <v>31</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AA1" t="s">
         <v>32</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AB1" t="s">
         <v>35</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AC1" t="s">
         <v>36</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AD1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -796,47 +874,71 @@
       <c r="M2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="N2" s="1" t="str">
+      <c r="N2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="R2">
+        <v>0.01</v>
+      </c>
+      <c r="S2" t="str">
+        <f>"""&amp;"&amp;RIGHT(K2,LEN(K2)-1)&amp;";"""</f>
+        <v>"&amp;pi;"</v>
+      </c>
+      <c r="T2" t="str">
+        <f>IF(F2=1,"""none""",IF(E2=F2,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
+      </c>
+      <c r="U2" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;O2&amp;", maxVal = "&amp;P2&amp;", startVals = "&amp;Q2&amp;", stepVal = "&amp;R2&amp;", paramHTML = "&amp;S2&amp;", multi = "&amp;T2&amp;")"</f>
+        <v>manyParamSliderMaker(minVal =0, maxVal = 1, startVals = c(.3), stepVal = 0.01, paramHTML = "&amp;pi;", multi = "none")</v>
+      </c>
+      <c r="V2" t="str">
         <f>B2&amp;"Slider"</f>
         <v>bernSlider</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P2" t="str">
+      <c r="W2" t="str">
         <f>IF(E2=1,"c()", IF(E2=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
-      <c r="Q2" t="str">
+      <c r="X2" t="str">
         <f>$B2&amp;"ParamTransform"</f>
         <v>bernParamTransform</v>
       </c>
-      <c r="R2" t="str">
-        <f t="shared" ref="R2:R15" si="0">B2&amp;"PlotDistr"</f>
+      <c r="Y2" t="str">
+        <f>B2&amp;"PlotDistr"</f>
         <v>bernPlotDistr</v>
       </c>
-      <c r="S2" t="str">
-        <f t="shared" ref="S2:S15" si="1">B2&amp;"Draws"</f>
+      <c r="Z2" t="str">
+        <f>B2&amp;"Draws"</f>
         <v>bernDraws</v>
       </c>
-      <c r="T2" t="str">
-        <f t="shared" ref="T2:T15" si="2">B2&amp;"Latex"</f>
+      <c r="AA2" t="str">
+        <f>B2&amp;"Latex"</f>
         <v>bernLatex</v>
       </c>
-      <c r="U2" t="str">
+      <c r="AB2" t="str">
         <f>$B2&amp;"ChartDomain"</f>
         <v>bernChartDomain</v>
       </c>
-      <c r="V2" t="str">
+      <c r="AC2" t="str">
         <f>$B2&amp;"LikelihoodFun"</f>
         <v>bernLikelihoodFun</v>
       </c>
-      <c r="W2" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;U2&amp;", likelihoodFun = "&amp;V2&amp;" , paramName = """&amp;G2&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;O2&amp;""")}"</f>
+      <c r="AD2" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB2&amp;", likelihoodFun = "&amp;AC2&amp;" , paramName = """&amp;G2&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N2&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernChartDomain, likelihoodFun = bernLikelihoodFun , paramName = "Pi",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -876,47 +978,71 @@
       <c r="M3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="N3" s="1" t="str">
-        <f t="shared" ref="N3:N14" si="3">B3&amp;"Slider"</f>
+      <c r="N3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O3" s="1">
+        <v>-2</v>
+      </c>
+      <c r="P3" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="R3">
+        <v>0.01</v>
+      </c>
+      <c r="S3" t="str">
+        <f t="shared" ref="S3:S15" si="0">"""&amp;"&amp;RIGHT(K3,LEN(K3)-1)&amp;";"""</f>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="T3" t="str">
+        <f t="shared" ref="T3:T15" si="1">IF(F3=1,"""none""",IF(E3=F3,"""betas""","""fullNorm"""))</f>
+        <v>"none"</v>
+      </c>
+      <c r="U3" t="str">
+        <f t="shared" ref="U3:U15" si="2">"manyParamSliderMaker(minVal ="&amp;O3&amp;", maxVal = "&amp;P3&amp;", startVals = "&amp;Q3&amp;", stepVal = "&amp;R3&amp;", paramHTML = "&amp;S3&amp;", multi = "&amp;T3&amp;")"</f>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none")</v>
+      </c>
+      <c r="V3" t="str">
+        <f>B3&amp;"Slider"</f>
         <v>bernLogitSlider</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P3" t="str">
-        <f t="shared" ref="P3:P15" si="4">IF(E3=1,"c()", IF(E3=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+      <c r="W3" t="str">
+        <f>IF(E3=1,"c()", IF(E3=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
-      <c r="Q3" t="str">
-        <f t="shared" ref="Q3:Q15" si="5">$B3&amp;"ParamTransform"</f>
+      <c r="X3" t="str">
+        <f t="shared" ref="X3:X15" si="3">$B3&amp;"ParamTransform"</f>
         <v>bernLogitParamTransform</v>
       </c>
-      <c r="R3" t="str">
-        <f t="shared" si="0"/>
+      <c r="Y3" t="str">
+        <f>B3&amp;"PlotDistr"</f>
         <v>bernLogitPlotDistr</v>
       </c>
-      <c r="S3" t="str">
-        <f t="shared" si="1"/>
+      <c r="Z3" t="str">
+        <f>B3&amp;"Draws"</f>
         <v>bernLogitDraws</v>
       </c>
-      <c r="T3" t="str">
-        <f t="shared" si="2"/>
+      <c r="AA3" t="str">
+        <f>B3&amp;"Latex"</f>
         <v>bernLogitLatex</v>
       </c>
-      <c r="U3" t="str">
-        <f t="shared" ref="U3:U15" si="6">$B3&amp;"ChartDomain"</f>
+      <c r="AB3" t="str">
+        <f t="shared" ref="AB3:AB15" si="4">$B3&amp;"ChartDomain"</f>
         <v>bernLogitChartDomain</v>
       </c>
-      <c r="V3" t="str">
-        <f t="shared" ref="V3:V15" si="7">$B3&amp;"LikelihoodFun"</f>
+      <c r="AC3" t="str">
+        <f t="shared" ref="AC3:AC15" si="5">$B3&amp;"LikelihoodFun"</f>
         <v>bernLogitLikelihoodFun</v>
       </c>
-      <c r="W3" t="str">
-        <f t="shared" ref="W3:W15" si="8">"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;U3&amp;", likelihoodFun = "&amp;V3&amp;" , paramName = """&amp;G3&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;O3&amp;""")}"</f>
+      <c r="AD3" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB3&amp;", likelihoodFun = "&amp;AC3&amp;" , paramName = """&amp;G3&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N3&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernLogitChartDomain, likelihoodFun = bernLogitLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -956,47 +1082,71 @@
       <c r="M4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="N4" s="1" t="str">
+      <c r="N4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O4" s="1">
+        <v>-2</v>
+      </c>
+      <c r="P4" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="R4">
+        <v>0.01</v>
+      </c>
+      <c r="S4" t="str">
+        <f t="shared" si="0"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="T4" t="str">
+        <f t="shared" si="1"/>
+        <v>"betas"</v>
+      </c>
+      <c r="U4" t="str">
+        <f t="shared" si="2"/>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas")</v>
+      </c>
+      <c r="V4" t="str">
+        <f>B4&amp;"Slider"</f>
+        <v>bernLogitXSlider</v>
+      </c>
+      <c r="W4" t="str">
+        <f>IF(E4=1,"c()", IF(E4=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+        <v>c("Beta0", "Beta1", "Beta2")</v>
+      </c>
+      <c r="X4" t="str">
         <f t="shared" si="3"/>
-        <v>bernLogitXSlider</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P4" t="str">
+        <v>bernLogitXParamTransform</v>
+      </c>
+      <c r="Y4" t="str">
+        <f>B4&amp;"PlotDistr"</f>
+        <v>bernLogitXPlotDistr</v>
+      </c>
+      <c r="Z4" t="str">
+        <f>B4&amp;"Draws"</f>
+        <v>bernLogitXDraws</v>
+      </c>
+      <c r="AA4" t="str">
+        <f>B4&amp;"Latex"</f>
+        <v>bernLogitXLatex</v>
+      </c>
+      <c r="AB4" t="str">
         <f t="shared" si="4"/>
-        <v>c("Beta0", "Beta1", "Beta2")</v>
-      </c>
-      <c r="Q4" t="str">
+        <v>bernLogitXChartDomain</v>
+      </c>
+      <c r="AC4" t="str">
         <f t="shared" si="5"/>
-        <v>bernLogitXParamTransform</v>
-      </c>
-      <c r="R4" t="str">
-        <f t="shared" si="0"/>
-        <v>bernLogitXPlotDistr</v>
-      </c>
-      <c r="S4" t="str">
-        <f t="shared" si="1"/>
-        <v>bernLogitXDraws</v>
-      </c>
-      <c r="T4" t="str">
-        <f t="shared" si="2"/>
-        <v>bernLogitXLatex</v>
-      </c>
-      <c r="U4" t="str">
-        <f t="shared" si="6"/>
-        <v>bernLogitXChartDomain</v>
-      </c>
-      <c r="V4" t="str">
-        <f t="shared" si="7"/>
         <v>bernLogitXLikelihoodFun</v>
       </c>
-      <c r="W4" t="str">
-        <f t="shared" si="8"/>
+      <c r="AD4" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB4&amp;", likelihoodFun = "&amp;AC4&amp;" , paramName = """&amp;G4&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N4&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernLogitXChartDomain, likelihoodFun = bernLogitXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1036,47 +1186,71 @@
       <c r="M5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="1" t="str">
+      <c r="N5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O5" s="1">
+        <v>-2</v>
+      </c>
+      <c r="P5" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R5">
+        <v>0.01</v>
+      </c>
+      <c r="S5" t="str">
+        <f t="shared" si="0"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="T5" t="str">
+        <f t="shared" si="1"/>
+        <v>"none"</v>
+      </c>
+      <c r="U5" t="str">
+        <f t="shared" si="2"/>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none")</v>
+      </c>
+      <c r="V5" t="str">
+        <f>B5&amp;"Slider"</f>
+        <v>styNormSlider</v>
+      </c>
+      <c r="W5" t="str">
+        <f>IF(E5=1,"c()", IF(E5=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+        <v>c()</v>
+      </c>
+      <c r="X5" t="str">
         <f t="shared" si="3"/>
-        <v>styNormSlider</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P5" t="str">
+        <v>styNormParamTransform</v>
+      </c>
+      <c r="Y5" t="str">
+        <f>B5&amp;"PlotDistr"</f>
+        <v>styNormPlotDistr</v>
+      </c>
+      <c r="Z5" t="str">
+        <f>B5&amp;"Draws"</f>
+        <v>styNormDraws</v>
+      </c>
+      <c r="AA5" t="str">
+        <f>B5&amp;"Latex"</f>
+        <v>styNormLatex</v>
+      </c>
+      <c r="AB5" t="str">
         <f t="shared" si="4"/>
-        <v>c()</v>
-      </c>
-      <c r="Q5" t="str">
+        <v>styNormChartDomain</v>
+      </c>
+      <c r="AC5" t="str">
         <f t="shared" si="5"/>
-        <v>styNormParamTransform</v>
-      </c>
-      <c r="R5" t="str">
-        <f t="shared" si="0"/>
-        <v>styNormPlotDistr</v>
-      </c>
-      <c r="S5" t="str">
-        <f t="shared" si="1"/>
-        <v>styNormDraws</v>
-      </c>
-      <c r="T5" t="str">
-        <f t="shared" si="2"/>
-        <v>styNormLatex</v>
-      </c>
-      <c r="U5" t="str">
-        <f t="shared" si="6"/>
-        <v>styNormChartDomain</v>
-      </c>
-      <c r="V5" t="str">
-        <f t="shared" si="7"/>
         <v>styNormLikelihoodFun</v>
       </c>
-      <c r="W5" t="str">
-        <f t="shared" si="8"/>
+      <c r="AD5" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB5&amp;", likelihoodFun = "&amp;AC5&amp;" , paramName = """&amp;G5&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N5&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = styNormChartDomain, likelihoodFun = styNormLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1116,47 +1290,71 @@
       <c r="M6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N6" s="1" t="str">
+      <c r="N6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O6" s="1">
+        <v>-2</v>
+      </c>
+      <c r="P6" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="R6">
+        <v>0.01</v>
+      </c>
+      <c r="S6" t="str">
+        <f t="shared" si="0"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="T6" t="str">
+        <f t="shared" si="1"/>
+        <v>"betas"</v>
+      </c>
+      <c r="U6" t="str">
+        <f t="shared" si="2"/>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas")</v>
+      </c>
+      <c r="V6" t="str">
+        <f>B6&amp;"Slider"</f>
+        <v>styNormXSlider</v>
+      </c>
+      <c r="W6" t="str">
+        <f>IF(E6=1,"c()", IF(E6=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+        <v>c("Beta0", "Beta1", "Beta2")</v>
+      </c>
+      <c r="X6" t="str">
         <f t="shared" si="3"/>
-        <v>styNormXSlider</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P6" t="str">
+        <v>styNormXParamTransform</v>
+      </c>
+      <c r="Y6" t="str">
+        <f>B6&amp;"PlotDistr"</f>
+        <v>styNormXPlotDistr</v>
+      </c>
+      <c r="Z6" t="str">
+        <f>B6&amp;"Draws"</f>
+        <v>styNormXDraws</v>
+      </c>
+      <c r="AA6" t="str">
+        <f>B6&amp;"Latex"</f>
+        <v>styNormXLatex</v>
+      </c>
+      <c r="AB6" t="str">
         <f t="shared" si="4"/>
-        <v>c("Beta0", "Beta1", "Beta2")</v>
-      </c>
-      <c r="Q6" t="str">
+        <v>styNormXChartDomain</v>
+      </c>
+      <c r="AC6" t="str">
         <f t="shared" si="5"/>
-        <v>styNormXParamTransform</v>
-      </c>
-      <c r="R6" t="str">
-        <f t="shared" si="0"/>
-        <v>styNormXPlotDistr</v>
-      </c>
-      <c r="S6" t="str">
-        <f t="shared" si="1"/>
-        <v>styNormXDraws</v>
-      </c>
-      <c r="T6" t="str">
-        <f t="shared" si="2"/>
-        <v>styNormXLatex</v>
-      </c>
-      <c r="U6" t="str">
-        <f t="shared" si="6"/>
-        <v>styNormXChartDomain</v>
-      </c>
-      <c r="V6" t="str">
-        <f t="shared" si="7"/>
         <v>styNormXLikelihoodFun</v>
       </c>
-      <c r="W6" t="str">
-        <f t="shared" si="8"/>
+      <c r="AD6" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB6&amp;", likelihoodFun = "&amp;AC6&amp;" , paramName = """&amp;G6&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N6&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = styNormXChartDomain, likelihoodFun = styNormXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1196,47 +1394,71 @@
       <c r="M7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N7" s="1" t="str">
+      <c r="N7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O7" s="1">
+        <v>-2</v>
+      </c>
+      <c r="P7" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="R7">
+        <v>0.01</v>
+      </c>
+      <c r="S7" t="str">
+        <f t="shared" si="0"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="T7" t="str">
+        <f t="shared" si="1"/>
+        <v>"fullNorm"</v>
+      </c>
+      <c r="U7" t="str">
+        <f t="shared" si="2"/>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25,1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm")</v>
+      </c>
+      <c r="V7" t="str">
+        <f>B7&amp;"Slider"</f>
+        <v>fullNormXSlider</v>
+      </c>
+      <c r="W7" t="str">
+        <f>IF(E7=1,"c()", IF(E7=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+        <v>c("Beta0", "Beta1", "Beta2","Sigma")</v>
+      </c>
+      <c r="X7" t="str">
         <f t="shared" si="3"/>
-        <v>fullNormXSlider</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P7" t="str">
+        <v>fullNormXParamTransform</v>
+      </c>
+      <c r="Y7" t="str">
+        <f>B7&amp;"PlotDistr"</f>
+        <v>fullNormXPlotDistr</v>
+      </c>
+      <c r="Z7" t="str">
+        <f>B7&amp;"Draws"</f>
+        <v>fullNormXDraws</v>
+      </c>
+      <c r="AA7" t="str">
+        <f>B7&amp;"Latex"</f>
+        <v>fullNormXLatex</v>
+      </c>
+      <c r="AB7" t="str">
         <f t="shared" si="4"/>
-        <v>c("Beta0", "Beta1", "Beta2","Sigma")</v>
-      </c>
-      <c r="Q7" t="str">
+        <v>fullNormXChartDomain</v>
+      </c>
+      <c r="AC7" t="str">
         <f t="shared" si="5"/>
-        <v>fullNormXParamTransform</v>
-      </c>
-      <c r="R7" t="str">
-        <f t="shared" si="0"/>
-        <v>fullNormXPlotDistr</v>
-      </c>
-      <c r="S7" t="str">
-        <f t="shared" si="1"/>
-        <v>fullNormXDraws</v>
-      </c>
-      <c r="T7" t="str">
-        <f t="shared" si="2"/>
-        <v>fullNormXLatex</v>
-      </c>
-      <c r="U7" t="str">
-        <f t="shared" si="6"/>
-        <v>fullNormXChartDomain</v>
-      </c>
-      <c r="V7" t="str">
-        <f t="shared" si="7"/>
         <v>fullNormXLikelihoodFun</v>
       </c>
-      <c r="W7" t="str">
-        <f t="shared" si="8"/>
+      <c r="AD7" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB7&amp;", likelihoodFun = "&amp;AC7&amp;" , paramName = """&amp;G7&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N7&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = fullNormXChartDomain, likelihoodFun = fullNormXLikelihoodFun , paramName = "Beta/Sigma",  xVals = xVals, margNum = margNum, optimMethod = "SANN")}</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1276,47 +1498,71 @@
       <c r="M8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N8" s="1" t="str">
+      <c r="N8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O8" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="P8" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R8">
+        <v>0.01</v>
+      </c>
+      <c r="S8" t="str">
+        <f t="shared" si="0"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="T8" t="str">
+        <f t="shared" si="1"/>
+        <v>"none"</v>
+      </c>
+      <c r="U8" t="str">
+        <f t="shared" si="2"/>
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 2, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none")</v>
+      </c>
+      <c r="V8" t="str">
+        <f>B8&amp;"Slider"</f>
+        <v>logNormSlider</v>
+      </c>
+      <c r="W8" t="str">
+        <f>IF(E8=1,"c()", IF(E8=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+        <v>c()</v>
+      </c>
+      <c r="X8" t="str">
         <f t="shared" si="3"/>
-        <v>logNormSlider</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P8" t="str">
+        <v>logNormParamTransform</v>
+      </c>
+      <c r="Y8" t="str">
+        <f>B8&amp;"PlotDistr"</f>
+        <v>logNormPlotDistr</v>
+      </c>
+      <c r="Z8" t="str">
+        <f>B8&amp;"Draws"</f>
+        <v>logNormDraws</v>
+      </c>
+      <c r="AA8" t="str">
+        <f>B8&amp;"Latex"</f>
+        <v>logNormLatex</v>
+      </c>
+      <c r="AB8" t="str">
         <f t="shared" si="4"/>
-        <v>c()</v>
-      </c>
-      <c r="Q8" t="str">
+        <v>logNormChartDomain</v>
+      </c>
+      <c r="AC8" t="str">
         <f t="shared" si="5"/>
-        <v>logNormParamTransform</v>
-      </c>
-      <c r="R8" t="str">
-        <f t="shared" si="0"/>
-        <v>logNormPlotDistr</v>
-      </c>
-      <c r="S8" t="str">
-        <f t="shared" si="1"/>
-        <v>logNormDraws</v>
-      </c>
-      <c r="T8" t="str">
-        <f t="shared" si="2"/>
-        <v>logNormLatex</v>
-      </c>
-      <c r="U8" t="str">
-        <f t="shared" si="6"/>
-        <v>logNormChartDomain</v>
-      </c>
-      <c r="V8" t="str">
-        <f t="shared" si="7"/>
         <v>logNormLikelihoodFun</v>
       </c>
-      <c r="W8" t="str">
-        <f t="shared" si="8"/>
+      <c r="AD8" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB8&amp;", likelihoodFun = "&amp;AC8&amp;" , paramName = """&amp;G8&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N8&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = logNormChartDomain, likelihoodFun = logNormLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1356,47 +1602,71 @@
       <c r="M9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="N9" s="1" t="str">
+      <c r="N9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P9" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R9">
+        <v>0.01</v>
+      </c>
+      <c r="S9" t="str">
+        <f t="shared" si="0"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="T9" t="str">
+        <f t="shared" si="1"/>
+        <v>"betas"</v>
+      </c>
+      <c r="U9" t="str">
+        <f t="shared" si="2"/>
+        <v>manyParamSliderMaker(minVal =-1, maxVal = 2, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas")</v>
+      </c>
+      <c r="V9" t="str">
+        <f>B9&amp;"Slider"</f>
+        <v>logNormXSlider</v>
+      </c>
+      <c r="W9" t="str">
+        <f>IF(E9=1,"c()", IF(E9=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+        <v>c("Beta0", "Beta1", "Beta2")</v>
+      </c>
+      <c r="X9" t="str">
         <f t="shared" si="3"/>
-        <v>logNormXSlider</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P9" t="str">
+        <v>logNormXParamTransform</v>
+      </c>
+      <c r="Y9" t="str">
+        <f>B9&amp;"PlotDistr"</f>
+        <v>logNormXPlotDistr</v>
+      </c>
+      <c r="Z9" t="str">
+        <f>B9&amp;"Draws"</f>
+        <v>logNormXDraws</v>
+      </c>
+      <c r="AA9" t="str">
+        <f>B9&amp;"Latex"</f>
+        <v>logNormXLatex</v>
+      </c>
+      <c r="AB9" t="str">
         <f t="shared" si="4"/>
-        <v>c("Beta0", "Beta1", "Beta2")</v>
-      </c>
-      <c r="Q9" t="str">
+        <v>logNormXChartDomain</v>
+      </c>
+      <c r="AC9" t="str">
         <f t="shared" si="5"/>
-        <v>logNormXParamTransform</v>
-      </c>
-      <c r="R9" t="str">
-        <f t="shared" si="0"/>
-        <v>logNormXPlotDistr</v>
-      </c>
-      <c r="S9" t="str">
-        <f t="shared" si="1"/>
-        <v>logNormXDraws</v>
-      </c>
-      <c r="T9" t="str">
-        <f t="shared" si="2"/>
-        <v>logNormXLatex</v>
-      </c>
-      <c r="U9" t="str">
-        <f t="shared" si="6"/>
-        <v>logNormXChartDomain</v>
-      </c>
-      <c r="V9" t="str">
-        <f t="shared" si="7"/>
         <v>logNormXLikelihoodFun</v>
       </c>
-      <c r="W9" t="str">
-        <f t="shared" si="8"/>
+      <c r="AD9" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB9&amp;", likelihoodFun = "&amp;AC9&amp;" , paramName = """&amp;G9&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N9&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = logNormXChartDomain, likelihoodFun = logNormXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1436,47 +1706,71 @@
       <c r="M10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="N10" s="1" t="str">
+      <c r="N10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O10" s="1">
+        <v>1</v>
+      </c>
+      <c r="P10" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="R10">
+        <v>0.01</v>
+      </c>
+      <c r="S10" t="str">
+        <f t="shared" si="0"/>
+        <v>"&amp;lambda;"</v>
+      </c>
+      <c r="T10" t="str">
+        <f t="shared" si="1"/>
+        <v>"none"</v>
+      </c>
+      <c r="U10" t="str">
+        <f t="shared" si="2"/>
+        <v>manyParamSliderMaker(minVal =1, maxVal = 10, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none")</v>
+      </c>
+      <c r="V10" t="str">
+        <f>B10&amp;"Slider"</f>
+        <v>poisSlider</v>
+      </c>
+      <c r="W10" t="str">
+        <f>IF(E10=1,"c()", IF(E10=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+        <v>c()</v>
+      </c>
+      <c r="X10" t="str">
         <f t="shared" si="3"/>
-        <v>poisSlider</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P10" t="str">
+        <v>poisParamTransform</v>
+      </c>
+      <c r="Y10" t="str">
+        <f>B10&amp;"PlotDistr"</f>
+        <v>poisPlotDistr</v>
+      </c>
+      <c r="Z10" t="str">
+        <f>B10&amp;"Draws"</f>
+        <v>poisDraws</v>
+      </c>
+      <c r="AA10" t="str">
+        <f>B10&amp;"Latex"</f>
+        <v>poisLatex</v>
+      </c>
+      <c r="AB10" t="str">
         <f t="shared" si="4"/>
-        <v>c()</v>
-      </c>
-      <c r="Q10" t="str">
+        <v>poisChartDomain</v>
+      </c>
+      <c r="AC10" t="str">
         <f t="shared" si="5"/>
-        <v>poisParamTransform</v>
-      </c>
-      <c r="R10" t="str">
-        <f t="shared" si="0"/>
-        <v>poisPlotDistr</v>
-      </c>
-      <c r="S10" t="str">
-        <f t="shared" si="1"/>
-        <v>poisDraws</v>
-      </c>
-      <c r="T10" t="str">
-        <f t="shared" si="2"/>
-        <v>poisLatex</v>
-      </c>
-      <c r="U10" t="str">
-        <f t="shared" si="6"/>
-        <v>poisChartDomain</v>
-      </c>
-      <c r="V10" t="str">
-        <f t="shared" si="7"/>
         <v>poisLikelihoodFun</v>
       </c>
-      <c r="W10" t="str">
-        <f t="shared" si="8"/>
+      <c r="AD10" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB10&amp;", likelihoodFun = "&amp;AC10&amp;" , paramName = """&amp;G10&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N10&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisChartDomain, likelihoodFun = poisLikelihoodFun , paramName = "Lambda",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1516,47 +1810,71 @@
       <c r="M11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N11" s="1" t="str">
+      <c r="N11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O11" s="1">
+        <v>-0.25</v>
+      </c>
+      <c r="P11" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R11">
+        <v>0.01</v>
+      </c>
+      <c r="S11" t="str">
+        <f t="shared" si="0"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="T11" t="str">
+        <f t="shared" si="1"/>
+        <v>"none"</v>
+      </c>
+      <c r="U11" t="str">
+        <f t="shared" si="2"/>
+        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none")</v>
+      </c>
+      <c r="V11" t="str">
+        <f>B11&amp;"Slider"</f>
+        <v>poisExpSlider</v>
+      </c>
+      <c r="W11" t="str">
+        <f>IF(E11=1,"c()", IF(E11=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+        <v>c()</v>
+      </c>
+      <c r="X11" t="str">
         <f t="shared" si="3"/>
-        <v>poisExpSlider</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P11" t="str">
+        <v>poisExpParamTransform</v>
+      </c>
+      <c r="Y11" t="str">
+        <f>B11&amp;"PlotDistr"</f>
+        <v>poisExpPlotDistr</v>
+      </c>
+      <c r="Z11" t="str">
+        <f>B11&amp;"Draws"</f>
+        <v>poisExpDraws</v>
+      </c>
+      <c r="AA11" t="str">
+        <f>B11&amp;"Latex"</f>
+        <v>poisExpLatex</v>
+      </c>
+      <c r="AB11" t="str">
         <f t="shared" si="4"/>
-        <v>c()</v>
-      </c>
-      <c r="Q11" t="str">
+        <v>poisExpChartDomain</v>
+      </c>
+      <c r="AC11" t="str">
         <f t="shared" si="5"/>
-        <v>poisExpParamTransform</v>
-      </c>
-      <c r="R11" t="str">
-        <f t="shared" si="0"/>
-        <v>poisExpPlotDistr</v>
-      </c>
-      <c r="S11" t="str">
-        <f t="shared" si="1"/>
-        <v>poisExpDraws</v>
-      </c>
-      <c r="T11" t="str">
-        <f t="shared" si="2"/>
-        <v>poisExpLatex</v>
-      </c>
-      <c r="U11" t="str">
-        <f t="shared" si="6"/>
-        <v>poisExpChartDomain</v>
-      </c>
-      <c r="V11" t="str">
-        <f t="shared" si="7"/>
         <v>poisExpLikelihoodFun</v>
       </c>
-      <c r="W11" t="str">
-        <f t="shared" si="8"/>
+      <c r="AD11" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB11&amp;", likelihoodFun = "&amp;AC11&amp;" , paramName = """&amp;G11&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N11&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisExpChartDomain, likelihoodFun = poisExpLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1596,47 +1914,71 @@
       <c r="M12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N12" s="1" t="str">
-        <f t="shared" ref="N12" si="9">B12&amp;"Slider"</f>
+      <c r="N12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P12" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="R12">
+        <v>0.01</v>
+      </c>
+      <c r="S12" t="str">
+        <f t="shared" si="0"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="T12" t="str">
+        <f t="shared" si="1"/>
+        <v>"betas"</v>
+      </c>
+      <c r="U12" t="str">
+        <f t="shared" si="2"/>
+        <v>manyParamSliderMaker(minVal =-1, maxVal = 1, startVals = c(-.3,1,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas")</v>
+      </c>
+      <c r="V12" t="str">
+        <f>B12&amp;"Slider"</f>
         <v>poisExpXSlider</v>
       </c>
-      <c r="O12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P12" t="str">
+      <c r="W12" t="str">
+        <f>IF(E12=1,"c()", IF(E12=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+        <v>c("Beta0", "Beta1", "Beta2")</v>
+      </c>
+      <c r="X12" t="str">
+        <f t="shared" si="3"/>
+        <v>poisExpXParamTransform</v>
+      </c>
+      <c r="Y12" t="str">
+        <f>B12&amp;"PlotDistr"</f>
+        <v>poisExpXPlotDistr</v>
+      </c>
+      <c r="Z12" t="str">
+        <f>B12&amp;"Draws"</f>
+        <v>poisExpXDraws</v>
+      </c>
+      <c r="AA12" t="str">
+        <f>B12&amp;"Latex"</f>
+        <v>poisExpXLatex</v>
+      </c>
+      <c r="AB12" t="str">
         <f t="shared" si="4"/>
-        <v>c("Beta0", "Beta1", "Beta2")</v>
-      </c>
-      <c r="Q12" t="str">
+        <v>poisExpXChartDomain</v>
+      </c>
+      <c r="AC12" t="str">
         <f t="shared" si="5"/>
-        <v>poisExpXParamTransform</v>
-      </c>
-      <c r="R12" t="str">
-        <f t="shared" si="0"/>
-        <v>poisExpXPlotDistr</v>
-      </c>
-      <c r="S12" t="str">
-        <f t="shared" si="1"/>
-        <v>poisExpXDraws</v>
-      </c>
-      <c r="T12" t="str">
-        <f t="shared" si="2"/>
-        <v>poisExpXLatex</v>
-      </c>
-      <c r="U12" t="str">
-        <f t="shared" si="6"/>
-        <v>poisExpXChartDomain</v>
-      </c>
-      <c r="V12" t="str">
-        <f t="shared" si="7"/>
         <v>poisExpXLikelihoodFun</v>
       </c>
-      <c r="W12" t="str">
-        <f t="shared" si="8"/>
+      <c r="AD12" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB12&amp;", likelihoodFun = "&amp;AC12&amp;" , paramName = """&amp;G12&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N12&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisExpXChartDomain, likelihoodFun = poisExpXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1676,47 +2018,71 @@
       <c r="M13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N13" s="1" t="str">
+      <c r="N13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="P13" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R13">
+        <v>0.01</v>
+      </c>
+      <c r="S13" t="str">
+        <f t="shared" si="0"/>
+        <v>"&amp;lambda;"</v>
+      </c>
+      <c r="T13" t="str">
+        <f t="shared" si="1"/>
+        <v>"none"</v>
+      </c>
+      <c r="U13" t="str">
+        <f t="shared" si="2"/>
+        <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none")</v>
+      </c>
+      <c r="V13" t="str">
+        <f>B13&amp;"Slider"</f>
+        <v>expSlider</v>
+      </c>
+      <c r="W13" t="str">
+        <f>IF(E13=1,"c()", IF(E13=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+        <v>c()</v>
+      </c>
+      <c r="X13" t="str">
         <f t="shared" si="3"/>
-        <v>expSlider</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P13" t="str">
+        <v>expParamTransform</v>
+      </c>
+      <c r="Y13" t="str">
+        <f>B13&amp;"PlotDistr"</f>
+        <v>expPlotDistr</v>
+      </c>
+      <c r="Z13" t="str">
+        <f>B13&amp;"Draws"</f>
+        <v>expDraws</v>
+      </c>
+      <c r="AA13" t="str">
+        <f>B13&amp;"Latex"</f>
+        <v>expLatex</v>
+      </c>
+      <c r="AB13" t="str">
         <f t="shared" si="4"/>
-        <v>c()</v>
-      </c>
-      <c r="Q13" t="str">
+        <v>expChartDomain</v>
+      </c>
+      <c r="AC13" t="str">
         <f t="shared" si="5"/>
-        <v>expParamTransform</v>
-      </c>
-      <c r="R13" t="str">
-        <f t="shared" si="0"/>
-        <v>expPlotDistr</v>
-      </c>
-      <c r="S13" t="str">
-        <f t="shared" si="1"/>
-        <v>expDraws</v>
-      </c>
-      <c r="T13" t="str">
-        <f t="shared" si="2"/>
-        <v>expLatex</v>
-      </c>
-      <c r="U13" t="str">
-        <f t="shared" si="6"/>
-        <v>expChartDomain</v>
-      </c>
-      <c r="V13" t="str">
-        <f t="shared" si="7"/>
         <v>expLikelihoodFun</v>
       </c>
-      <c r="W13" t="str">
-        <f t="shared" si="8"/>
+      <c r="AD13" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB13&amp;", likelihoodFun = "&amp;AC13&amp;" , paramName = """&amp;G13&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N13&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expChartDomain, likelihoodFun = expLikelihoodFun , paramName = "Lambda",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1756,47 +2122,71 @@
       <c r="M14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N14" s="1" t="str">
+      <c r="N14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O14" s="1">
+        <v>-2</v>
+      </c>
+      <c r="P14" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R14">
+        <v>0.01</v>
+      </c>
+      <c r="S14" t="str">
+        <f t="shared" si="0"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="T14" t="str">
+        <f t="shared" si="1"/>
+        <v>"none"</v>
+      </c>
+      <c r="U14" t="str">
+        <f t="shared" si="2"/>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none")</v>
+      </c>
+      <c r="V14" t="str">
+        <f>B14&amp;"Slider"</f>
+        <v>expExpSlider</v>
+      </c>
+      <c r="W14" t="str">
+        <f>IF(E14=1,"c()", IF(E14=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+        <v>c()</v>
+      </c>
+      <c r="X14" t="str">
         <f t="shared" si="3"/>
-        <v>expExpSlider</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P14" t="str">
+        <v>expExpParamTransform</v>
+      </c>
+      <c r="Y14" t="str">
+        <f>B14&amp;"PlotDistr"</f>
+        <v>expExpPlotDistr</v>
+      </c>
+      <c r="Z14" t="str">
+        <f>B14&amp;"Draws"</f>
+        <v>expExpDraws</v>
+      </c>
+      <c r="AA14" t="str">
+        <f>B14&amp;"Latex"</f>
+        <v>expExpLatex</v>
+      </c>
+      <c r="AB14" t="str">
         <f t="shared" si="4"/>
-        <v>c()</v>
-      </c>
-      <c r="Q14" t="str">
+        <v>expExpChartDomain</v>
+      </c>
+      <c r="AC14" t="str">
         <f t="shared" si="5"/>
-        <v>expExpParamTransform</v>
-      </c>
-      <c r="R14" t="str">
-        <f t="shared" si="0"/>
-        <v>expExpPlotDistr</v>
-      </c>
-      <c r="S14" t="str">
-        <f t="shared" si="1"/>
-        <v>expExpDraws</v>
-      </c>
-      <c r="T14" t="str">
-        <f t="shared" si="2"/>
-        <v>expExpLatex</v>
-      </c>
-      <c r="U14" t="str">
-        <f t="shared" si="6"/>
-        <v>expExpChartDomain</v>
-      </c>
-      <c r="V14" t="str">
-        <f t="shared" si="7"/>
         <v>expExpLikelihoodFun</v>
       </c>
-      <c r="W14" t="str">
-        <f t="shared" si="8"/>
+      <c r="AD14" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB14&amp;", likelihoodFun = "&amp;AC14&amp;" , paramName = """&amp;G14&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N14&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expExpChartDomain, likelihoodFun = expExpLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1836,43 +2226,67 @@
       <c r="M15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N15" s="1" t="str">
-        <f t="shared" ref="N15" si="10">B15&amp;"Slider"</f>
+      <c r="N15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O15" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="R15">
+        <v>0.01</v>
+      </c>
+      <c r="S15" t="str">
+        <f t="shared" si="0"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="T15" t="str">
+        <f t="shared" si="1"/>
+        <v>"betas"</v>
+      </c>
+      <c r="U15" t="str">
+        <f t="shared" si="2"/>
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas")</v>
+      </c>
+      <c r="V15" t="str">
+        <f>B15&amp;"Slider"</f>
         <v>expExpXSlider</v>
       </c>
-      <c r="O15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P15" t="str">
+      <c r="W15" t="str">
+        <f>IF(E15=1,"c()", IF(E15=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+        <v>c("Beta0", "Beta1", "Beta2")</v>
+      </c>
+      <c r="X15" t="str">
+        <f t="shared" si="3"/>
+        <v>expExpXParamTransform</v>
+      </c>
+      <c r="Y15" t="str">
+        <f>B15&amp;"PlotDistr"</f>
+        <v>expExpXPlotDistr</v>
+      </c>
+      <c r="Z15" t="str">
+        <f>B15&amp;"Draws"</f>
+        <v>expExpXDraws</v>
+      </c>
+      <c r="AA15" t="str">
+        <f>B15&amp;"Latex"</f>
+        <v>expExpXLatex</v>
+      </c>
+      <c r="AB15" t="str">
         <f t="shared" si="4"/>
-        <v>c("Beta0", "Beta1", "Beta2")</v>
-      </c>
-      <c r="Q15" t="str">
+        <v>expExpXChartDomain</v>
+      </c>
+      <c r="AC15" t="str">
         <f t="shared" si="5"/>
-        <v>expExpXParamTransform</v>
-      </c>
-      <c r="R15" t="str">
-        <f t="shared" si="0"/>
-        <v>expExpXPlotDistr</v>
-      </c>
-      <c r="S15" t="str">
-        <f t="shared" si="1"/>
-        <v>expExpXDraws</v>
-      </c>
-      <c r="T15" t="str">
-        <f t="shared" si="2"/>
-        <v>expExpXLatex</v>
-      </c>
-      <c r="U15" t="str">
-        <f t="shared" si="6"/>
-        <v>expExpXChartDomain</v>
-      </c>
-      <c r="V15" t="str">
-        <f t="shared" si="7"/>
         <v>expExpXLikelihoodFun</v>
       </c>
-      <c r="W15" t="str">
-        <f t="shared" si="8"/>
+      <c r="AD15" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB15&amp;", likelihoodFun = "&amp;AC15&amp;" , paramName = """&amp;G15&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N15&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expExpXChartDomain, likelihoodFun = expExpXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>

</xml_diff>

<commit_message>
large refactor needed for manual MLE
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB57B2A4-D612-48C0-A489-7468D490E158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D30026-19C5-4760-88B0-411C48242F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="110">
   <si>
     <t>Bernoulli-Pi</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Normal</t>
   </si>
   <si>
-    <t>sliderList</t>
-  </si>
-  <si>
     <t>shortName</t>
   </si>
   <si>
@@ -343,6 +340,30 @@
   </si>
   <si>
     <t>c(1,-1,.25,1)</t>
+  </si>
+  <si>
+    <t>analyticDomain</t>
+  </si>
+  <si>
+    <t>c(-5,5)</t>
+  </si>
+  <si>
+    <t>c(-7,7)</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>analyticRange</t>
+  </si>
+  <si>
+    <t>c(0,.5)</t>
+  </si>
+  <si>
+    <t>c(0,.75)</t>
+  </si>
+  <si>
+    <t>pdfList</t>
   </si>
 </sst>
 </file>
@@ -709,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
-  <dimension ref="A1:AD15"/>
+  <dimension ref="A1:AF15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,120 +747,125 @@
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" customWidth="1"/>
-    <col min="14" max="14" width="16" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" customWidth="1"/>
-    <col min="16" max="16" width="4.28515625" customWidth="1"/>
-    <col min="17" max="17" width="5.5703125" customWidth="1"/>
-    <col min="18" max="18" width="6" customWidth="1"/>
-    <col min="19" max="20" width="4.28515625" customWidth="1"/>
-    <col min="21" max="21" width="16" customWidth="1"/>
-    <col min="22" max="22" width="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="26" customWidth="1"/>
-    <col min="25" max="25" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="15.5703125" customWidth="1"/>
+    <col min="14" max="16" width="16" customWidth="1"/>
+    <col min="17" max="17" width="6.140625" customWidth="1"/>
+    <col min="18" max="18" width="4.28515625" customWidth="1"/>
+    <col min="19" max="19" width="5.5703125" customWidth="1"/>
+    <col min="20" max="20" width="6" customWidth="1"/>
+    <col min="21" max="22" width="4.28515625" customWidth="1"/>
+    <col min="23" max="23" width="16" customWidth="1"/>
+    <col min="24" max="24" width="26" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="26" customWidth="1"/>
+    <col min="27" max="27" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" t="s">
+        <v>102</v>
+      </c>
+      <c r="P1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>86</v>
+      </c>
+      <c r="R1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1" t="s">
+        <v>88</v>
+      </c>
+      <c r="T1" t="s">
+        <v>89</v>
+      </c>
+      <c r="U1" t="s">
+        <v>90</v>
+      </c>
+      <c r="V1" t="s">
+        <v>91</v>
+      </c>
+      <c r="W1" t="s">
+        <v>92</v>
+      </c>
+      <c r="X1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="Y1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" t="s">
-        <v>53</v>
-      </c>
-      <c r="M1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N1" t="s">
-        <v>72</v>
-      </c>
-      <c r="O1" t="s">
-        <v>87</v>
-      </c>
-      <c r="P1" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>89</v>
-      </c>
-      <c r="R1" t="s">
-        <v>90</v>
-      </c>
-      <c r="S1" t="s">
-        <v>91</v>
-      </c>
-      <c r="T1" t="s">
-        <v>92</v>
-      </c>
-      <c r="U1" t="s">
-        <v>93</v>
-      </c>
-      <c r="V1" t="s">
-        <v>11</v>
-      </c>
-      <c r="W1" t="s">
-        <v>27</v>
-      </c>
-      <c r="X1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y1" t="s">
+      <c r="AC1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -854,96 +880,102 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O2" s="1">
+        <v>72</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" s="1">
         <v>0</v>
       </c>
-      <c r="P2" s="1">
+      <c r="R2" s="1">
         <v>1</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="R2">
+      <c r="S2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="T2">
         <v>0.01</v>
       </c>
-      <c r="S2" t="str">
+      <c r="U2" t="str">
         <f>"""&amp;"&amp;RIGHT(K2,LEN(K2)-1)&amp;";"""</f>
         <v>"&amp;pi;"</v>
       </c>
-      <c r="T2" t="str">
+      <c r="V2" t="str">
         <f>IF(F2=1,"""none""",IF(E2=F2,"""betas""","""fullNorm"""))</f>
         <v>"none"</v>
       </c>
-      <c r="U2" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;O2&amp;", maxVal = "&amp;P2&amp;", startVals = "&amp;Q2&amp;", stepVal = "&amp;R2&amp;", paramHTML = "&amp;S2&amp;", multi = "&amp;T2&amp;")"</f>
-        <v>manyParamSliderMaker(minVal =0, maxVal = 1, startVals = c(.3), stepVal = 0.01, paramHTML = "&amp;pi;", multi = "none")</v>
-      </c>
-      <c r="V2" t="str">
-        <f>B2&amp;"Slider"</f>
-        <v>bernSlider</v>
-      </c>
       <c r="W2" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;Q2&amp;", maxVal = "&amp;R2&amp;", startVals = "&amp;S2&amp;", stepVal = "&amp;T2&amp;", paramHTML = "&amp;U2&amp;", multi = "&amp;V2&amp;","</f>
+        <v>manyParamSliderMaker(minVal =0, maxVal = 1, startVals = c(.3), stepVal = 0.01, paramHTML = "&amp;pi;", multi = "none",</v>
+      </c>
+      <c r="X2" t="str">
         <f>IF(E2=1,"c()", IF(E2=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
-      <c r="X2" t="str">
+      <c r="Y2" t="str">
         <f>$B2&amp;"ParamTransform"</f>
         <v>bernParamTransform</v>
       </c>
-      <c r="Y2" t="str">
+      <c r="Z2" t="str">
+        <f>$B2&amp;"PDF"</f>
+        <v>bernPDF</v>
+      </c>
+      <c r="AA2" t="str">
         <f>B2&amp;"PlotDistr"</f>
         <v>bernPlotDistr</v>
       </c>
-      <c r="Z2" t="str">
+      <c r="AB2" t="str">
         <f>B2&amp;"Draws"</f>
         <v>bernDraws</v>
       </c>
-      <c r="AA2" t="str">
+      <c r="AC2" t="str">
         <f>B2&amp;"Latex"</f>
         <v>bernLatex</v>
       </c>
-      <c r="AB2" t="str">
+      <c r="AD2" t="str">
         <f>$B2&amp;"ChartDomain"</f>
         <v>bernChartDomain</v>
       </c>
-      <c r="AC2" t="str">
+      <c r="AE2" t="str">
         <f>$B2&amp;"LikelihoodFun"</f>
         <v>bernLikelihoodFun</v>
       </c>
-      <c r="AD2" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB2&amp;", likelihoodFun = "&amp;AC2&amp;" , paramName = """&amp;G2&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N2&amp;""")}"</f>
+      <c r="AF2" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD2&amp;", likelihoodFun = "&amp;AE2&amp;" , paramName = """&amp;G2&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N2&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernChartDomain, likelihoodFun = bernLikelihoodFun , paramName = "Pi",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
@@ -958,96 +990,102 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O3" s="1">
+        <v>72</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q3" s="1">
         <v>-2</v>
       </c>
-      <c r="P3" s="1">
+      <c r="R3" s="1">
         <v>2</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="R3">
+      <c r="S3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="T3">
         <v>0.01</v>
       </c>
-      <c r="S3" t="str">
-        <f t="shared" ref="S3:S15" si="0">"""&amp;"&amp;RIGHT(K3,LEN(K3)-1)&amp;";"""</f>
+      <c r="U3" t="str">
+        <f t="shared" ref="U3:U15" si="0">"""&amp;"&amp;RIGHT(K3,LEN(K3)-1)&amp;";"""</f>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="T3" t="str">
-        <f t="shared" ref="T3:T15" si="1">IF(F3=1,"""none""",IF(E3=F3,"""betas""","""fullNorm"""))</f>
+      <c r="V3" t="str">
+        <f t="shared" ref="V3:V15" si="1">IF(F3=1,"""none""",IF(E3=F3,"""betas""","""fullNorm"""))</f>
         <v>"none"</v>
       </c>
-      <c r="U3" t="str">
-        <f t="shared" ref="U3:U15" si="2">"manyParamSliderMaker(minVal ="&amp;O3&amp;", maxVal = "&amp;P3&amp;", startVals = "&amp;Q3&amp;", stepVal = "&amp;R3&amp;", paramHTML = "&amp;S3&amp;", multi = "&amp;T3&amp;")"</f>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none")</v>
-      </c>
-      <c r="V3" t="str">
-        <f>B3&amp;"Slider"</f>
-        <v>bernLogitSlider</v>
-      </c>
       <c r="W3" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;Q3&amp;", maxVal = "&amp;R3&amp;", startVals = "&amp;S3&amp;", stepVal = "&amp;T3&amp;", paramHTML = "&amp;U3&amp;", multi = "&amp;V3&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
+      </c>
+      <c r="X3" t="str">
         <f>IF(E3=1,"c()", IF(E3=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
-      <c r="X3" t="str">
-        <f t="shared" ref="X3:X15" si="3">$B3&amp;"ParamTransform"</f>
+      <c r="Y3" t="str">
+        <f t="shared" ref="Y3:Y15" si="2">$B3&amp;"ParamTransform"</f>
         <v>bernLogitParamTransform</v>
       </c>
-      <c r="Y3" t="str">
+      <c r="Z3" t="str">
+        <f t="shared" ref="Z3:Z15" si="3">$B3&amp;"PDF"</f>
+        <v>bernLogitPDF</v>
+      </c>
+      <c r="AA3" t="str">
         <f>B3&amp;"PlotDistr"</f>
         <v>bernLogitPlotDistr</v>
       </c>
-      <c r="Z3" t="str">
+      <c r="AB3" t="str">
         <f>B3&amp;"Draws"</f>
         <v>bernLogitDraws</v>
       </c>
-      <c r="AA3" t="str">
+      <c r="AC3" t="str">
         <f>B3&amp;"Latex"</f>
         <v>bernLogitLatex</v>
       </c>
-      <c r="AB3" t="str">
-        <f t="shared" ref="AB3:AB15" si="4">$B3&amp;"ChartDomain"</f>
+      <c r="AD3" t="str">
+        <f t="shared" ref="AD3:AD15" si="4">$B3&amp;"ChartDomain"</f>
         <v>bernLogitChartDomain</v>
       </c>
-      <c r="AC3" t="str">
-        <f t="shared" ref="AC3:AC15" si="5">$B3&amp;"LikelihoodFun"</f>
+      <c r="AE3" t="str">
+        <f t="shared" ref="AE3:AE15" si="5">$B3&amp;"LikelihoodFun"</f>
         <v>bernLogitLikelihoodFun</v>
       </c>
-      <c r="AD3" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB3&amp;", likelihoodFun = "&amp;AC3&amp;" , paramName = """&amp;G3&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N3&amp;""")}"</f>
+      <c r="AF3" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD3&amp;", likelihoodFun = "&amp;AE3&amp;" , paramName = """&amp;G3&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N3&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernLogitChartDomain, likelihoodFun = bernLogitLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
@@ -1062,96 +1100,102 @@
         <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O4" s="1">
+        <v>72</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q4" s="1">
         <v>-2</v>
       </c>
-      <c r="P4" s="1">
+      <c r="R4" s="1">
         <v>2</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R4">
+      <c r="S4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="T4">
         <v>0.01</v>
       </c>
-      <c r="S4" t="str">
+      <c r="U4" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="T4" t="str">
+      <c r="V4" t="str">
         <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="U4" t="str">
-        <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas")</v>
-      </c>
-      <c r="V4" t="str">
-        <f>B4&amp;"Slider"</f>
-        <v>bernLogitXSlider</v>
-      </c>
       <c r="W4" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;Q4&amp;", maxVal = "&amp;R4&amp;", startVals = "&amp;S4&amp;", stepVal = "&amp;T4&amp;", paramHTML = "&amp;U4&amp;", multi = "&amp;V4&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
+      </c>
+      <c r="X4" t="str">
         <f>IF(E4=1,"c()", IF(E4=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
-      <c r="X4" t="str">
+      <c r="Y4" t="str">
+        <f t="shared" si="2"/>
+        <v>bernLogitXParamTransform</v>
+      </c>
+      <c r="Z4" t="str">
         <f t="shared" si="3"/>
-        <v>bernLogitXParamTransform</v>
-      </c>
-      <c r="Y4" t="str">
+        <v>bernLogitXPDF</v>
+      </c>
+      <c r="AA4" t="str">
         <f>B4&amp;"PlotDistr"</f>
         <v>bernLogitXPlotDistr</v>
       </c>
-      <c r="Z4" t="str">
+      <c r="AB4" t="str">
         <f>B4&amp;"Draws"</f>
         <v>bernLogitXDraws</v>
       </c>
-      <c r="AA4" t="str">
+      <c r="AC4" t="str">
         <f>B4&amp;"Latex"</f>
         <v>bernLogitXLatex</v>
       </c>
-      <c r="AB4" t="str">
+      <c r="AD4" t="str">
         <f t="shared" si="4"/>
         <v>bernLogitXChartDomain</v>
       </c>
-      <c r="AC4" t="str">
+      <c r="AE4" t="str">
         <f t="shared" si="5"/>
         <v>bernLogitXLikelihoodFun</v>
       </c>
-      <c r="AD4" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB4&amp;", likelihoodFun = "&amp;AC4&amp;" , paramName = """&amp;G4&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N4&amp;""")}"</f>
+      <c r="AF4" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD4&amp;", likelihoodFun = "&amp;AE4&amp;" , paramName = """&amp;G4&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N4&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernLogitXChartDomain, likelihoodFun = bernLogitXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
@@ -1166,96 +1210,102 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O5" s="1">
+        <v>72</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q5" s="1">
         <v>-2</v>
       </c>
-      <c r="P5" s="1">
+      <c r="R5" s="1">
         <v>2</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="R5">
+      <c r="S5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="T5">
         <v>0.01</v>
       </c>
-      <c r="S5" t="str">
+      <c r="U5" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="T5" t="str">
+      <c r="V5" t="str">
         <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="U5" t="str">
-        <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none")</v>
-      </c>
-      <c r="V5" t="str">
-        <f>B5&amp;"Slider"</f>
-        <v>styNormSlider</v>
-      </c>
       <c r="W5" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;Q5&amp;", maxVal = "&amp;R5&amp;", startVals = "&amp;S5&amp;", stepVal = "&amp;T5&amp;", paramHTML = "&amp;U5&amp;", multi = "&amp;V5&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
+      </c>
+      <c r="X5" t="str">
         <f>IF(E5=1,"c()", IF(E5=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
-      <c r="X5" t="str">
+      <c r="Y5" t="str">
+        <f t="shared" si="2"/>
+        <v>styNormParamTransform</v>
+      </c>
+      <c r="Z5" t="str">
         <f t="shared" si="3"/>
-        <v>styNormParamTransform</v>
-      </c>
-      <c r="Y5" t="str">
+        <v>styNormPDF</v>
+      </c>
+      <c r="AA5" t="str">
         <f>B5&amp;"PlotDistr"</f>
         <v>styNormPlotDistr</v>
       </c>
-      <c r="Z5" t="str">
+      <c r="AB5" t="str">
         <f>B5&amp;"Draws"</f>
         <v>styNormDraws</v>
       </c>
-      <c r="AA5" t="str">
+      <c r="AC5" t="str">
         <f>B5&amp;"Latex"</f>
         <v>styNormLatex</v>
       </c>
-      <c r="AB5" t="str">
+      <c r="AD5" t="str">
         <f t="shared" si="4"/>
         <v>styNormChartDomain</v>
       </c>
-      <c r="AC5" t="str">
+      <c r="AE5" t="str">
         <f t="shared" si="5"/>
         <v>styNormLikelihoodFun</v>
       </c>
-      <c r="AD5" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB5&amp;", likelihoodFun = "&amp;AC5&amp;" , paramName = """&amp;G5&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N5&amp;""")}"</f>
+      <c r="AF5" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD5&amp;", likelihoodFun = "&amp;AE5&amp;" , paramName = """&amp;G5&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N5&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = styNormChartDomain, likelihoodFun = styNormLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
@@ -1270,99 +1320,105 @@
         <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O6" s="1">
+        <v>72</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q6" s="1">
         <v>-2</v>
       </c>
-      <c r="P6" s="1">
+      <c r="R6" s="1">
         <v>2</v>
       </c>
-      <c r="Q6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R6">
+      <c r="S6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="T6">
         <v>0.01</v>
       </c>
-      <c r="S6" t="str">
+      <c r="U6" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="T6" t="str">
+      <c r="V6" t="str">
         <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="U6" t="str">
-        <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas")</v>
-      </c>
-      <c r="V6" t="str">
-        <f>B6&amp;"Slider"</f>
-        <v>styNormXSlider</v>
-      </c>
       <c r="W6" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;Q6&amp;", maxVal = "&amp;R6&amp;", startVals = "&amp;S6&amp;", stepVal = "&amp;T6&amp;", paramHTML = "&amp;U6&amp;", multi = "&amp;V6&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
+      </c>
+      <c r="X6" t="str">
         <f>IF(E6=1,"c()", IF(E6=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
-      <c r="X6" t="str">
+      <c r="Y6" t="str">
+        <f t="shared" si="2"/>
+        <v>styNormXParamTransform</v>
+      </c>
+      <c r="Z6" t="str">
         <f t="shared" si="3"/>
-        <v>styNormXParamTransform</v>
-      </c>
-      <c r="Y6" t="str">
+        <v>styNormXPDF</v>
+      </c>
+      <c r="AA6" t="str">
         <f>B6&amp;"PlotDistr"</f>
         <v>styNormXPlotDistr</v>
       </c>
-      <c r="Z6" t="str">
+      <c r="AB6" t="str">
         <f>B6&amp;"Draws"</f>
         <v>styNormXDraws</v>
       </c>
-      <c r="AA6" t="str">
+      <c r="AC6" t="str">
         <f>B6&amp;"Latex"</f>
         <v>styNormXLatex</v>
       </c>
-      <c r="AB6" t="str">
+      <c r="AD6" t="str">
         <f t="shared" si="4"/>
         <v>styNormXChartDomain</v>
       </c>
-      <c r="AC6" t="str">
+      <c r="AE6" t="str">
         <f t="shared" si="5"/>
         <v>styNormXLikelihoodFun</v>
       </c>
-      <c r="AD6" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB6&amp;", likelihoodFun = "&amp;AC6&amp;" , paramName = """&amp;G6&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N6&amp;""")}"</f>
+      <c r="AF6" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD6&amp;", likelihoodFun = "&amp;AE6&amp;" , paramName = """&amp;G6&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N6&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = styNormXChartDomain, likelihoodFun = styNormXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
@@ -1374,96 +1430,102 @@
         <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="O7" s="1">
+        <v>73</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q7" s="1">
         <v>-2</v>
       </c>
-      <c r="P7" s="1">
+      <c r="R7" s="1">
         <v>2</v>
       </c>
-      <c r="Q7" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="R7">
+      <c r="S7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="T7">
         <v>0.01</v>
       </c>
-      <c r="S7" t="str">
+      <c r="U7" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="T7" t="str">
+      <c r="V7" t="str">
         <f t="shared" si="1"/>
         <v>"fullNorm"</v>
       </c>
-      <c r="U7" t="str">
-        <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25,1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm")</v>
-      </c>
-      <c r="V7" t="str">
-        <f>B7&amp;"Slider"</f>
-        <v>fullNormXSlider</v>
-      </c>
       <c r="W7" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;Q7&amp;", maxVal = "&amp;R7&amp;", startVals = "&amp;S7&amp;", stepVal = "&amp;T7&amp;", paramHTML = "&amp;U7&amp;", multi = "&amp;V7&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25,1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm",</v>
+      </c>
+      <c r="X7" t="str">
         <f>IF(E7=1,"c()", IF(E7=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2","Sigma")</v>
       </c>
-      <c r="X7" t="str">
+      <c r="Y7" t="str">
+        <f t="shared" si="2"/>
+        <v>fullNormXParamTransform</v>
+      </c>
+      <c r="Z7" t="str">
         <f t="shared" si="3"/>
-        <v>fullNormXParamTransform</v>
-      </c>
-      <c r="Y7" t="str">
+        <v>fullNormXPDF</v>
+      </c>
+      <c r="AA7" t="str">
         <f>B7&amp;"PlotDistr"</f>
         <v>fullNormXPlotDistr</v>
       </c>
-      <c r="Z7" t="str">
+      <c r="AB7" t="str">
         <f>B7&amp;"Draws"</f>
         <v>fullNormXDraws</v>
       </c>
-      <c r="AA7" t="str">
+      <c r="AC7" t="str">
         <f>B7&amp;"Latex"</f>
         <v>fullNormXLatex</v>
       </c>
-      <c r="AB7" t="str">
+      <c r="AD7" t="str">
         <f t="shared" si="4"/>
         <v>fullNormXChartDomain</v>
       </c>
-      <c r="AC7" t="str">
+      <c r="AE7" t="str">
         <f t="shared" si="5"/>
         <v>fullNormXLikelihoodFun</v>
       </c>
-      <c r="AD7" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB7&amp;", likelihoodFun = "&amp;AC7&amp;" , paramName = """&amp;G7&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N7&amp;""")}"</f>
+      <c r="AF7" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD7&amp;", likelihoodFun = "&amp;AE7&amp;" , paramName = """&amp;G7&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N7&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = fullNormXChartDomain, likelihoodFun = fullNormXLikelihoodFun , paramName = "Beta/Sigma",  xVals = xVals, margNum = margNum, optimMethod = "SANN")}</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -1478,96 +1540,102 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O8" s="1">
+        <v>72</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q8" s="1">
         <v>-0.5</v>
       </c>
-      <c r="P8" s="1">
+      <c r="R8" s="1">
         <v>2</v>
       </c>
-      <c r="Q8" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="R8">
+      <c r="S8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="T8">
         <v>0.01</v>
       </c>
-      <c r="S8" t="str">
+      <c r="U8" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="T8" t="str">
+      <c r="V8" t="str">
         <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="U8" t="str">
-        <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 2, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none")</v>
-      </c>
-      <c r="V8" t="str">
-        <f>B8&amp;"Slider"</f>
-        <v>logNormSlider</v>
-      </c>
       <c r="W8" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;Q8&amp;", maxVal = "&amp;R8&amp;", startVals = "&amp;S8&amp;", stepVal = "&amp;T8&amp;", paramHTML = "&amp;U8&amp;", multi = "&amp;V8&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 2, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
+      </c>
+      <c r="X8" t="str">
         <f>IF(E8=1,"c()", IF(E8=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
-      <c r="X8" t="str">
+      <c r="Y8" t="str">
+        <f t="shared" si="2"/>
+        <v>logNormParamTransform</v>
+      </c>
+      <c r="Z8" t="str">
         <f t="shared" si="3"/>
-        <v>logNormParamTransform</v>
-      </c>
-      <c r="Y8" t="str">
+        <v>logNormPDF</v>
+      </c>
+      <c r="AA8" t="str">
         <f>B8&amp;"PlotDistr"</f>
         <v>logNormPlotDistr</v>
       </c>
-      <c r="Z8" t="str">
+      <c r="AB8" t="str">
         <f>B8&amp;"Draws"</f>
         <v>logNormDraws</v>
       </c>
-      <c r="AA8" t="str">
+      <c r="AC8" t="str">
         <f>B8&amp;"Latex"</f>
         <v>logNormLatex</v>
       </c>
-      <c r="AB8" t="str">
+      <c r="AD8" t="str">
         <f t="shared" si="4"/>
         <v>logNormChartDomain</v>
       </c>
-      <c r="AC8" t="str">
+      <c r="AE8" t="str">
         <f t="shared" si="5"/>
         <v>logNormLikelihoodFun</v>
       </c>
-      <c r="AD8" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB8&amp;", likelihoodFun = "&amp;AC8&amp;" , paramName = """&amp;G8&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N8&amp;""")}"</f>
+      <c r="AF8" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD8&amp;", likelihoodFun = "&amp;AE8&amp;" , paramName = """&amp;G8&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N8&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = logNormChartDomain, likelihoodFun = logNormLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
@@ -1582,96 +1650,102 @@
         <v>3</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="N9" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O9" s="1">
+        <v>72</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q9" s="1">
         <v>-1</v>
       </c>
-      <c r="P9" s="1">
+      <c r="R9" s="1">
         <v>2</v>
       </c>
-      <c r="Q9" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="R9">
+      <c r="S9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="T9">
         <v>0.01</v>
       </c>
-      <c r="S9" t="str">
+      <c r="U9" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="T9" t="str">
+      <c r="V9" t="str">
         <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="U9" t="str">
-        <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-1, maxVal = 2, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas")</v>
-      </c>
-      <c r="V9" t="str">
-        <f>B9&amp;"Slider"</f>
-        <v>logNormXSlider</v>
-      </c>
       <c r="W9" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;Q9&amp;", maxVal = "&amp;R9&amp;", startVals = "&amp;S9&amp;", stepVal = "&amp;T9&amp;", paramHTML = "&amp;U9&amp;", multi = "&amp;V9&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-1, maxVal = 2, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
+      </c>
+      <c r="X9" t="str">
         <f>IF(E9=1,"c()", IF(E9=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
-      <c r="X9" t="str">
+      <c r="Y9" t="str">
+        <f t="shared" si="2"/>
+        <v>logNormXParamTransform</v>
+      </c>
+      <c r="Z9" t="str">
         <f t="shared" si="3"/>
-        <v>logNormXParamTransform</v>
-      </c>
-      <c r="Y9" t="str">
+        <v>logNormXPDF</v>
+      </c>
+      <c r="AA9" t="str">
         <f>B9&amp;"PlotDistr"</f>
         <v>logNormXPlotDistr</v>
       </c>
-      <c r="Z9" t="str">
+      <c r="AB9" t="str">
         <f>B9&amp;"Draws"</f>
         <v>logNormXDraws</v>
       </c>
-      <c r="AA9" t="str">
+      <c r="AC9" t="str">
         <f>B9&amp;"Latex"</f>
         <v>logNormXLatex</v>
       </c>
-      <c r="AB9" t="str">
+      <c r="AD9" t="str">
         <f t="shared" si="4"/>
         <v>logNormXChartDomain</v>
       </c>
-      <c r="AC9" t="str">
+      <c r="AE9" t="str">
         <f t="shared" si="5"/>
         <v>logNormXLikelihoodFun</v>
       </c>
-      <c r="AD9" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB9&amp;", likelihoodFun = "&amp;AC9&amp;" , paramName = """&amp;G9&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N9&amp;""")}"</f>
+      <c r="AF9" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD9&amp;", likelihoodFun = "&amp;AE9&amp;" , paramName = """&amp;G9&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N9&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = logNormXChartDomain, likelihoodFun = logNormXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
@@ -1686,99 +1760,105 @@
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O10" s="1">
+        <v>72</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q10" s="1">
         <v>1</v>
       </c>
-      <c r="P10" s="1">
+      <c r="R10" s="1">
         <v>10</v>
       </c>
-      <c r="Q10" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="R10">
+      <c r="S10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="T10">
         <v>0.01</v>
       </c>
-      <c r="S10" t="str">
+      <c r="U10" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;lambda;"</v>
       </c>
-      <c r="T10" t="str">
+      <c r="V10" t="str">
         <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="U10" t="str">
-        <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =1, maxVal = 10, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none")</v>
-      </c>
-      <c r="V10" t="str">
-        <f>B10&amp;"Slider"</f>
-        <v>poisSlider</v>
-      </c>
       <c r="W10" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;Q10&amp;", maxVal = "&amp;R10&amp;", startVals = "&amp;S10&amp;", stepVal = "&amp;T10&amp;", paramHTML = "&amp;U10&amp;", multi = "&amp;V10&amp;","</f>
+        <v>manyParamSliderMaker(minVal =1, maxVal = 10, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none",</v>
+      </c>
+      <c r="X10" t="str">
         <f>IF(E10=1,"c()", IF(E10=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
-      <c r="X10" t="str">
+      <c r="Y10" t="str">
+        <f t="shared" si="2"/>
+        <v>poisParamTransform</v>
+      </c>
+      <c r="Z10" t="str">
         <f t="shared" si="3"/>
-        <v>poisParamTransform</v>
-      </c>
-      <c r="Y10" t="str">
+        <v>poisPDF</v>
+      </c>
+      <c r="AA10" t="str">
         <f>B10&amp;"PlotDistr"</f>
         <v>poisPlotDistr</v>
       </c>
-      <c r="Z10" t="str">
+      <c r="AB10" t="str">
         <f>B10&amp;"Draws"</f>
         <v>poisDraws</v>
       </c>
-      <c r="AA10" t="str">
+      <c r="AC10" t="str">
         <f>B10&amp;"Latex"</f>
         <v>poisLatex</v>
       </c>
-      <c r="AB10" t="str">
+      <c r="AD10" t="str">
         <f t="shared" si="4"/>
         <v>poisChartDomain</v>
       </c>
-      <c r="AC10" t="str">
+      <c r="AE10" t="str">
         <f t="shared" si="5"/>
         <v>poisLikelihoodFun</v>
       </c>
-      <c r="AD10" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB10&amp;", likelihoodFun = "&amp;AC10&amp;" , paramName = """&amp;G10&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N10&amp;""")}"</f>
+      <c r="AF10" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD10&amp;", likelihoodFun = "&amp;AE10&amp;" , paramName = """&amp;G10&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N10&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisChartDomain, likelihoodFun = poisLikelihoodFun , paramName = "Lambda",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>7</v>
@@ -1790,99 +1870,105 @@
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="M11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O11" s="1">
+        <v>72</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q11" s="1">
         <v>-0.25</v>
       </c>
-      <c r="P11" s="1">
+      <c r="R11" s="1">
         <v>3</v>
       </c>
-      <c r="Q11" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="R11">
+      <c r="S11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="T11">
         <v>0.01</v>
       </c>
-      <c r="S11" t="str">
+      <c r="U11" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="T11" t="str">
+      <c r="V11" t="str">
         <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="U11" t="str">
-        <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none")</v>
-      </c>
-      <c r="V11" t="str">
-        <f>B11&amp;"Slider"</f>
-        <v>poisExpSlider</v>
-      </c>
       <c r="W11" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;Q11&amp;", maxVal = "&amp;R11&amp;", startVals = "&amp;S11&amp;", stepVal = "&amp;T11&amp;", paramHTML = "&amp;U11&amp;", multi = "&amp;V11&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
+      </c>
+      <c r="X11" t="str">
         <f>IF(E11=1,"c()", IF(E11=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
-      <c r="X11" t="str">
+      <c r="Y11" t="str">
+        <f t="shared" si="2"/>
+        <v>poisExpParamTransform</v>
+      </c>
+      <c r="Z11" t="str">
         <f t="shared" si="3"/>
-        <v>poisExpParamTransform</v>
-      </c>
-      <c r="Y11" t="str">
+        <v>poisExpPDF</v>
+      </c>
+      <c r="AA11" t="str">
         <f>B11&amp;"PlotDistr"</f>
         <v>poisExpPlotDistr</v>
       </c>
-      <c r="Z11" t="str">
+      <c r="AB11" t="str">
         <f>B11&amp;"Draws"</f>
         <v>poisExpDraws</v>
       </c>
-      <c r="AA11" t="str">
+      <c r="AC11" t="str">
         <f>B11&amp;"Latex"</f>
         <v>poisExpLatex</v>
       </c>
-      <c r="AB11" t="str">
+      <c r="AD11" t="str">
         <f t="shared" si="4"/>
         <v>poisExpChartDomain</v>
       </c>
-      <c r="AC11" t="str">
+      <c r="AE11" t="str">
         <f t="shared" si="5"/>
         <v>poisExpLikelihoodFun</v>
       </c>
-      <c r="AD11" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB11&amp;", likelihoodFun = "&amp;AC11&amp;" , paramName = """&amp;G11&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N11&amp;""")}"</f>
+      <c r="AF11" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD11&amp;", likelihoodFun = "&amp;AE11&amp;" , paramName = """&amp;G11&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N11&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisExpChartDomain, likelihoodFun = poisExpLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>7</v>
@@ -1894,96 +1980,102 @@
         <v>3</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="M12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O12" s="1">
+        <v>72</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q12" s="1">
         <v>-1</v>
       </c>
-      <c r="P12" s="1">
+      <c r="R12" s="1">
         <v>1</v>
       </c>
-      <c r="Q12" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="R12">
+      <c r="S12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="T12">
         <v>0.01</v>
       </c>
-      <c r="S12" t="str">
+      <c r="U12" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="T12" t="str">
+      <c r="V12" t="str">
         <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="U12" t="str">
-        <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-1, maxVal = 1, startVals = c(-.3,1,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas")</v>
-      </c>
-      <c r="V12" t="str">
-        <f>B12&amp;"Slider"</f>
-        <v>poisExpXSlider</v>
-      </c>
       <c r="W12" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;Q12&amp;", maxVal = "&amp;R12&amp;", startVals = "&amp;S12&amp;", stepVal = "&amp;T12&amp;", paramHTML = "&amp;U12&amp;", multi = "&amp;V12&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-1, maxVal = 1, startVals = c(-.3,1,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
+      </c>
+      <c r="X12" t="str">
         <f>IF(E12=1,"c()", IF(E12=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
-      <c r="X12" t="str">
+      <c r="Y12" t="str">
+        <f t="shared" si="2"/>
+        <v>poisExpXParamTransform</v>
+      </c>
+      <c r="Z12" t="str">
         <f t="shared" si="3"/>
-        <v>poisExpXParamTransform</v>
-      </c>
-      <c r="Y12" t="str">
+        <v>poisExpXPDF</v>
+      </c>
+      <c r="AA12" t="str">
         <f>B12&amp;"PlotDistr"</f>
         <v>poisExpXPlotDistr</v>
       </c>
-      <c r="Z12" t="str">
+      <c r="AB12" t="str">
         <f>B12&amp;"Draws"</f>
         <v>poisExpXDraws</v>
       </c>
-      <c r="AA12" t="str">
+      <c r="AC12" t="str">
         <f>B12&amp;"Latex"</f>
         <v>poisExpXLatex</v>
       </c>
-      <c r="AB12" t="str">
+      <c r="AD12" t="str">
         <f t="shared" si="4"/>
         <v>poisExpXChartDomain</v>
       </c>
-      <c r="AC12" t="str">
+      <c r="AE12" t="str">
         <f t="shared" si="5"/>
         <v>poisExpXLikelihoodFun</v>
       </c>
-      <c r="AD12" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB12&amp;", likelihoodFun = "&amp;AC12&amp;" , paramName = """&amp;G12&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N12&amp;""")}"</f>
+      <c r="AF12" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD12&amp;", likelihoodFun = "&amp;AE12&amp;" , paramName = """&amp;G12&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N12&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisExpXChartDomain, likelihoodFun = poisExpXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>8</v>
@@ -1998,99 +2090,105 @@
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O13" s="1">
+        <v>72</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q13" s="1">
         <v>0.25</v>
       </c>
-      <c r="P13" s="1">
+      <c r="R13" s="1">
         <v>1.5</v>
       </c>
-      <c r="Q13" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="R13">
+      <c r="S13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="T13">
         <v>0.01</v>
       </c>
-      <c r="S13" t="str">
+      <c r="U13" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;lambda;"</v>
       </c>
-      <c r="T13" t="str">
+      <c r="V13" t="str">
         <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="U13" t="str">
-        <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none")</v>
-      </c>
-      <c r="V13" t="str">
-        <f>B13&amp;"Slider"</f>
-        <v>expSlider</v>
-      </c>
       <c r="W13" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;Q13&amp;", maxVal = "&amp;R13&amp;", startVals = "&amp;S13&amp;", stepVal = "&amp;T13&amp;", paramHTML = "&amp;U13&amp;", multi = "&amp;V13&amp;","</f>
+        <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none",</v>
+      </c>
+      <c r="X13" t="str">
         <f>IF(E13=1,"c()", IF(E13=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
-      <c r="X13" t="str">
+      <c r="Y13" t="str">
+        <f t="shared" si="2"/>
+        <v>expParamTransform</v>
+      </c>
+      <c r="Z13" t="str">
         <f t="shared" si="3"/>
-        <v>expParamTransform</v>
-      </c>
-      <c r="Y13" t="str">
+        <v>expPDF</v>
+      </c>
+      <c r="AA13" t="str">
         <f>B13&amp;"PlotDistr"</f>
         <v>expPlotDistr</v>
       </c>
-      <c r="Z13" t="str">
+      <c r="AB13" t="str">
         <f>B13&amp;"Draws"</f>
         <v>expDraws</v>
       </c>
-      <c r="AA13" t="str">
+      <c r="AC13" t="str">
         <f>B13&amp;"Latex"</f>
         <v>expLatex</v>
       </c>
-      <c r="AB13" t="str">
+      <c r="AD13" t="str">
         <f t="shared" si="4"/>
         <v>expChartDomain</v>
       </c>
-      <c r="AC13" t="str">
+      <c r="AE13" t="str">
         <f t="shared" si="5"/>
         <v>expLikelihoodFun</v>
       </c>
-      <c r="AD13" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB13&amp;", likelihoodFun = "&amp;AC13&amp;" , paramName = """&amp;G13&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N13&amp;""")}"</f>
+      <c r="AF13" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD13&amp;", likelihoodFun = "&amp;AE13&amp;" , paramName = """&amp;G13&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N13&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expChartDomain, likelihoodFun = expLikelihoodFun , paramName = "Lambda",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
@@ -2102,99 +2200,105 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="M14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O14" s="1">
+        <v>72</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q14" s="1">
         <v>-2</v>
       </c>
-      <c r="P14" s="1">
+      <c r="R14" s="1">
         <v>2</v>
       </c>
-      <c r="Q14" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="R14">
+      <c r="S14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="T14">
         <v>0.01</v>
       </c>
-      <c r="S14" t="str">
+      <c r="U14" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="T14" t="str">
+      <c r="V14" t="str">
         <f t="shared" si="1"/>
         <v>"none"</v>
       </c>
-      <c r="U14" t="str">
-        <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none")</v>
-      </c>
-      <c r="V14" t="str">
-        <f>B14&amp;"Slider"</f>
-        <v>expExpSlider</v>
-      </c>
       <c r="W14" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;Q14&amp;", maxVal = "&amp;R14&amp;", startVals = "&amp;S14&amp;", stepVal = "&amp;T14&amp;", paramHTML = "&amp;U14&amp;", multi = "&amp;V14&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
+      </c>
+      <c r="X14" t="str">
         <f>IF(E14=1,"c()", IF(E14=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
-      <c r="X14" t="str">
+      <c r="Y14" t="str">
+        <f t="shared" si="2"/>
+        <v>expExpParamTransform</v>
+      </c>
+      <c r="Z14" t="str">
         <f t="shared" si="3"/>
-        <v>expExpParamTransform</v>
-      </c>
-      <c r="Y14" t="str">
+        <v>expExpPDF</v>
+      </c>
+      <c r="AA14" t="str">
         <f>B14&amp;"PlotDistr"</f>
         <v>expExpPlotDistr</v>
       </c>
-      <c r="Z14" t="str">
+      <c r="AB14" t="str">
         <f>B14&amp;"Draws"</f>
         <v>expExpDraws</v>
       </c>
-      <c r="AA14" t="str">
+      <c r="AC14" t="str">
         <f>B14&amp;"Latex"</f>
         <v>expExpLatex</v>
       </c>
-      <c r="AB14" t="str">
+      <c r="AD14" t="str">
         <f t="shared" si="4"/>
         <v>expExpChartDomain</v>
       </c>
-      <c r="AC14" t="str">
+      <c r="AE14" t="str">
         <f t="shared" si="5"/>
         <v>expExpLikelihoodFun</v>
       </c>
-      <c r="AD14" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB14&amp;", likelihoodFun = "&amp;AC14&amp;" , paramName = """&amp;G14&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N14&amp;""")}"</f>
+      <c r="AF14" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD14&amp;", likelihoodFun = "&amp;AE14&amp;" , paramName = """&amp;G14&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N14&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expExpChartDomain, likelihoodFun = expExpLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>8</v>
@@ -2206,87 +2310,93 @@
         <v>3</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="M15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="O15" s="1">
+        <v>72</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q15" s="1">
         <v>-0.5</v>
       </c>
-      <c r="P15" s="1">
+      <c r="R15" s="1">
         <v>0.5</v>
       </c>
-      <c r="Q15" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="R15">
+      <c r="S15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="T15">
         <v>0.01</v>
       </c>
-      <c r="S15" t="str">
+      <c r="U15" t="str">
         <f t="shared" si="0"/>
         <v>"&amp;beta;"</v>
       </c>
-      <c r="T15" t="str">
+      <c r="V15" t="str">
         <f t="shared" si="1"/>
         <v>"betas"</v>
       </c>
-      <c r="U15" t="str">
-        <f t="shared" si="2"/>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas")</v>
-      </c>
-      <c r="V15" t="str">
-        <f>B15&amp;"Slider"</f>
-        <v>expExpXSlider</v>
-      </c>
       <c r="W15" t="str">
+        <f>"manyParamSliderMaker(minVal ="&amp;Q15&amp;", maxVal = "&amp;R15&amp;", startVals = "&amp;S15&amp;", stepVal = "&amp;T15&amp;", paramHTML = "&amp;U15&amp;", multi = "&amp;V15&amp;","</f>
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
+      </c>
+      <c r="X15" t="str">
         <f>IF(E15=1,"c()", IF(E15=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
-      <c r="X15" t="str">
+      <c r="Y15" t="str">
+        <f t="shared" si="2"/>
+        <v>expExpXParamTransform</v>
+      </c>
+      <c r="Z15" t="str">
         <f t="shared" si="3"/>
-        <v>expExpXParamTransform</v>
-      </c>
-      <c r="Y15" t="str">
+        <v>expExpXPDF</v>
+      </c>
+      <c r="AA15" t="str">
         <f>B15&amp;"PlotDistr"</f>
         <v>expExpXPlotDistr</v>
       </c>
-      <c r="Z15" t="str">
+      <c r="AB15" t="str">
         <f>B15&amp;"Draws"</f>
         <v>expExpXDraws</v>
       </c>
-      <c r="AA15" t="str">
+      <c r="AC15" t="str">
         <f>B15&amp;"Latex"</f>
         <v>expExpXLatex</v>
       </c>
-      <c r="AB15" t="str">
+      <c r="AD15" t="str">
         <f t="shared" si="4"/>
         <v>expExpXChartDomain</v>
       </c>
-      <c r="AC15" t="str">
+      <c r="AE15" t="str">
         <f t="shared" si="5"/>
         <v>expExpXLikelihoodFun</v>
       </c>
-      <c r="AD15" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AB15&amp;", likelihoodFun = "&amp;AC15&amp;" , paramName = """&amp;G15&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N15&amp;""")}"</f>
+      <c r="AF15" t="str">
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD15&amp;", likelihoodFun = "&amp;AE15&amp;" , paramName = """&amp;G15&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N15&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expExpXChartDomain, likelihoodFun = expExpXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add MLE by hand for all non-covariates
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D30026-19C5-4760-88B0-411C48242F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6771BF4C-08A9-4552-BF18-7DC4CCB9EB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="117">
   <si>
     <t>Bernoulli-Pi</t>
   </si>
@@ -364,6 +364,27 @@
   </si>
   <si>
     <t>pdfList</t>
+  </si>
+  <si>
+    <t>c(0,.4)</t>
+  </si>
+  <si>
+    <t>c(0,10)</t>
+  </si>
+  <si>
+    <t>c(0,20)</t>
+  </si>
+  <si>
+    <t>c(0,30)</t>
+  </si>
+  <si>
+    <t>c(0,1)</t>
+  </si>
+  <si>
+    <t>c(0,1.5)</t>
+  </si>
+  <si>
+    <t>c(0,5)</t>
   </si>
 </sst>
 </file>
@@ -733,7 +754,7 @@
   <dimension ref="A1:AF15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+      <selection activeCell="O13" sqref="O13:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +768,9 @@
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" customWidth="1"/>
-    <col min="14" max="16" width="16" customWidth="1"/>
+    <col min="14" max="14" width="16" customWidth="1"/>
+    <col min="15" max="15" width="10" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" customWidth="1"/>
     <col min="17" max="17" width="6.140625" customWidth="1"/>
     <col min="18" max="18" width="4.28515625" customWidth="1"/>
     <col min="19" max="19" width="5.5703125" customWidth="1"/>
@@ -930,11 +953,11 @@
         <v>"none"</v>
       </c>
       <c r="W2" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;Q2&amp;", maxVal = "&amp;R2&amp;", startVals = "&amp;S2&amp;", stepVal = "&amp;T2&amp;", paramHTML = "&amp;U2&amp;", multi = "&amp;V2&amp;","</f>
+        <f t="shared" ref="W2:W15" si="0">"manyParamSliderMaker(minVal ="&amp;Q2&amp;", maxVal = "&amp;R2&amp;", startVals = "&amp;S2&amp;", stepVal = "&amp;T2&amp;", paramHTML = "&amp;U2&amp;", multi = "&amp;V2&amp;","</f>
         <v>manyParamSliderMaker(minVal =0, maxVal = 1, startVals = c(.3), stepVal = 0.01, paramHTML = "&amp;pi;", multi = "none",</v>
       </c>
       <c r="X2" t="str">
-        <f>IF(E2=1,"c()", IF(E2=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+        <f t="shared" ref="X2:X15" si="1">IF(E2=1,"c()", IF(E2=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
       <c r="Y2" t="str">
@@ -946,15 +969,15 @@
         <v>bernPDF</v>
       </c>
       <c r="AA2" t="str">
-        <f>B2&amp;"PlotDistr"</f>
+        <f t="shared" ref="AA2:AA15" si="2">B2&amp;"PlotDistr"</f>
         <v>bernPlotDistr</v>
       </c>
       <c r="AB2" t="str">
-        <f>B2&amp;"Draws"</f>
+        <f t="shared" ref="AB2:AB15" si="3">B2&amp;"Draws"</f>
         <v>bernDraws</v>
       </c>
       <c r="AC2" t="str">
-        <f>B2&amp;"Latex"</f>
+        <f t="shared" ref="AC2:AC15" si="4">B2&amp;"Latex"</f>
         <v>bernLatex</v>
       </c>
       <c r="AD2" t="str">
@@ -966,7 +989,7 @@
         <v>bernLikelihoodFun</v>
       </c>
       <c r="AF2" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD2&amp;", likelihoodFun = "&amp;AE2&amp;" , paramName = """&amp;G2&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N2&amp;""")}"</f>
+        <f t="shared" ref="AF2:AF15" si="5">"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD2&amp;", likelihoodFun = "&amp;AE2&amp;" , paramName = """&amp;G2&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N2&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernChartDomain, likelihoodFun = bernLikelihoodFun , paramName = "Pi",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -1032,51 +1055,51 @@
         <v>0.01</v>
       </c>
       <c r="U3" t="str">
-        <f t="shared" ref="U3:U15" si="0">"""&amp;"&amp;RIGHT(K3,LEN(K3)-1)&amp;";"""</f>
+        <f t="shared" ref="U3:U15" si="6">"""&amp;"&amp;RIGHT(K3,LEN(K3)-1)&amp;";"""</f>
         <v>"&amp;beta;"</v>
       </c>
       <c r="V3" t="str">
-        <f t="shared" ref="V3:V15" si="1">IF(F3=1,"""none""",IF(E3=F3,"""betas""","""fullNorm"""))</f>
+        <f t="shared" ref="V3:V15" si="7">IF(F3=1,"""none""",IF(E3=F3,"""betas""","""fullNorm"""))</f>
         <v>"none"</v>
       </c>
       <c r="W3" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;Q3&amp;", maxVal = "&amp;R3&amp;", startVals = "&amp;S3&amp;", stepVal = "&amp;T3&amp;", paramHTML = "&amp;U3&amp;", multi = "&amp;V3&amp;","</f>
+        <f t="shared" si="0"/>
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
       </c>
       <c r="X3" t="str">
-        <f>IF(E3=1,"c()", IF(E3=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+        <f t="shared" si="1"/>
         <v>c()</v>
       </c>
       <c r="Y3" t="str">
-        <f t="shared" ref="Y3:Y15" si="2">$B3&amp;"ParamTransform"</f>
+        <f t="shared" ref="Y3:Y15" si="8">$B3&amp;"ParamTransform"</f>
         <v>bernLogitParamTransform</v>
       </c>
       <c r="Z3" t="str">
-        <f t="shared" ref="Z3:Z15" si="3">$B3&amp;"PDF"</f>
+        <f t="shared" ref="Z3:Z15" si="9">$B3&amp;"PDF"</f>
         <v>bernLogitPDF</v>
       </c>
       <c r="AA3" t="str">
-        <f>B3&amp;"PlotDistr"</f>
+        <f t="shared" si="2"/>
         <v>bernLogitPlotDistr</v>
       </c>
       <c r="AB3" t="str">
-        <f>B3&amp;"Draws"</f>
+        <f t="shared" si="3"/>
         <v>bernLogitDraws</v>
       </c>
       <c r="AC3" t="str">
-        <f>B3&amp;"Latex"</f>
+        <f t="shared" si="4"/>
         <v>bernLogitLatex</v>
       </c>
       <c r="AD3" t="str">
-        <f t="shared" ref="AD3:AD15" si="4">$B3&amp;"ChartDomain"</f>
+        <f t="shared" ref="AD3:AD15" si="10">$B3&amp;"ChartDomain"</f>
         <v>bernLogitChartDomain</v>
       </c>
       <c r="AE3" t="str">
-        <f t="shared" ref="AE3:AE15" si="5">$B3&amp;"LikelihoodFun"</f>
+        <f t="shared" ref="AE3:AE15" si="11">$B3&amp;"LikelihoodFun"</f>
         <v>bernLogitLikelihoodFun</v>
       </c>
       <c r="AF3" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD3&amp;", likelihoodFun = "&amp;AE3&amp;" , paramName = """&amp;G3&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N3&amp;""")}"</f>
+        <f t="shared" si="5"/>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernLogitChartDomain, likelihoodFun = bernLogitLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -1142,51 +1165,51 @@
         <v>0.01</v>
       </c>
       <c r="U4" t="str">
+        <f t="shared" si="6"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="V4" t="str">
+        <f t="shared" si="7"/>
+        <v>"betas"</v>
+      </c>
+      <c r="W4" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="V4" t="str">
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
+      </c>
+      <c r="X4" t="str">
         <f t="shared" si="1"/>
-        <v>"betas"</v>
-      </c>
-      <c r="W4" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;Q4&amp;", maxVal = "&amp;R4&amp;", startVals = "&amp;S4&amp;", stepVal = "&amp;T4&amp;", paramHTML = "&amp;U4&amp;", multi = "&amp;V4&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
-      </c>
-      <c r="X4" t="str">
-        <f>IF(E4=1,"c()", IF(E4=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="Y4" t="str">
+        <f t="shared" si="8"/>
+        <v>bernLogitXParamTransform</v>
+      </c>
+      <c r="Z4" t="str">
+        <f t="shared" si="9"/>
+        <v>bernLogitXPDF</v>
+      </c>
+      <c r="AA4" t="str">
         <f t="shared" si="2"/>
-        <v>bernLogitXParamTransform</v>
-      </c>
-      <c r="Z4" t="str">
+        <v>bernLogitXPlotDistr</v>
+      </c>
+      <c r="AB4" t="str">
         <f t="shared" si="3"/>
-        <v>bernLogitXPDF</v>
-      </c>
-      <c r="AA4" t="str">
-        <f>B4&amp;"PlotDistr"</f>
-        <v>bernLogitXPlotDistr</v>
-      </c>
-      <c r="AB4" t="str">
-        <f>B4&amp;"Draws"</f>
         <v>bernLogitXDraws</v>
       </c>
       <c r="AC4" t="str">
-        <f>B4&amp;"Latex"</f>
+        <f t="shared" si="4"/>
         <v>bernLogitXLatex</v>
       </c>
       <c r="AD4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>bernLogitXChartDomain</v>
       </c>
       <c r="AE4" t="str">
+        <f t="shared" si="11"/>
+        <v>bernLogitXLikelihoodFun</v>
+      </c>
+      <c r="AF4" t="str">
         <f t="shared" si="5"/>
-        <v>bernLogitXLikelihoodFun</v>
-      </c>
-      <c r="AF4" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD4&amp;", likelihoodFun = "&amp;AE4&amp;" , paramName = """&amp;G4&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N4&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernLogitXChartDomain, likelihoodFun = bernLogitXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -1252,51 +1275,51 @@
         <v>0.01</v>
       </c>
       <c r="U5" t="str">
+        <f t="shared" si="6"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="V5" t="str">
+        <f t="shared" si="7"/>
+        <v>"none"</v>
+      </c>
+      <c r="W5" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="V5" t="str">
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
+      </c>
+      <c r="X5" t="str">
         <f t="shared" si="1"/>
-        <v>"none"</v>
-      </c>
-      <c r="W5" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;Q5&amp;", maxVal = "&amp;R5&amp;", startVals = "&amp;S5&amp;", stepVal = "&amp;T5&amp;", paramHTML = "&amp;U5&amp;", multi = "&amp;V5&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
-      </c>
-      <c r="X5" t="str">
-        <f>IF(E5=1,"c()", IF(E5=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
       <c r="Y5" t="str">
+        <f t="shared" si="8"/>
+        <v>styNormParamTransform</v>
+      </c>
+      <c r="Z5" t="str">
+        <f t="shared" si="9"/>
+        <v>styNormPDF</v>
+      </c>
+      <c r="AA5" t="str">
         <f t="shared" si="2"/>
-        <v>styNormParamTransform</v>
-      </c>
-      <c r="Z5" t="str">
+        <v>styNormPlotDistr</v>
+      </c>
+      <c r="AB5" t="str">
         <f t="shared" si="3"/>
-        <v>styNormPDF</v>
-      </c>
-      <c r="AA5" t="str">
-        <f>B5&amp;"PlotDistr"</f>
-        <v>styNormPlotDistr</v>
-      </c>
-      <c r="AB5" t="str">
-        <f>B5&amp;"Draws"</f>
         <v>styNormDraws</v>
       </c>
       <c r="AC5" t="str">
-        <f>B5&amp;"Latex"</f>
+        <f t="shared" si="4"/>
         <v>styNormLatex</v>
       </c>
       <c r="AD5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>styNormChartDomain</v>
       </c>
       <c r="AE5" t="str">
+        <f t="shared" si="11"/>
+        <v>styNormLikelihoodFun</v>
+      </c>
+      <c r="AF5" t="str">
         <f t="shared" si="5"/>
-        <v>styNormLikelihoodFun</v>
-      </c>
-      <c r="AF5" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD5&amp;", likelihoodFun = "&amp;AE5&amp;" , paramName = """&amp;G5&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N5&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = styNormChartDomain, likelihoodFun = styNormLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -1362,51 +1385,51 @@
         <v>0.01</v>
       </c>
       <c r="U6" t="str">
+        <f t="shared" si="6"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="V6" t="str">
+        <f t="shared" si="7"/>
+        <v>"betas"</v>
+      </c>
+      <c r="W6" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="V6" t="str">
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
+      </c>
+      <c r="X6" t="str">
         <f t="shared" si="1"/>
-        <v>"betas"</v>
-      </c>
-      <c r="W6" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;Q6&amp;", maxVal = "&amp;R6&amp;", startVals = "&amp;S6&amp;", stepVal = "&amp;T6&amp;", paramHTML = "&amp;U6&amp;", multi = "&amp;V6&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
-      </c>
-      <c r="X6" t="str">
-        <f>IF(E6=1,"c()", IF(E6=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="Y6" t="str">
+        <f t="shared" si="8"/>
+        <v>styNormXParamTransform</v>
+      </c>
+      <c r="Z6" t="str">
+        <f t="shared" si="9"/>
+        <v>styNormXPDF</v>
+      </c>
+      <c r="AA6" t="str">
         <f t="shared" si="2"/>
-        <v>styNormXParamTransform</v>
-      </c>
-      <c r="Z6" t="str">
+        <v>styNormXPlotDistr</v>
+      </c>
+      <c r="AB6" t="str">
         <f t="shared" si="3"/>
-        <v>styNormXPDF</v>
-      </c>
-      <c r="AA6" t="str">
-        <f>B6&amp;"PlotDistr"</f>
-        <v>styNormXPlotDistr</v>
-      </c>
-      <c r="AB6" t="str">
-        <f>B6&amp;"Draws"</f>
         <v>styNormXDraws</v>
       </c>
       <c r="AC6" t="str">
-        <f>B6&amp;"Latex"</f>
+        <f t="shared" si="4"/>
         <v>styNormXLatex</v>
       </c>
       <c r="AD6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>styNormXChartDomain</v>
       </c>
       <c r="AE6" t="str">
+        <f t="shared" si="11"/>
+        <v>styNormXLikelihoodFun</v>
+      </c>
+      <c r="AF6" t="str">
         <f t="shared" si="5"/>
-        <v>styNormXLikelihoodFun</v>
-      </c>
-      <c r="AF6" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD6&amp;", likelihoodFun = "&amp;AE6&amp;" , paramName = """&amp;G6&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N6&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = styNormXChartDomain, likelihoodFun = styNormXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -1472,51 +1495,51 @@
         <v>0.01</v>
       </c>
       <c r="U7" t="str">
+        <f t="shared" si="6"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="V7" t="str">
+        <f t="shared" si="7"/>
+        <v>"fullNorm"</v>
+      </c>
+      <c r="W7" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="V7" t="str">
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25,1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm",</v>
+      </c>
+      <c r="X7" t="str">
         <f t="shared" si="1"/>
-        <v>"fullNorm"</v>
-      </c>
-      <c r="W7" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;Q7&amp;", maxVal = "&amp;R7&amp;", startVals = "&amp;S7&amp;", stepVal = "&amp;T7&amp;", paramHTML = "&amp;U7&amp;", multi = "&amp;V7&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1,-1,.25,1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm",</v>
-      </c>
-      <c r="X7" t="str">
-        <f>IF(E7=1,"c()", IF(E7=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2","Sigma")</v>
       </c>
       <c r="Y7" t="str">
+        <f t="shared" si="8"/>
+        <v>fullNormXParamTransform</v>
+      </c>
+      <c r="Z7" t="str">
+        <f t="shared" si="9"/>
+        <v>fullNormXPDF</v>
+      </c>
+      <c r="AA7" t="str">
         <f t="shared" si="2"/>
-        <v>fullNormXParamTransform</v>
-      </c>
-      <c r="Z7" t="str">
+        <v>fullNormXPlotDistr</v>
+      </c>
+      <c r="AB7" t="str">
         <f t="shared" si="3"/>
-        <v>fullNormXPDF</v>
-      </c>
-      <c r="AA7" t="str">
-        <f>B7&amp;"PlotDistr"</f>
-        <v>fullNormXPlotDistr</v>
-      </c>
-      <c r="AB7" t="str">
-        <f>B7&amp;"Draws"</f>
         <v>fullNormXDraws</v>
       </c>
       <c r="AC7" t="str">
-        <f>B7&amp;"Latex"</f>
+        <f t="shared" si="4"/>
         <v>fullNormXLatex</v>
       </c>
       <c r="AD7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>fullNormXChartDomain</v>
       </c>
       <c r="AE7" t="str">
+        <f t="shared" si="11"/>
+        <v>fullNormXLikelihoodFun</v>
+      </c>
+      <c r="AF7" t="str">
         <f t="shared" si="5"/>
-        <v>fullNormXLikelihoodFun</v>
-      </c>
-      <c r="AF7" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD7&amp;", likelihoodFun = "&amp;AE7&amp;" , paramName = """&amp;G7&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N7&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = fullNormXChartDomain, likelihoodFun = fullNormXLikelihoodFun , paramName = "Beta/Sigma",  xVals = xVals, margNum = margNum, optimMethod = "SANN")}</v>
       </c>
     </row>
@@ -1564,10 +1587,10 @@
         <v>72</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="Q8" s="1">
         <v>-0.5</v>
@@ -1582,51 +1605,51 @@
         <v>0.01</v>
       </c>
       <c r="U8" t="str">
+        <f t="shared" si="6"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="V8" t="str">
+        <f t="shared" si="7"/>
+        <v>"none"</v>
+      </c>
+      <c r="W8" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="V8" t="str">
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 2, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
+      </c>
+      <c r="X8" t="str">
         <f t="shared" si="1"/>
-        <v>"none"</v>
-      </c>
-      <c r="W8" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;Q8&amp;", maxVal = "&amp;R8&amp;", startVals = "&amp;S8&amp;", stepVal = "&amp;T8&amp;", paramHTML = "&amp;U8&amp;", multi = "&amp;V8&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 2, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
-      </c>
-      <c r="X8" t="str">
-        <f>IF(E8=1,"c()", IF(E8=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
       <c r="Y8" t="str">
+        <f t="shared" si="8"/>
+        <v>logNormParamTransform</v>
+      </c>
+      <c r="Z8" t="str">
+        <f t="shared" si="9"/>
+        <v>logNormPDF</v>
+      </c>
+      <c r="AA8" t="str">
         <f t="shared" si="2"/>
-        <v>logNormParamTransform</v>
-      </c>
-      <c r="Z8" t="str">
+        <v>logNormPlotDistr</v>
+      </c>
+      <c r="AB8" t="str">
         <f t="shared" si="3"/>
-        <v>logNormPDF</v>
-      </c>
-      <c r="AA8" t="str">
-        <f>B8&amp;"PlotDistr"</f>
-        <v>logNormPlotDistr</v>
-      </c>
-      <c r="AB8" t="str">
-        <f>B8&amp;"Draws"</f>
         <v>logNormDraws</v>
       </c>
       <c r="AC8" t="str">
-        <f>B8&amp;"Latex"</f>
+        <f t="shared" si="4"/>
         <v>logNormLatex</v>
       </c>
       <c r="AD8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>logNormChartDomain</v>
       </c>
       <c r="AE8" t="str">
+        <f t="shared" si="11"/>
+        <v>logNormLikelihoodFun</v>
+      </c>
+      <c r="AF8" t="str">
         <f t="shared" si="5"/>
-        <v>logNormLikelihoodFun</v>
-      </c>
-      <c r="AF8" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD8&amp;", likelihoodFun = "&amp;AE8&amp;" , paramName = """&amp;G8&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N8&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = logNormChartDomain, likelihoodFun = logNormLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -1674,10 +1697,10 @@
         <v>72</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Q9" s="1">
         <v>-1</v>
@@ -1692,51 +1715,51 @@
         <v>0.01</v>
       </c>
       <c r="U9" t="str">
+        <f t="shared" si="6"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="V9" t="str">
+        <f t="shared" si="7"/>
+        <v>"betas"</v>
+      </c>
+      <c r="W9" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="V9" t="str">
+        <v>manyParamSliderMaker(minVal =-1, maxVal = 2, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
+      </c>
+      <c r="X9" t="str">
         <f t="shared" si="1"/>
-        <v>"betas"</v>
-      </c>
-      <c r="W9" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;Q9&amp;", maxVal = "&amp;R9&amp;", startVals = "&amp;S9&amp;", stepVal = "&amp;T9&amp;", paramHTML = "&amp;U9&amp;", multi = "&amp;V9&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-1, maxVal = 2, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
-      </c>
-      <c r="X9" t="str">
-        <f>IF(E9=1,"c()", IF(E9=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="Y9" t="str">
+        <f t="shared" si="8"/>
+        <v>logNormXParamTransform</v>
+      </c>
+      <c r="Z9" t="str">
+        <f t="shared" si="9"/>
+        <v>logNormXPDF</v>
+      </c>
+      <c r="AA9" t="str">
         <f t="shared" si="2"/>
-        <v>logNormXParamTransform</v>
-      </c>
-      <c r="Z9" t="str">
+        <v>logNormXPlotDistr</v>
+      </c>
+      <c r="AB9" t="str">
         <f t="shared" si="3"/>
-        <v>logNormXPDF</v>
-      </c>
-      <c r="AA9" t="str">
-        <f>B9&amp;"PlotDistr"</f>
-        <v>logNormXPlotDistr</v>
-      </c>
-      <c r="AB9" t="str">
-        <f>B9&amp;"Draws"</f>
         <v>logNormXDraws</v>
       </c>
       <c r="AC9" t="str">
-        <f>B9&amp;"Latex"</f>
+        <f t="shared" si="4"/>
         <v>logNormXLatex</v>
       </c>
       <c r="AD9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>logNormXChartDomain</v>
       </c>
       <c r="AE9" t="str">
+        <f t="shared" si="11"/>
+        <v>logNormXLikelihoodFun</v>
+      </c>
+      <c r="AF9" t="str">
         <f t="shared" si="5"/>
-        <v>logNormXLikelihoodFun</v>
-      </c>
-      <c r="AF9" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD9&amp;", likelihoodFun = "&amp;AE9&amp;" , paramName = """&amp;G9&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N9&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = logNormXChartDomain, likelihoodFun = logNormXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -1784,10 +1807,10 @@
         <v>72</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="Q10" s="1">
         <v>1</v>
@@ -1802,51 +1825,51 @@
         <v>0.01</v>
       </c>
       <c r="U10" t="str">
+        <f t="shared" si="6"/>
+        <v>"&amp;lambda;"</v>
+      </c>
+      <c r="V10" t="str">
+        <f t="shared" si="7"/>
+        <v>"none"</v>
+      </c>
+      <c r="W10" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;lambda;"</v>
-      </c>
-      <c r="V10" t="str">
+        <v>manyParamSliderMaker(minVal =1, maxVal = 10, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none",</v>
+      </c>
+      <c r="X10" t="str">
         <f t="shared" si="1"/>
-        <v>"none"</v>
-      </c>
-      <c r="W10" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;Q10&amp;", maxVal = "&amp;R10&amp;", startVals = "&amp;S10&amp;", stepVal = "&amp;T10&amp;", paramHTML = "&amp;U10&amp;", multi = "&amp;V10&amp;","</f>
-        <v>manyParamSliderMaker(minVal =1, maxVal = 10, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none",</v>
-      </c>
-      <c r="X10" t="str">
-        <f>IF(E10=1,"c()", IF(E10=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
       <c r="Y10" t="str">
+        <f t="shared" si="8"/>
+        <v>poisParamTransform</v>
+      </c>
+      <c r="Z10" t="str">
+        <f t="shared" si="9"/>
+        <v>poisPDF</v>
+      </c>
+      <c r="AA10" t="str">
         <f t="shared" si="2"/>
-        <v>poisParamTransform</v>
-      </c>
-      <c r="Z10" t="str">
+        <v>poisPlotDistr</v>
+      </c>
+      <c r="AB10" t="str">
         <f t="shared" si="3"/>
-        <v>poisPDF</v>
-      </c>
-      <c r="AA10" t="str">
-        <f>B10&amp;"PlotDistr"</f>
-        <v>poisPlotDistr</v>
-      </c>
-      <c r="AB10" t="str">
-        <f>B10&amp;"Draws"</f>
         <v>poisDraws</v>
       </c>
       <c r="AC10" t="str">
-        <f>B10&amp;"Latex"</f>
+        <f t="shared" si="4"/>
         <v>poisLatex</v>
       </c>
       <c r="AD10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>poisChartDomain</v>
       </c>
       <c r="AE10" t="str">
+        <f t="shared" si="11"/>
+        <v>poisLikelihoodFun</v>
+      </c>
+      <c r="AF10" t="str">
         <f t="shared" si="5"/>
-        <v>poisLikelihoodFun</v>
-      </c>
-      <c r="AF10" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD10&amp;", likelihoodFun = "&amp;AE10&amp;" , paramName = """&amp;G10&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N10&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisChartDomain, likelihoodFun = poisLikelihoodFun , paramName = "Lambda",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -1894,10 +1917,10 @@
         <v>72</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Q11" s="1">
         <v>-0.25</v>
@@ -1912,51 +1935,51 @@
         <v>0.01</v>
       </c>
       <c r="U11" t="str">
+        <f t="shared" si="6"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="V11" t="str">
+        <f t="shared" si="7"/>
+        <v>"none"</v>
+      </c>
+      <c r="W11" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="V11" t="str">
+        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
+      </c>
+      <c r="X11" t="str">
         <f t="shared" si="1"/>
-        <v>"none"</v>
-      </c>
-      <c r="W11" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;Q11&amp;", maxVal = "&amp;R11&amp;", startVals = "&amp;S11&amp;", stepVal = "&amp;T11&amp;", paramHTML = "&amp;U11&amp;", multi = "&amp;V11&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
-      </c>
-      <c r="X11" t="str">
-        <f>IF(E11=1,"c()", IF(E11=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
       <c r="Y11" t="str">
+        <f t="shared" si="8"/>
+        <v>poisExpParamTransform</v>
+      </c>
+      <c r="Z11" t="str">
+        <f t="shared" si="9"/>
+        <v>poisExpPDF</v>
+      </c>
+      <c r="AA11" t="str">
         <f t="shared" si="2"/>
-        <v>poisExpParamTransform</v>
-      </c>
-      <c r="Z11" t="str">
+        <v>poisExpPlotDistr</v>
+      </c>
+      <c r="AB11" t="str">
         <f t="shared" si="3"/>
-        <v>poisExpPDF</v>
-      </c>
-      <c r="AA11" t="str">
-        <f>B11&amp;"PlotDistr"</f>
-        <v>poisExpPlotDistr</v>
-      </c>
-      <c r="AB11" t="str">
-        <f>B11&amp;"Draws"</f>
         <v>poisExpDraws</v>
       </c>
       <c r="AC11" t="str">
-        <f>B11&amp;"Latex"</f>
+        <f t="shared" si="4"/>
         <v>poisExpLatex</v>
       </c>
       <c r="AD11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>poisExpChartDomain</v>
       </c>
       <c r="AE11" t="str">
+        <f t="shared" si="11"/>
+        <v>poisExpLikelihoodFun</v>
+      </c>
+      <c r="AF11" t="str">
         <f t="shared" si="5"/>
-        <v>poisExpLikelihoodFun</v>
-      </c>
-      <c r="AF11" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD11&amp;", likelihoodFun = "&amp;AE11&amp;" , paramName = """&amp;G11&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N11&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisExpChartDomain, likelihoodFun = poisExpLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -2004,10 +2027,10 @@
         <v>72</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Q12" s="1">
         <v>-1</v>
@@ -2022,51 +2045,51 @@
         <v>0.01</v>
       </c>
       <c r="U12" t="str">
+        <f t="shared" si="6"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="V12" t="str">
+        <f t="shared" si="7"/>
+        <v>"betas"</v>
+      </c>
+      <c r="W12" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="V12" t="str">
+        <v>manyParamSliderMaker(minVal =-1, maxVal = 1, startVals = c(-.3,1,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
+      </c>
+      <c r="X12" t="str">
         <f t="shared" si="1"/>
-        <v>"betas"</v>
-      </c>
-      <c r="W12" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;Q12&amp;", maxVal = "&amp;R12&amp;", startVals = "&amp;S12&amp;", stepVal = "&amp;T12&amp;", paramHTML = "&amp;U12&amp;", multi = "&amp;V12&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-1, maxVal = 1, startVals = c(-.3,1,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
-      </c>
-      <c r="X12" t="str">
-        <f>IF(E12=1,"c()", IF(E12=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="Y12" t="str">
+        <f t="shared" si="8"/>
+        <v>poisExpXParamTransform</v>
+      </c>
+      <c r="Z12" t="str">
+        <f t="shared" si="9"/>
+        <v>poisExpXPDF</v>
+      </c>
+      <c r="AA12" t="str">
         <f t="shared" si="2"/>
-        <v>poisExpXParamTransform</v>
-      </c>
-      <c r="Z12" t="str">
+        <v>poisExpXPlotDistr</v>
+      </c>
+      <c r="AB12" t="str">
         <f t="shared" si="3"/>
-        <v>poisExpXPDF</v>
-      </c>
-      <c r="AA12" t="str">
-        <f>B12&amp;"PlotDistr"</f>
-        <v>poisExpXPlotDistr</v>
-      </c>
-      <c r="AB12" t="str">
-        <f>B12&amp;"Draws"</f>
         <v>poisExpXDraws</v>
       </c>
       <c r="AC12" t="str">
-        <f>B12&amp;"Latex"</f>
+        <f t="shared" si="4"/>
         <v>poisExpXLatex</v>
       </c>
       <c r="AD12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>poisExpXChartDomain</v>
       </c>
       <c r="AE12" t="str">
+        <f t="shared" si="11"/>
+        <v>poisExpXLikelihoodFun</v>
+      </c>
+      <c r="AF12" t="str">
         <f t="shared" si="5"/>
-        <v>poisExpXLikelihoodFun</v>
-      </c>
-      <c r="AF12" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD12&amp;", likelihoodFun = "&amp;AE12&amp;" , paramName = """&amp;G12&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N12&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisExpXChartDomain, likelihoodFun = poisExpXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -2114,10 +2137,10 @@
         <v>72</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="Q13" s="1">
         <v>0.25</v>
@@ -2132,51 +2155,51 @@
         <v>0.01</v>
       </c>
       <c r="U13" t="str">
+        <f t="shared" si="6"/>
+        <v>"&amp;lambda;"</v>
+      </c>
+      <c r="V13" t="str">
+        <f t="shared" si="7"/>
+        <v>"none"</v>
+      </c>
+      <c r="W13" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;lambda;"</v>
-      </c>
-      <c r="V13" t="str">
+        <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none",</v>
+      </c>
+      <c r="X13" t="str">
         <f t="shared" si="1"/>
-        <v>"none"</v>
-      </c>
-      <c r="W13" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;Q13&amp;", maxVal = "&amp;R13&amp;", startVals = "&amp;S13&amp;", stepVal = "&amp;T13&amp;", paramHTML = "&amp;U13&amp;", multi = "&amp;V13&amp;","</f>
-        <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none",</v>
-      </c>
-      <c r="X13" t="str">
-        <f>IF(E13=1,"c()", IF(E13=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
       <c r="Y13" t="str">
+        <f t="shared" si="8"/>
+        <v>expParamTransform</v>
+      </c>
+      <c r="Z13" t="str">
+        <f t="shared" si="9"/>
+        <v>expPDF</v>
+      </c>
+      <c r="AA13" t="str">
         <f t="shared" si="2"/>
-        <v>expParamTransform</v>
-      </c>
-      <c r="Z13" t="str">
+        <v>expPlotDistr</v>
+      </c>
+      <c r="AB13" t="str">
         <f t="shared" si="3"/>
-        <v>expPDF</v>
-      </c>
-      <c r="AA13" t="str">
-        <f>B13&amp;"PlotDistr"</f>
-        <v>expPlotDistr</v>
-      </c>
-      <c r="AB13" t="str">
-        <f>B13&amp;"Draws"</f>
         <v>expDraws</v>
       </c>
       <c r="AC13" t="str">
-        <f>B13&amp;"Latex"</f>
+        <f t="shared" si="4"/>
         <v>expLatex</v>
       </c>
       <c r="AD13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>expChartDomain</v>
       </c>
       <c r="AE13" t="str">
+        <f t="shared" si="11"/>
+        <v>expLikelihoodFun</v>
+      </c>
+      <c r="AF13" t="str">
         <f t="shared" si="5"/>
-        <v>expLikelihoodFun</v>
-      </c>
-      <c r="AF13" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD13&amp;", likelihoodFun = "&amp;AE13&amp;" , paramName = """&amp;G13&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N13&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expChartDomain, likelihoodFun = expLikelihoodFun , paramName = "Lambda",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -2224,10 +2247,10 @@
         <v>72</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="Q14" s="1">
         <v>-2</v>
@@ -2242,51 +2265,51 @@
         <v>0.01</v>
       </c>
       <c r="U14" t="str">
+        <f t="shared" si="6"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="V14" t="str">
+        <f t="shared" si="7"/>
+        <v>"none"</v>
+      </c>
+      <c r="W14" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="V14" t="str">
+        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
+      </c>
+      <c r="X14" t="str">
         <f t="shared" si="1"/>
-        <v>"none"</v>
-      </c>
-      <c r="W14" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;Q14&amp;", maxVal = "&amp;R14&amp;", startVals = "&amp;S14&amp;", stepVal = "&amp;T14&amp;", paramHTML = "&amp;U14&amp;", multi = "&amp;V14&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
-      </c>
-      <c r="X14" t="str">
-        <f>IF(E14=1,"c()", IF(E14=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
       <c r="Y14" t="str">
+        <f t="shared" si="8"/>
+        <v>expExpParamTransform</v>
+      </c>
+      <c r="Z14" t="str">
+        <f t="shared" si="9"/>
+        <v>expExpPDF</v>
+      </c>
+      <c r="AA14" t="str">
         <f t="shared" si="2"/>
-        <v>expExpParamTransform</v>
-      </c>
-      <c r="Z14" t="str">
+        <v>expExpPlotDistr</v>
+      </c>
+      <c r="AB14" t="str">
         <f t="shared" si="3"/>
-        <v>expExpPDF</v>
-      </c>
-      <c r="AA14" t="str">
-        <f>B14&amp;"PlotDistr"</f>
-        <v>expExpPlotDistr</v>
-      </c>
-      <c r="AB14" t="str">
-        <f>B14&amp;"Draws"</f>
         <v>expExpDraws</v>
       </c>
       <c r="AC14" t="str">
-        <f>B14&amp;"Latex"</f>
+        <f t="shared" si="4"/>
         <v>expExpLatex</v>
       </c>
       <c r="AD14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>expExpChartDomain</v>
       </c>
       <c r="AE14" t="str">
+        <f t="shared" si="11"/>
+        <v>expExpLikelihoodFun</v>
+      </c>
+      <c r="AF14" t="str">
         <f t="shared" si="5"/>
-        <v>expExpLikelihoodFun</v>
-      </c>
-      <c r="AF14" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD14&amp;", likelihoodFun = "&amp;AE14&amp;" , paramName = """&amp;G14&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N14&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expExpChartDomain, likelihoodFun = expExpLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -2334,10 +2357,10 @@
         <v>72</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="Q15" s="1">
         <v>-0.5</v>
@@ -2352,51 +2375,51 @@
         <v>0.01</v>
       </c>
       <c r="U15" t="str">
+        <f t="shared" si="6"/>
+        <v>"&amp;beta;"</v>
+      </c>
+      <c r="V15" t="str">
+        <f t="shared" si="7"/>
+        <v>"betas"</v>
+      </c>
+      <c r="W15" t="str">
         <f t="shared" si="0"/>
-        <v>"&amp;beta;"</v>
-      </c>
-      <c r="V15" t="str">
+        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
+      </c>
+      <c r="X15" t="str">
         <f t="shared" si="1"/>
-        <v>"betas"</v>
-      </c>
-      <c r="W15" t="str">
-        <f>"manyParamSliderMaker(minVal ="&amp;Q15&amp;", maxVal = "&amp;R15&amp;", startVals = "&amp;S15&amp;", stepVal = "&amp;T15&amp;", paramHTML = "&amp;U15&amp;", multi = "&amp;V15&amp;","</f>
-        <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
-      </c>
-      <c r="X15" t="str">
-        <f>IF(E15=1,"c()", IF(E15=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="Y15" t="str">
+        <f t="shared" si="8"/>
+        <v>expExpXParamTransform</v>
+      </c>
+      <c r="Z15" t="str">
+        <f t="shared" si="9"/>
+        <v>expExpXPDF</v>
+      </c>
+      <c r="AA15" t="str">
         <f t="shared" si="2"/>
-        <v>expExpXParamTransform</v>
-      </c>
-      <c r="Z15" t="str">
+        <v>expExpXPlotDistr</v>
+      </c>
+      <c r="AB15" t="str">
         <f t="shared" si="3"/>
-        <v>expExpXPDF</v>
-      </c>
-      <c r="AA15" t="str">
-        <f>B15&amp;"PlotDistr"</f>
-        <v>expExpXPlotDistr</v>
-      </c>
-      <c r="AB15" t="str">
-        <f>B15&amp;"Draws"</f>
         <v>expExpXDraws</v>
       </c>
       <c r="AC15" t="str">
-        <f>B15&amp;"Latex"</f>
+        <f t="shared" si="4"/>
         <v>expExpXLatex</v>
       </c>
       <c r="AD15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>expExpXChartDomain</v>
       </c>
       <c r="AE15" t="str">
+        <f t="shared" si="11"/>
+        <v>expExpXLikelihoodFun</v>
+      </c>
+      <c r="AF15" t="str">
         <f t="shared" si="5"/>
-        <v>expExpXLikelihoodFun</v>
-      </c>
-      <c r="AF15" t="str">
-        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD15&amp;", likelihoodFun = "&amp;AE15&amp;" , paramName = """&amp;G15&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N15&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expExpXChartDomain, likelihoodFun = expExpXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>

</xml_diff>

<commit_message>
composite distributions 1st page
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F6C1F4-357A-49F2-A2A9-28E2F93CE9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875B1657-EC97-4DDA-A483-FD88208DC9C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="119">
   <si>
     <t>Bernoulli-Pi</t>
   </si>
@@ -336,12 +336,6 @@
     <t>c(2)</t>
   </si>
   <si>
-    <t>c(-.3,1,.3)</t>
-  </si>
-  <si>
-    <t>c(1,-1,.25,1)</t>
-  </si>
-  <si>
     <t>analyticDomain</t>
   </si>
   <si>
@@ -388,6 +382,15 @@
   </si>
   <si>
     <t>c(.1)</t>
+  </si>
+  <si>
+    <t>c(-1,3,.25,1)</t>
+  </si>
+  <si>
+    <t>c(-1,3,.25)</t>
+  </si>
+  <si>
+    <t>c(-.05,2,.3)</t>
   </si>
 </sst>
 </file>
@@ -756,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93666C39-8581-483B-B5D6-1BA873560E18}">
   <dimension ref="A1:AF15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +779,7 @@
     <col min="16" max="16" width="9.42578125" customWidth="1"/>
     <col min="17" max="17" width="6.140625" customWidth="1"/>
     <col min="18" max="18" width="4.28515625" customWidth="1"/>
-    <col min="19" max="19" width="5.5703125" customWidth="1"/>
+    <col min="19" max="19" width="7.140625" customWidth="1"/>
     <col min="20" max="20" width="6" customWidth="1"/>
     <col min="21" max="22" width="4.28515625" customWidth="1"/>
     <col min="23" max="23" width="16" customWidth="1"/>
@@ -832,10 +835,10 @@
         <v>71</v>
       </c>
       <c r="O1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="P1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Q1" t="s">
         <v>86</v>
@@ -865,7 +868,7 @@
         <v>47</v>
       </c>
       <c r="Z1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AA1" t="s">
         <v>27</v>
@@ -930,10 +933,10 @@
         <v>72</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q2" s="1">
         <v>0</v>
@@ -1040,10 +1043,10 @@
         <v>72</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q3" s="1">
         <v>-2</v>
@@ -1150,10 +1153,10 @@
         <v>72</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q4" s="1">
         <v>-3</v>
@@ -1260,10 +1263,10 @@
         <v>72</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Q5" s="1">
         <v>-3</v>
@@ -1370,10 +1373,10 @@
         <v>72</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Q6" s="1">
         <v>-3</v>
@@ -1382,7 +1385,7 @@
         <v>3</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="T6">
         <v>0.01</v>
@@ -1397,7 +1400,7 @@
       </c>
       <c r="W6" t="str">
         <f t="shared" si="0"/>
-        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,3,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
       </c>
       <c r="X6" t="str">
         <f t="shared" si="1"/>
@@ -1480,10 +1483,10 @@
         <v>73</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Q7" s="1">
         <v>-3</v>
@@ -1492,7 +1495,7 @@
         <v>3</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="T7">
         <v>0.01</v>
@@ -1507,7 +1510,7 @@
       </c>
       <c r="W7" t="str">
         <f t="shared" si="0"/>
-        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-1,.25,1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm",</v>
+        <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,3,.25,1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm",</v>
       </c>
       <c r="X7" t="str">
         <f t="shared" si="1"/>
@@ -1590,10 +1593,10 @@
         <v>72</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="Q8" s="1">
         <v>-0.5</v>
@@ -1602,7 +1605,7 @@
         <v>0.5</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="T8">
         <v>0.01</v>
@@ -1700,10 +1703,10 @@
         <v>72</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Q9" s="1">
         <v>-1</v>
@@ -1810,10 +1813,10 @@
         <v>72</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="Q10" s="1">
         <v>1</v>
@@ -1920,10 +1923,10 @@
         <v>72</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Q11" s="1">
         <v>-0.25</v>
@@ -2030,19 +2033,19 @@
         <v>72</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Q12" s="1">
-        <v>-1</v>
+        <v>-0.25</v>
       </c>
       <c r="R12" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="T12">
         <v>0.01</v>
@@ -2057,7 +2060,7 @@
       </c>
       <c r="W12" t="str">
         <f t="shared" si="0"/>
-        <v>manyParamSliderMaker(minVal =-1, maxVal = 1, startVals = c(-.3,1,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
+        <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(-.05,2,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
       </c>
       <c r="X12" t="str">
         <f t="shared" si="1"/>
@@ -2140,10 +2143,10 @@
         <v>72</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Q13" s="1">
         <v>0.25</v>
@@ -2250,10 +2253,10 @@
         <v>72</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Q14" s="1">
         <v>-2</v>
@@ -2360,10 +2363,10 @@
         <v>72</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Q15" s="1">
         <v>-0.5</v>

</xml_diff>

<commit_message>
major refactor: simplify MLE chart domain, make it responsive to parameter guesses
</commit_message>
<xml_diff>
--- a/DistrNames.xlsx
+++ b/DistrNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Classes\Gov2001\App\probSimulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B360F132-B70E-4E82-8AD3-793A0EDE0D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A61E5D4-530E-4769-B925-14E68164334E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EE83A7B5-564E-4C96-948F-97A222FEAA63}"/>
   </bookViews>
@@ -760,7 +760,7 @@
   <dimension ref="A1:AF15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,9 +771,9 @@
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
     <col min="16" max="16" width="9.42578125" customWidth="1"/>
@@ -811,16 +811,16 @@
         <v>68</v>
       </c>
       <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" t="s">
         <v>36</v>
-      </c>
-      <c r="H1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" t="s">
-        <v>56</v>
       </c>
       <c r="K1" t="s">
         <v>48</v>
@@ -909,16 +909,16 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>49</v>
@@ -963,7 +963,7 @@
         <v>manyParamSliderMaker(minVal =0, maxVal = 1, startVals = c(.3), stepVal = 0.01, paramHTML = "&amp;pi;", multi = "none",</v>
       </c>
       <c r="X2" t="str">
-        <f t="shared" ref="X2:X15" si="1">IF(E2=1,"c()", IF(E2=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
+        <f>IF(E2=1,"c()", IF(E2=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
       <c r="Y2" t="str">
@@ -975,15 +975,15 @@
         <v>bernPDF</v>
       </c>
       <c r="AA2" t="str">
-        <f t="shared" ref="AA2:AA15" si="2">B2&amp;"PlotDistr"</f>
+        <f>B2&amp;"PlotDistr"</f>
         <v>bernPlotDistr</v>
       </c>
       <c r="AB2" t="str">
-        <f t="shared" ref="AB2:AB15" si="3">B2&amp;"Draws"</f>
+        <f>B2&amp;"Draws"</f>
         <v>bernDraws</v>
       </c>
       <c r="AC2" t="str">
-        <f t="shared" ref="AC2:AC15" si="4">B2&amp;"Latex"</f>
+        <f>B2&amp;"Latex"</f>
         <v>bernLatex</v>
       </c>
       <c r="AD2" t="str">
@@ -995,7 +995,7 @@
         <v>bernLikelihoodFun</v>
       </c>
       <c r="AF2" t="str">
-        <f t="shared" ref="AF2:AF15" si="5">"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD2&amp;", likelihoodFun = "&amp;AE2&amp;" , paramName = """&amp;G2&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N2&amp;""")}"</f>
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD2&amp;", likelihoodFun = "&amp;AE2&amp;" , paramName = """&amp;J2&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N2&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernChartDomain, likelihoodFun = bernLikelihoodFun , paramName = "Pi",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -1019,16 +1019,16 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>50</v>
@@ -1061,11 +1061,11 @@
         <v>0.01</v>
       </c>
       <c r="U3" t="str">
-        <f t="shared" ref="U3:U15" si="6">"""&amp;"&amp;RIGHT(K3,LEN(K3)-1)&amp;";"""</f>
+        <f t="shared" ref="U3:U15" si="1">"""&amp;"&amp;RIGHT(K3,LEN(K3)-1)&amp;";"""</f>
         <v>"&amp;beta;"</v>
       </c>
       <c r="V3" t="str">
-        <f t="shared" ref="V3:V15" si="7">IF(F3=1,"""none""",IF(E3=F3,"""betas""","""fullNorm"""))</f>
+        <f t="shared" ref="V3:V15" si="2">IF(F3=1,"""none""",IF(E3=F3,"""betas""","""fullNorm"""))</f>
         <v>"none"</v>
       </c>
       <c r="W3" t="str">
@@ -1073,39 +1073,39 @@
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(1.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
       </c>
       <c r="X3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(E3=1,"c()", IF(E3=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
       <c r="Y3" t="str">
-        <f t="shared" ref="Y3:Y15" si="8">$B3&amp;"ParamTransform"</f>
+        <f t="shared" ref="Y3:Y15" si="3">$B3&amp;"ParamTransform"</f>
         <v>bernLogitParamTransform</v>
       </c>
       <c r="Z3" t="str">
-        <f t="shared" ref="Z3:Z15" si="9">$B3&amp;"PDF"</f>
+        <f t="shared" ref="Z3:Z15" si="4">$B3&amp;"PDF"</f>
         <v>bernLogitPDF</v>
       </c>
       <c r="AA3" t="str">
-        <f t="shared" si="2"/>
+        <f>B3&amp;"PlotDistr"</f>
         <v>bernLogitPlotDistr</v>
       </c>
       <c r="AB3" t="str">
-        <f t="shared" si="3"/>
+        <f>B3&amp;"Draws"</f>
         <v>bernLogitDraws</v>
       </c>
       <c r="AC3" t="str">
-        <f t="shared" si="4"/>
+        <f>B3&amp;"Latex"</f>
         <v>bernLogitLatex</v>
       </c>
       <c r="AD3" t="str">
-        <f t="shared" ref="AD3:AD15" si="10">$B3&amp;"ChartDomain"</f>
+        <f t="shared" ref="AD3:AD15" si="5">$B3&amp;"ChartDomain"</f>
         <v>bernLogitChartDomain</v>
       </c>
       <c r="AE3" t="str">
-        <f t="shared" ref="AE3:AE15" si="11">$B3&amp;"LikelihoodFun"</f>
+        <f t="shared" ref="AE3:AE15" si="6">$B3&amp;"LikelihoodFun"</f>
         <v>bernLogitLikelihoodFun</v>
       </c>
       <c r="AF3" t="str">
-        <f t="shared" si="5"/>
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD3&amp;", likelihoodFun = "&amp;AE3&amp;" , paramName = """&amp;J3&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N3&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernLogitChartDomain, likelihoodFun = bernLogitLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -1129,16 +1129,16 @@
         <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>50</v>
@@ -1171,11 +1171,11 @@
         <v>0.01</v>
       </c>
       <c r="U4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>"&amp;beta;"</v>
       </c>
       <c r="V4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>"betas"</v>
       </c>
       <c r="W4" t="str">
@@ -1183,39 +1183,39 @@
         <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1,-1,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
       </c>
       <c r="X4" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(E4=1,"c()", IF(E4=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="Y4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>bernLogitXParamTransform</v>
       </c>
       <c r="Z4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>bernLogitXPDF</v>
       </c>
       <c r="AA4" t="str">
-        <f t="shared" si="2"/>
+        <f>B4&amp;"PlotDistr"</f>
         <v>bernLogitXPlotDistr</v>
       </c>
       <c r="AB4" t="str">
-        <f t="shared" si="3"/>
+        <f>B4&amp;"Draws"</f>
         <v>bernLogitXDraws</v>
       </c>
       <c r="AC4" t="str">
-        <f t="shared" si="4"/>
+        <f>B4&amp;"Latex"</f>
         <v>bernLogitXLatex</v>
       </c>
       <c r="AD4" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>bernLogitXChartDomain</v>
       </c>
       <c r="AE4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>bernLogitXLikelihoodFun</v>
       </c>
       <c r="AF4" t="str">
-        <f t="shared" si="5"/>
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD4&amp;", likelihoodFun = "&amp;AE4&amp;" , paramName = """&amp;J4&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N4&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = bernLogitXChartDomain, likelihoodFun = bernLogitXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -1239,16 +1239,16 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>50</v>
@@ -1281,11 +1281,11 @@
         <v>0.01</v>
       </c>
       <c r="U5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>"&amp;beta;"</v>
       </c>
       <c r="V5" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>"none"</v>
       </c>
       <c r="W5" t="str">
@@ -1293,39 +1293,39 @@
         <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
       </c>
       <c r="X5" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(E5=1,"c()", IF(E5=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
       <c r="Y5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>styNormParamTransform</v>
       </c>
       <c r="Z5" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>styNormPDF</v>
       </c>
       <c r="AA5" t="str">
-        <f t="shared" si="2"/>
+        <f>B5&amp;"PlotDistr"</f>
         <v>styNormPlotDistr</v>
       </c>
       <c r="AB5" t="str">
-        <f t="shared" si="3"/>
+        <f>B5&amp;"Draws"</f>
         <v>styNormDraws</v>
       </c>
       <c r="AC5" t="str">
-        <f t="shared" si="4"/>
+        <f>B5&amp;"Latex"</f>
         <v>styNormLatex</v>
       </c>
       <c r="AD5" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>styNormChartDomain</v>
       </c>
       <c r="AE5" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>styNormLikelihoodFun</v>
       </c>
       <c r="AF5" t="str">
-        <f t="shared" si="5"/>
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD5&amp;", likelihoodFun = "&amp;AE5&amp;" , paramName = """&amp;J5&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N5&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = styNormChartDomain, likelihoodFun = styNormLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -1349,16 +1349,16 @@
         <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>50</v>
@@ -1391,11 +1391,11 @@
         <v>0.01</v>
       </c>
       <c r="U6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>"&amp;beta;"</v>
       </c>
       <c r="V6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>"betas"</v>
       </c>
       <c r="W6" t="str">
@@ -1403,39 +1403,39 @@
         <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,3,.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
       </c>
       <c r="X6" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(E6=1,"c()", IF(E6=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="Y6" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>styNormXParamTransform</v>
       </c>
       <c r="Z6" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>styNormXPDF</v>
       </c>
       <c r="AA6" t="str">
-        <f t="shared" si="2"/>
+        <f>B6&amp;"PlotDistr"</f>
         <v>styNormXPlotDistr</v>
       </c>
       <c r="AB6" t="str">
-        <f t="shared" si="3"/>
+        <f>B6&amp;"Draws"</f>
         <v>styNormXDraws</v>
       </c>
       <c r="AC6" t="str">
-        <f t="shared" si="4"/>
+        <f>B6&amp;"Latex"</f>
         <v>styNormXLatex</v>
       </c>
       <c r="AD6" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>styNormXChartDomain</v>
       </c>
       <c r="AE6" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>styNormXLikelihoodFun</v>
       </c>
       <c r="AF6" t="str">
-        <f t="shared" si="5"/>
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD6&amp;", likelihoodFun = "&amp;AE6&amp;" , paramName = """&amp;J6&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N6&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = styNormXChartDomain, likelihoodFun = styNormXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -1459,16 +1459,16 @@
         <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>50</v>
@@ -1501,11 +1501,11 @@
         <v>0.01</v>
       </c>
       <c r="U7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>"&amp;beta;"</v>
       </c>
       <c r="V7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>"fullNorm"</v>
       </c>
       <c r="W7" t="str">
@@ -1513,39 +1513,39 @@
         <v>manyParamSliderMaker(minVal =-3, maxVal = 3, startVals = c(-1,3,.25,1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "fullNorm",</v>
       </c>
       <c r="X7" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(E7=1,"c()", IF(E7=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2","Sigma")</v>
       </c>
       <c r="Y7" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>fullNormXParamTransform</v>
       </c>
       <c r="Z7" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>fullNormXPDF</v>
       </c>
       <c r="AA7" t="str">
-        <f t="shared" si="2"/>
+        <f>B7&amp;"PlotDistr"</f>
         <v>fullNormXPlotDistr</v>
       </c>
       <c r="AB7" t="str">
-        <f t="shared" si="3"/>
+        <f>B7&amp;"Draws"</f>
         <v>fullNormXDraws</v>
       </c>
       <c r="AC7" t="str">
-        <f t="shared" si="4"/>
+        <f>B7&amp;"Latex"</f>
         <v>fullNormXLatex</v>
       </c>
       <c r="AD7" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>fullNormXChartDomain</v>
       </c>
       <c r="AE7" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>fullNormXLikelihoodFun</v>
       </c>
       <c r="AF7" t="str">
-        <f t="shared" si="5"/>
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD7&amp;", likelihoodFun = "&amp;AE7&amp;" , paramName = """&amp;J7&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N7&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = fullNormXChartDomain, likelihoodFun = fullNormXLikelihoodFun , paramName = "Beta/Sigma",  xVals = xVals, margNum = margNum, optimMethod = "SANN")}</v>
       </c>
     </row>
@@ -1569,16 +1569,16 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>50</v>
@@ -1611,11 +1611,11 @@
         <v>0.01</v>
       </c>
       <c r="U8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>"&amp;beta;"</v>
       </c>
       <c r="V8" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>"none"</v>
       </c>
       <c r="W8" t="str">
@@ -1623,39 +1623,39 @@
         <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
       </c>
       <c r="X8" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(E8=1,"c()", IF(E8=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
       <c r="Y8" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>logNormParamTransform</v>
       </c>
       <c r="Z8" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>logNormPDF</v>
       </c>
       <c r="AA8" t="str">
-        <f t="shared" si="2"/>
+        <f>B8&amp;"PlotDistr"</f>
         <v>logNormPlotDistr</v>
       </c>
       <c r="AB8" t="str">
-        <f t="shared" si="3"/>
+        <f>B8&amp;"Draws"</f>
         <v>logNormDraws</v>
       </c>
       <c r="AC8" t="str">
-        <f t="shared" si="4"/>
+        <f>B8&amp;"Latex"</f>
         <v>logNormLatex</v>
       </c>
       <c r="AD8" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>logNormChartDomain</v>
       </c>
       <c r="AE8" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>logNormLikelihoodFun</v>
       </c>
       <c r="AF8" t="str">
-        <f t="shared" si="5"/>
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD8&amp;", likelihoodFun = "&amp;AE8&amp;" , paramName = """&amp;J8&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N8&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = logNormChartDomain, likelihoodFun = logNormLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -1679,16 +1679,16 @@
         <v>3</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>50</v>
@@ -1721,11 +1721,11 @@
         <v>0.01</v>
       </c>
       <c r="U9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>"&amp;beta;"</v>
       </c>
       <c r="V9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>"betas"</v>
       </c>
       <c r="W9" t="str">
@@ -1733,39 +1733,39 @@
         <v>manyParamSliderMaker(minVal =-1, maxVal = 2, startVals = c(1,-1,.5), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
       </c>
       <c r="X9" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(E9=1,"c()", IF(E9=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="Y9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>logNormXParamTransform</v>
       </c>
       <c r="Z9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>logNormXPDF</v>
       </c>
       <c r="AA9" t="str">
-        <f t="shared" si="2"/>
+        <f>B9&amp;"PlotDistr"</f>
         <v>logNormXPlotDistr</v>
       </c>
       <c r="AB9" t="str">
-        <f t="shared" si="3"/>
+        <f>B9&amp;"Draws"</f>
         <v>logNormXDraws</v>
       </c>
       <c r="AC9" t="str">
-        <f t="shared" si="4"/>
+        <f>B9&amp;"Latex"</f>
         <v>logNormXLatex</v>
       </c>
       <c r="AD9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>logNormXChartDomain</v>
       </c>
       <c r="AE9" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>logNormXLikelihoodFun</v>
       </c>
       <c r="AF9" t="str">
-        <f t="shared" si="5"/>
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD9&amp;", likelihoodFun = "&amp;AE9&amp;" , paramName = """&amp;J9&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N9&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = logNormXChartDomain, likelihoodFun = logNormXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -1789,16 +1789,16 @@
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>51</v>
@@ -1831,11 +1831,11 @@
         <v>0.01</v>
       </c>
       <c r="U10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>"&amp;lambda;"</v>
       </c>
       <c r="V10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>"none"</v>
       </c>
       <c r="W10" t="str">
@@ -1843,39 +1843,39 @@
         <v>manyParamSliderMaker(minVal =1, maxVal = 10, startVals = c(2), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none",</v>
       </c>
       <c r="X10" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(E10=1,"c()", IF(E10=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
       <c r="Y10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>poisParamTransform</v>
       </c>
       <c r="Z10" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>poisPDF</v>
       </c>
       <c r="AA10" t="str">
-        <f t="shared" si="2"/>
+        <f>B10&amp;"PlotDistr"</f>
         <v>poisPlotDistr</v>
       </c>
       <c r="AB10" t="str">
-        <f t="shared" si="3"/>
+        <f>B10&amp;"Draws"</f>
         <v>poisDraws</v>
       </c>
       <c r="AC10" t="str">
-        <f t="shared" si="4"/>
+        <f>B10&amp;"Latex"</f>
         <v>poisLatex</v>
       </c>
       <c r="AD10" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>poisChartDomain</v>
       </c>
       <c r="AE10" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>poisLikelihoodFun</v>
       </c>
       <c r="AF10" t="str">
-        <f t="shared" si="5"/>
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD10&amp;", likelihoodFun = "&amp;AE10&amp;" , paramName = """&amp;J10&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N10&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisChartDomain, likelihoodFun = poisLikelihoodFun , paramName = "Lambda",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -1899,16 +1899,16 @@
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>50</v>
@@ -1941,11 +1941,11 @@
         <v>0.01</v>
       </c>
       <c r="U11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>"&amp;beta;"</v>
       </c>
       <c r="V11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>"none"</v>
       </c>
       <c r="W11" t="str">
@@ -1953,39 +1953,39 @@
         <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(1), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
       </c>
       <c r="X11" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(E11=1,"c()", IF(E11=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
       <c r="Y11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>poisExpParamTransform</v>
       </c>
       <c r="Z11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>poisExpPDF</v>
       </c>
       <c r="AA11" t="str">
-        <f t="shared" si="2"/>
+        <f>B11&amp;"PlotDistr"</f>
         <v>poisExpPlotDistr</v>
       </c>
       <c r="AB11" t="str">
-        <f t="shared" si="3"/>
+        <f>B11&amp;"Draws"</f>
         <v>poisExpDraws</v>
       </c>
       <c r="AC11" t="str">
-        <f t="shared" si="4"/>
+        <f>B11&amp;"Latex"</f>
         <v>poisExpLatex</v>
       </c>
       <c r="AD11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>poisExpChartDomain</v>
       </c>
       <c r="AE11" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>poisExpLikelihoodFun</v>
       </c>
       <c r="AF11" t="str">
-        <f t="shared" si="5"/>
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD11&amp;", likelihoodFun = "&amp;AE11&amp;" , paramName = """&amp;J11&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N11&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisExpChartDomain, likelihoodFun = poisExpLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -2009,16 +2009,16 @@
         <v>3</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>50</v>
@@ -2051,11 +2051,11 @@
         <v>0.01</v>
       </c>
       <c r="U12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>"&amp;beta;"</v>
       </c>
       <c r="V12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>"betas"</v>
       </c>
       <c r="W12" t="str">
@@ -2063,39 +2063,39 @@
         <v>manyParamSliderMaker(minVal =-0.25, maxVal = 3, startVals = c(-.05,2,.3), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
       </c>
       <c r="X12" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(E12=1,"c()", IF(E12=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="Y12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>poisExpXParamTransform</v>
       </c>
       <c r="Z12" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>poisExpXPDF</v>
       </c>
       <c r="AA12" t="str">
-        <f t="shared" si="2"/>
+        <f>B12&amp;"PlotDistr"</f>
         <v>poisExpXPlotDistr</v>
       </c>
       <c r="AB12" t="str">
-        <f t="shared" si="3"/>
+        <f>B12&amp;"Draws"</f>
         <v>poisExpXDraws</v>
       </c>
       <c r="AC12" t="str">
-        <f t="shared" si="4"/>
+        <f>B12&amp;"Latex"</f>
         <v>poisExpXLatex</v>
       </c>
       <c r="AD12" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>poisExpXChartDomain</v>
       </c>
       <c r="AE12" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>poisExpXLikelihoodFun</v>
       </c>
       <c r="AF12" t="str">
-        <f t="shared" si="5"/>
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD12&amp;", likelihoodFun = "&amp;AE12&amp;" , paramName = """&amp;J12&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N12&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = poisExpXChartDomain, likelihoodFun = poisExpXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -2119,16 +2119,16 @@
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>51</v>
@@ -2161,11 +2161,11 @@
         <v>0.01</v>
       </c>
       <c r="U13" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>"&amp;lambda;"</v>
       </c>
       <c r="V13" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>"none"</v>
       </c>
       <c r="W13" t="str">
@@ -2173,39 +2173,39 @@
         <v>manyParamSliderMaker(minVal =0.25, maxVal = 1.5, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;lambda;", multi = "none",</v>
       </c>
       <c r="X13" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(E13=1,"c()", IF(E13=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
       <c r="Y13" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>expParamTransform</v>
       </c>
       <c r="Z13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>expPDF</v>
       </c>
       <c r="AA13" t="str">
-        <f t="shared" si="2"/>
+        <f>B13&amp;"PlotDistr"</f>
         <v>expPlotDistr</v>
       </c>
       <c r="AB13" t="str">
-        <f t="shared" si="3"/>
+        <f>B13&amp;"Draws"</f>
         <v>expDraws</v>
       </c>
       <c r="AC13" t="str">
-        <f t="shared" si="4"/>
+        <f>B13&amp;"Latex"</f>
         <v>expLatex</v>
       </c>
       <c r="AD13" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>expChartDomain</v>
       </c>
       <c r="AE13" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>expLikelihoodFun</v>
       </c>
       <c r="AF13" t="str">
-        <f t="shared" si="5"/>
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD13&amp;", likelihoodFun = "&amp;AE13&amp;" , paramName = """&amp;J13&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N13&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expChartDomain, likelihoodFun = expLikelihoodFun , paramName = "Lambda",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -2229,16 +2229,16 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>50</v>
@@ -2271,11 +2271,11 @@
         <v>0.01</v>
       </c>
       <c r="U14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>"&amp;beta;"</v>
       </c>
       <c r="V14" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>"none"</v>
       </c>
       <c r="W14" t="str">
@@ -2283,39 +2283,39 @@
         <v>manyParamSliderMaker(minVal =-2, maxVal = 2, startVals = c(.25), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "none",</v>
       </c>
       <c r="X14" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(E14=1,"c()", IF(E14=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c()</v>
       </c>
       <c r="Y14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>expExpParamTransform</v>
       </c>
       <c r="Z14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>expExpPDF</v>
       </c>
       <c r="AA14" t="str">
-        <f t="shared" si="2"/>
+        <f>B14&amp;"PlotDistr"</f>
         <v>expExpPlotDistr</v>
       </c>
       <c r="AB14" t="str">
-        <f t="shared" si="3"/>
+        <f>B14&amp;"Draws"</f>
         <v>expExpDraws</v>
       </c>
       <c r="AC14" t="str">
-        <f t="shared" si="4"/>
+        <f>B14&amp;"Latex"</f>
         <v>expExpLatex</v>
       </c>
       <c r="AD14" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>expExpChartDomain</v>
       </c>
       <c r="AE14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>expExpLikelihoodFun</v>
       </c>
       <c r="AF14" t="str">
-        <f t="shared" si="5"/>
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD14&amp;", likelihoodFun = "&amp;AE14&amp;" , paramName = """&amp;J14&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N14&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expExpChartDomain, likelihoodFun = expExpLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>
@@ -2339,16 +2339,16 @@
         <v>3</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>50</v>
@@ -2381,11 +2381,11 @@
         <v>0.01</v>
       </c>
       <c r="U15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>"&amp;beta;"</v>
       </c>
       <c r="V15" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>"betas"</v>
       </c>
       <c r="W15" t="str">
@@ -2393,39 +2393,39 @@
         <v>manyParamSliderMaker(minVal =-0.5, maxVal = 0.5, startVals = c(.2, .1, -.2), stepVal = 0.01, paramHTML = "&amp;beta;", multi = "betas",</v>
       </c>
       <c r="X15" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(E15=1,"c()", IF(E15=3,"c(""Beta0"", ""Beta1"", ""Beta2"")","c(""Beta0"", ""Beta1"", ""Beta2"",""Sigma"")"))</f>
         <v>c("Beta0", "Beta1", "Beta2")</v>
       </c>
       <c r="Y15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="3"/>
         <v>expExpXParamTransform</v>
       </c>
       <c r="Z15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="4"/>
         <v>expExpXPDF</v>
       </c>
       <c r="AA15" t="str">
-        <f t="shared" si="2"/>
+        <f>B15&amp;"PlotDistr"</f>
         <v>expExpXPlotDistr</v>
       </c>
       <c r="AB15" t="str">
-        <f t="shared" si="3"/>
+        <f>B15&amp;"Draws"</f>
         <v>expExpXDraws</v>
       </c>
       <c r="AC15" t="str">
-        <f t="shared" si="4"/>
+        <f>B15&amp;"Latex"</f>
         <v>expExpXLatex</v>
       </c>
       <c r="AD15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="5"/>
         <v>expExpXChartDomain</v>
       </c>
       <c r="AE15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="6"/>
         <v>expExpXLikelihoodFun</v>
       </c>
       <c r="AF15" t="str">
-        <f t="shared" si="5"/>
+        <f>"function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = "&amp;AD15&amp;", likelihoodFun = "&amp;AE15&amp;" , paramName = """&amp;J15&amp;""",  xVals = xVals, margNum = margNum, "&amp;"optimMethod = """&amp;N15&amp;""")}"</f>
         <v>function(outcome, xVals, margNum){MLEstimator(outcome = outcome, chartDomain = expExpXChartDomain, likelihoodFun = expExpXLikelihoodFun , paramName = "Beta",  xVals = xVals, margNum = margNum, optimMethod = "Nelder-Mead")}</v>
       </c>
     </row>

</xml_diff>